<commit_message>
WIP_implementación de método para obtención de iFrameMap_Completed:)
</commit_message>
<xml_diff>
--- a/testingAllImports.xlsx
+++ b/testingAllImports.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:W6"/>
+  <dimension ref="A1:X11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -428,48 +428,51 @@
         <v>urlgMaps</v>
       </c>
       <c r="I1" t="str">
+        <v>iframeMap</v>
+      </c>
+      <c r="J1" t="str">
         <v>city</v>
       </c>
-      <c r="J1" t="str">
+      <c r="K1" t="str">
         <v>stars</v>
       </c>
-      <c r="K1" t="str">
+      <c r="L1" t="str">
         <v>CantidadResenas</v>
       </c>
-      <c r="L1" t="str">
+      <c r="M1" t="str">
         <v>opiniones</v>
       </c>
-      <c r="M1" t="str">
+      <c r="N1" t="str">
         <v>photoOriginalURL</v>
       </c>
-      <c r="N1" t="str">
+      <c r="O1" t="str">
         <v>photoDownloadScript</v>
       </c>
-      <c r="O1" t="str">
+      <c r="P1" t="str">
         <v>photoFileName</v>
       </c>
-      <c r="P1" t="str">
+      <c r="Q1" t="str">
         <v>photoNewName</v>
       </c>
-      <c r="Q1" t="str">
+      <c r="R1" t="str">
         <v>photoNewURL</v>
       </c>
-      <c r="R1" t="str">
+      <c r="S1" t="str">
         <v>fileNameConversionScript</v>
       </c>
-      <c r="S1" t="str">
+      <c r="T1" t="str">
         <v>articleIntro</v>
       </c>
-      <c r="T1" t="str">
+      <c r="U1" t="str">
         <v>photoNewFileNameFull</v>
       </c>
-      <c r="U1" t="str">
+      <c r="V1" t="str">
         <v>structuredData</v>
       </c>
-      <c r="V1" t="str">
+      <c r="W1" t="str">
         <v>photoLocal</v>
       </c>
-      <c r="W1" t="str">
+      <c r="X1" t="str">
         <v>missingData</v>
       </c>
     </row>
@@ -493,70 +496,76 @@
         <v>Durango</v>
       </c>
       <c r="H2" t="str">
-        <v>https://www.google.com.mx/maps/place/Vivero+Santa+Fe/data=!4m7!3m6!1s0x869bb7e17f5ebdfd:0x329bbfbf57717ca0!8m2!3d24.0199748!4d-104.6558555!16s%2Fg%2F11btmr25_0!19sChIJ_b1ef-G3m4YRoHxxV7-_mzI?authuser=0&amp;hl=es&amp;rclk=1</v>
+        <v>https://www.google.com.mx/maps/place/Vivero+Santa+Fe/@24.0199748,-104.6558555,17z/data=!3m1!4b1!4m6!3m5!1s0x869bb7e17f5ebdfd:0x329bbfbf57717ca0!8m2!3d24.0199748!4d-104.6558555!16s%2Fg%2F11btmr25_0?authuser=0&amp;hl=es</v>
       </c>
       <c r="I2" t="str">
+        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3644.3144297120525!2d-104.6558555!3d24.0199748!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x869bb7e17f5ebdfd%3A0x329bbfbf57717ca0!2sVivero%20Santa%20Fe!5e0!3m2!1ses!2smx!4v1678840872234!5m2!1ses!2smx" width="600" height="450" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
+      </c>
+      <c r="J2" t="str">
         <v>289V+XM Durango</v>
       </c>
-      <c r="J2" t="str">
+      <c r="K2" t="str">
         <v>4.2</v>
       </c>
-      <c r="K2" t="str">
+      <c r="L2" t="str">
         <v>33</v>
       </c>
-      <c r="L2" t="str">
+      <c r="M2" t="str">
         <v>Super mala atención. Tienen muy bonitas plantas pero la señora que atendie, nunca me hizo caso, le mostre la planta que quería y me ignoro por completo, pésimo. No lo recomiendo y no vuelvo a ir,Excelente atención variedad de plantas  adornos para jardín lo recomiendo Buen Trato y novedades,Excelente atención y plantas de muy buena calidad</v>
       </c>
-      <c r="M2" t="str">
+      <c r="N2" t="str">
         <v>https://lh5.googleusercontent.com/p/AF1QipOC7w7iQu2kg7BiEaF1hoYdzwUX11Mfy6wYJIgK=w408-h306-k-no</v>
       </c>
-      <c r="N2" t="str">
+      <c r="O2" t="str">
         <v>wget --no-check-certificate https://lh5.googleusercontent.com/p/AF1QipOC7w7iQu2kg7BiEaF1hoYdzwUX11Mfy6wYJIgK=w408-h306-k-no</v>
       </c>
-      <c r="O2" t="str">
+      <c r="P2" t="str">
         <v>AF1QipOC7w7iQu2kg7BiEaF1hoYdzwUX11Mfy6wYJIgK=w408-h306-k-no</v>
       </c>
-      <c r="P2" t="str">
+      <c r="Q2" t="str">
         <v>Vivero_Santa_Fe_0</v>
       </c>
-      <c r="Q2" t="str">
+      <c r="R2" t="str">
         <v>https://rumbonaturaleza.com/wp-content/uploads/2023/03/Vivero_Santa_Fe_0.jpg</v>
       </c>
-      <c r="R2" t="str">
+      <c r="S2" t="str">
         <v>ren "AF1QipOC7w7iQu2kg7BiEaF1hoYdzwUX11Mfy6wYJIgK=w408-h306-k-no" "Vivero_Santa_Fe_0.jpg"</v>
       </c>
-      <c r="S2" t="str" xml:space="preserve">
+      <c r="T2" t="str" xml:space="preserve">
         <v xml:space="preserve">
                     &lt;p&gt; ¿Estás buscando los mejores Parques Ecoturísticos en Tabasco? ¡Estás en el lugar correcto! Pues en este artículo vamos a presentarte cuáles son los  Parque Natural que han sido mejor evaluados en este estado. 
- Para esto, realizamos consultas en un montón de fuentes oficiales, redes sociales, rankings e incluso entrevistas para poder determinar cuáles son los  Parque Ecoturístico que mejor calificación han recibido en Tabasco durante los últimos años. 
- Con esta prueba social como respaldo, hoy te daremos los Parque Natural mejor calificados y te compartiremos su ubicación, medios oficiales de contacto, horarios y cómo llegar hasta ellos, junto con la calificación promedio con la que cuenta cada lugar. 
- Así que prepárate y ¡a disfrutar del ecoturismo en Tabasco!&lt;/p&gt;                    
-                    </v>
-      </c>
-      <c r="T2" t="str" xml:space="preserve">
+ Para esto, realizamos consultas en un montón de fuentes oficiales, redes sociales, rankings e incluso entrevistas para poder determinar cuáles son los  Centro Ecoturístico que mejor calificación han recibido en Tabasco durante los últimos años. 
+ Con esta prueba social como respaldo, hoy te daremos los Parque Ecológico mejor calificados y te compartiremos su ubicación, medios oficiales de contacto, horarios y cómo llegar hasta ellos, junto con la calificación promedio con la que cuenta cada lugar. 
+ Así que prepárate y ¡a disfrutar del ecoturismo en Tabasco!&lt;/p&gt;                    
+                    </v>
+      </c>
+      <c r="U2" t="str" xml:space="preserve">
         <v xml:space="preserve">
                     &lt;p&gt; ¿Estás buscando los mejores Parques Ecoturísticos en Tabasco? ¡Estás en el lugar correcto! Pues en este artículo vamos a presentarte cuáles son los  Parque Natural que han sido mejor evaluados en este estado. 
- Para esto, realizamos consultas en un montón de fuentes oficiales, redes sociales, rankings e incluso entrevistas para poder determinar cuáles son los  Parque Ecoturístico que mejor calificación han recibido en Tabasco durante los últimos años. 
- Con esta prueba social como respaldo, hoy te daremos los Parque Natural mejor calificados y te compartiremos su ubicación, medios oficiales de contacto, horarios y cómo llegar hasta ellos, junto con la calificación promedio con la que cuenta cada lugar. 
- Así que prepárate y ¡a disfrutar del ecoturismo en Tabasco!&lt;/p&gt;                    
-                    </v>
-      </c>
-      <c r="U2" t="str" xml:space="preserve">
+ Para esto, realizamos consultas en un montón de fuentes oficiales, redes sociales, rankings e incluso entrevistas para poder determinar cuáles son los  Centro Ecoturístico que mejor calificación han recibido en Tabasco durante los últimos años. 
+ Con esta prueba social como respaldo, hoy te daremos los Parque Ecológico mejor calificados y te compartiremos su ubicación, medios oficiales de contacto, horarios y cómo llegar hasta ellos, junto con la calificación promedio con la que cuenta cada lugar. 
+ Así que prepárate y ¡a disfrutar del ecoturismo en Tabasco!&lt;/p&gt;                    
+                    </v>
+      </c>
+      <c r="V2" t="str" xml:space="preserve">
         <v xml:space="preserve">
                     &lt;h2&gt;&lt;b&gt;Parque Ecoturístico Vivero Santa Fe&lt;/b&gt;&lt;/h2&gt;
-                        &lt;p&gt;El Parque Ecoturístico undefined es una opción fantástica para tener una aventura natural en Tabasco. Su calificación promedio es de 4.2 respaldada por más de 33visitantes, así que no tenemos duda de que este lugar pertenece a la lista de los Parque Ecoturístico mejor rankeados de Tabasco y que se trata de uno de los principales atractivos naturales en la región. Así que ya sabes... ¿ganas de naturaleza?... pues el Parque Ecoturístico undefined es una grandísima opción.&lt;/p&gt;
-                        &lt;h3&gt;&lt;b&gt;¿Cómo llegar al Parque Ecoturístico Vivero Santa Fe? &lt;/b&gt;&lt;/h3&gt;
-                            &lt;p&gt;El Centro Ecoturístico se ubica enBlvd. Cnel. Enrique Carrola Antuna 909, Ciénega, 34090 Durango, Dgo.. Puedes ir a este lugar sin problemas manejando, sólo coloca su dirección oficial en waze, google maps o equivalente, o guíate con este &lt;a href='https://www.google.com.mx/maps/place/Vivero+Santa+Fe/data=!4m7!3m6!1s0x869bb7e17f5ebdfd:0x329bbfbf57717ca0!8m2!3d24.0199748!4d-104.6558555!16s%2Fg%2F11btmr25_0!19sChIJ_b1ef-G3m4YRoHxxV7-_mzI?authuser=0&amp;hl=es&amp;rclk=1'&gt;Mapa del Parque Ecoturístico Vivero Santa Fe&lt;/a&gt;&lt;/p&gt;
+                        &lt;img src="https://rumbonaturaleza.com/wp-content/uploads/2023/03/Vivero_Santa_Fe_0.jpg" alt="Vivero Santa Fe"&gt;   
+                        &lt;div&gt;&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3644.3144297120525!2d-104.6558555!3d24.0199748!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x869bb7e17f5ebdfd%3A0x329bbfbf57717ca0!2sVivero%20Santa%20Fe!5e0!3m2!1ses!2smx!4v1678840872234!5m2!1ses!2smx" width="600" height="450" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;&lt;/div&gt;
+                        &lt;div&gt;&lt;/div&gt;
+                        &lt;p&gt;Bueno pues si eres de quienes ama estar en contacto con la naturaleza y andas por Tabasco, entonces no puedes perderte la experiencia de visitar el Parque Ecoturístico undefined. Con una calificación promedio de 4.2 estrellas de más de Super mala atención. Tienen muy bonitas plantas pero la señora que atendie, nunca me hizo caso, le mostre la planta que quería y me ignoro por completo, pésimo. No lo recomiendo y no vuelvo a ir,Excelente atención variedad de plantas  adornos para jardín lo recomiendo Buen Trato y novedades,Excelente atención y plantas de muy buena calidad visitantes, no tenemos duda de que se trata de un favorito de esta región. Así que nada...prepárate para sumergirte y disfrutar a tope de los paisajes naturales de Tabasco&lt;/p&gt;
+                        &lt;h3&gt;&lt;b&gt;¿Cómo llegar al Centro Ecoturístico Vivero Santa Fe? &lt;/b&gt;&lt;/h3&gt;
+                            &lt;p&gt;El Parque Ecológico se ubica enBlvd. Cnel. Enrique Carrola Antuna 909, Ciénega, 34090 Durango, Dgo.. LLegar al lugar es bastante sencillo. Símplemente coloca la dirección en una app con gps, o apóyate con este &lt;a href='https://www.google.com.mx/maps/place/Vivero+Santa+Fe/@24.0199748,-104.6558555,17z/data=!3m1!4b1!4m6!3m5!1s0x869bb7e17f5ebdfd:0x329bbfbf57717ca0!8m2!3d24.0199748!4d-104.6558555!16s%2Fg%2F11btmr25_0?authuser=0&amp;hl=es'&gt;Mapa del Parque Ecoturístico Vivero Santa Fe&lt;/a&gt;&lt;/p&gt;
                         &lt;h3&gt;&lt;b&gt;¿Cuáles son los contactos del Parque Ecoturístico Vivero Santa Fe?&lt;/b&gt;&lt;/h3&gt;
                             &lt;p&gt;Los contactos disponibles del Parque Ecoturístico Vivero Santa Fe son: &lt;/p&gt;
                             &lt;ul&gt;
                                 &lt;li&gt;&lt;b&gt;Teléfono:&lt;/b&gt;618 235 9375&lt;/li&gt;
                                 &lt;li&gt;&lt;b&gt;SitioWeb:&lt;/b&gt;web no disponible&lt;/li&gt;                                
                             &lt;/ul&gt;
-                        &lt;h3&gt;&lt;b&gt;¿En qué horarios y días se puede visitar el Parque Ecoturístico Vivero Santa Fe?&lt;/b&gt;&lt;/h3&gt;
+                        &lt;h3&gt;&lt;b&gt;¿En qué horarios y días se puede visitar el Centro Ecoturístico Vivero Santa Fe?&lt;/b&gt;&lt;/h3&gt;
                             &lt;p&gt;Los horarios oficiales del Parque Ecoturístico Vivero Santa Fe son los siguientes:&lt;/p&gt;                       
                             &lt;ul&gt;
-                                &lt;li&gt;Lunes de 09:30 a 19:30&lt;/li&gt;
+                                &lt;li&gt;Lunes (Natalicio de Benito Juárez (feriado)) de 09:30 a 19:30 El horario podría cambiar&lt;/li&gt;
                                 &lt;li&gt;Martes de 09:30 a 19:30&lt;/li&gt;
                                 &lt;li&gt;Miércoles de 09:30 a 19:30&lt;/li&gt;
                                 &lt;li&gt;Jueves de 09:30 a 19:30&lt;/li&gt;
@@ -564,15 +573,15 @@
                                 &lt;li&gt;Sábado de 09:30 a 19:30&lt;/li&gt;
                                 &lt;li&gt;Domingo de 09:30 a 19:30&lt;/li&gt;
                             &lt;/ul&gt;
-                            &lt;p&gt;Aunque cuentes ya con los horarios oficiales de apertura de este lugar, siempre te recomendamos que antes de ir eches un ojito a sus redes sociales y vías de contacto, para asegurarte de que no hayan tenido algún cambio logístico de última hora&lt;/p&gt;                 
-                    </v>
-      </c>
-      <c r="V2" t="str" xml:space="preserve">
+                            &lt;p&gt;Aunque estos horarios están oficialmente vigentes, siempre es bueno consultar sus sitios de contacto y redes oficiales antes de visitarlos, por cualquier cambio extraordinario que pudieran tener.&lt;/p&gt;                 
+                    </v>
+      </c>
+      <c r="W2" t="str" xml:space="preserve">
         <v xml:space="preserve">
                     &lt;img src="https://rumbonaturaleza.com/wp-content/uploads/2023/03/Vivero_Santa_Fe_0.jpg" alt="Vivero Santa Fe"&gt;                
                 </v>
       </c>
-      <c r="W2" t="str">
+      <c r="X2" t="str">
         <v>Añadir sitio web</v>
       </c>
     </row>
@@ -596,71 +605,77 @@
         <v>Durango</v>
       </c>
       <c r="H3" t="str">
-        <v>https://www.google.com.mx/maps/place/Vivero+Las+Magnolias/data=!4m7!3m6!1s0x869bb7b871872b85:0x65cc8cefdc6b7345!8m2!3d24.0374832!4d-104.6351623!16s%2Fg%2F11b6j5b_lw!19sChIJhSuHcbi3m4YRRXNr3O-MzGU?authuser=0&amp;hl=es&amp;rclk=1</v>
+        <v>https://www.google.com.mx/maps/place/Vivero+Las+Magnolias/@24.0374832,-104.6351623,17z/data=!3m1!4b1!4m6!3m5!1s0x869bb7b871872b85:0x65cc8cefdc6b7345!8m2!3d24.0374832!4d-104.6351623!16s%2Fg%2F11b6j5b_lw?authuser=0&amp;hl=es</v>
       </c>
       <c r="I3" t="str">
+        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3643.8179757079024!2d-104.63516229999999!3d24.037483200000004!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x869bb7b871872b85%3A0x65cc8cefdc6b7345!2sVivero%20Las%20Magnolias!5e0!3m2!1ses!2smx!4v1678840876876!5m2!1ses!2smx" width="600" height="450" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
+      </c>
+      <c r="J3" t="str">
         <v>29P7+XW Durango</v>
       </c>
-      <c r="J3" t="str">
+      <c r="K3" t="str">
         <v>4.7</v>
       </c>
-      <c r="K3" t="str">
+      <c r="L3" t="str">
         <v>106</v>
       </c>
-      <c r="L3" t="str" xml:space="preserve">
+      <c r="M3" t="str" xml:space="preserve">
         <v xml:space="preserve">Excelente atención del joven y mucha variedad de plantas!!
 Compré tierra para macetas, me dijo el joven que era muy buena, pero huele muy mal, me pueden dar alguna sugerencia para eliminar ese olor tan fuerte?! Por favor!!,Me encantan todas las plantas, son muy amables, los precios justos🤩…,Muy bonito vivero</v>
       </c>
-      <c r="M3" t="str">
+      <c r="N3" t="str">
         <v>https://lh5.googleusercontent.com/p/AF1QipPmQSXM5PoyrFj8IU2GdEEKh9C_3Ku5CJxKUUUM=w408-h306-k-no</v>
       </c>
-      <c r="N3" t="str">
+      <c r="O3" t="str">
         <v>wget --no-check-certificate https://lh5.googleusercontent.com/p/AF1QipPmQSXM5PoyrFj8IU2GdEEKh9C_3Ku5CJxKUUUM=w408-h306-k-no</v>
       </c>
-      <c r="O3" t="str">
+      <c r="P3" t="str">
         <v>AF1QipPmQSXM5PoyrFj8IU2GdEEKh9C_3Ku5CJxKUUUM=w408-h306-k-no</v>
       </c>
-      <c r="P3" t="str">
+      <c r="Q3" t="str">
         <v>Vivero_Las_Magnolias_1</v>
       </c>
-      <c r="Q3" t="str">
+      <c r="R3" t="str">
         <v>https://rumbonaturaleza.com/wp-content/uploads/2023/03/Vivero_Las_Magnolias_1.jpg</v>
       </c>
-      <c r="R3" t="str">
+      <c r="S3" t="str">
         <v>ren "AF1QipPmQSXM5PoyrFj8IU2GdEEKh9C_3Ku5CJxKUUUM=w408-h306-k-no" "Vivero_Las_Magnolias_1.jpg"</v>
       </c>
-      <c r="S3" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-                    &lt;p&gt; ¿Estás buscando los mejores Parques Ecoturísticos en Tabasco? ¡Estás en el lugar correcto! Pues en este artículo vamos a presentarte cuáles son los  Sitio Ecoturístico que han sido mejor evaluados en este estado. 
- Para esto, realizamos consultas en un montón de fuentes oficiales, redes sociales, rankings e incluso entrevistas para poder determinar cuáles son los  Parque de Ecoturismo que mejor calificación han recibido en Tabasco durante los últimos años. 
- Con esta prueba social como respaldo, hoy te daremos los Centro Ecoturístico mejor calificados y te compartiremos su ubicación, medios oficiales de contacto, horarios y cómo llegar hasta ellos, junto con la calificación promedio con la que cuenta cada lugar. 
- Así que prepárate y ¡a disfrutar del ecoturismo en Tabasco!&lt;/p&gt;                    
-                    </v>
-      </c>
       <c r="T3" t="str" xml:space="preserve">
         <v xml:space="preserve">
-                    &lt;p&gt; ¿Estás buscando los mejores Parques Ecoturísticos en Tabasco? ¡Estás en el lugar correcto! Pues en este artículo vamos a presentarte cuáles son los  Sitio Ecoturístico que han sido mejor evaluados en este estado. 
- Para esto, realizamos consultas en un montón de fuentes oficiales, redes sociales, rankings e incluso entrevistas para poder determinar cuáles son los  Parque de Ecoturismo que mejor calificación han recibido en Tabasco durante los últimos años. 
- Con esta prueba social como respaldo, hoy te daremos los Centro Ecoturístico mejor calificados y te compartiremos su ubicación, medios oficiales de contacto, horarios y cómo llegar hasta ellos, junto con la calificación promedio con la que cuenta cada lugar. 
+                    &lt;p&gt; ¿Estás buscando los mejores Parques Ecoturísticos en Tabasco? ¡Estás en el lugar correcto! Pues en este artículo vamos a presentarte cuáles son los  Parque Natural que han sido mejor evaluados en este estado. 
+ Para esto, realizamos consultas en un montón de fuentes oficiales, redes sociales, rankings e incluso entrevistas para poder determinar cuáles son los  Parque Ecológico que mejor calificación han recibido en Tabasco durante los últimos años. 
+ Con esta prueba social como respaldo, hoy te daremos los Parque Ecológico mejor calificados y te compartiremos su ubicación, medios oficiales de contacto, horarios y cómo llegar hasta ellos, junto con la calificación promedio con la que cuenta cada lugar. 
  Así que prepárate y ¡a disfrutar del ecoturismo en Tabasco!&lt;/p&gt;                    
                     </v>
       </c>
       <c r="U3" t="str" xml:space="preserve">
         <v xml:space="preserve">
+                    &lt;p&gt; ¿Estás buscando los mejores Parques Ecoturísticos en Tabasco? ¡Estás en el lugar correcto! Pues en este artículo vamos a presentarte cuáles son los  Parque Natural que han sido mejor evaluados en este estado. 
+ Para esto, realizamos consultas en un montón de fuentes oficiales, redes sociales, rankings e incluso entrevistas para poder determinar cuáles son los  Parque Ecológico que mejor calificación han recibido en Tabasco durante los últimos años. 
+ Con esta prueba social como respaldo, hoy te daremos los Parque Ecológico mejor calificados y te compartiremos su ubicación, medios oficiales de contacto, horarios y cómo llegar hasta ellos, junto con la calificación promedio con la que cuenta cada lugar. 
+ Así que prepárate y ¡a disfrutar del ecoturismo en Tabasco!&lt;/p&gt;                    
+                    </v>
+      </c>
+      <c r="V3" t="str" xml:space="preserve">
+        <v xml:space="preserve">
                     &lt;h2&gt;&lt;b&gt;Parque Ecoturístico Vivero Las Magnolias&lt;/b&gt;&lt;/h2&gt;
-                        &lt;p&gt;Este Parque Ecoturístico tiene 4.7 de calificación promedio, a partir de las más de 106 opiniones de sus visitantes... ¿nada mal no?. Es por eso que es parte de esta lista de los Parque Ecoturístico mejor calificados de Tabasco. Con este respaldo estamos más que seguras(os) que se trata  de un sitio que vas a disfrutar al Máximo. Así que ya sabes, si lo que buscas es naturaleza, el Parque Ecoturístico undefineden Tabasco, es sin duda una gran opción&lt;/p&gt;
-                        &lt;h3&gt;&lt;b&gt;¿Cómo llegar al Parque Natural Vivero Las Magnolias? &lt;/b&gt;&lt;/h3&gt;
-                            &lt;p&gt;El Parque de Ecoturismo se ubica enSauca 103, Jardines de Durango, 34200 Durango, Dgo.. Puedes ir a este lugar sin problemas manejando, sólo coloca su dirección oficial en waze, google maps o equivalente, o guíate con este &lt;a href='https://www.google.com.mx/maps/place/Vivero+Las+Magnolias/data=!4m7!3m6!1s0x869bb7b871872b85:0x65cc8cefdc6b7345!8m2!3d24.0374832!4d-104.6351623!16s%2Fg%2F11b6j5b_lw!19sChIJhSuHcbi3m4YRRXNr3O-MzGU?authuser=0&amp;hl=es&amp;rclk=1'&gt;Mapa del Parque Ecoturístico Vivero Las Magnolias&lt;/a&gt;&lt;/p&gt;
-                        &lt;h3&gt;&lt;b&gt;¿Cuáles son los contactos del Sitio Ecoturístico Vivero Las Magnolias?&lt;/b&gt;&lt;/h3&gt;
-                            &lt;p&gt;Los contactos disponibles del Centro de Ecoturismo Vivero Las Magnolias son: &lt;/p&gt;
+                        &lt;img src="https://rumbonaturaleza.com/wp-content/uploads/2023/03/Vivero_Las_Magnolias_1.jpg" alt="Vivero Las Magnolias"&gt;   
+                        &lt;div&gt;&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3643.8179757079024!2d-104.63516229999999!3d24.037483200000004!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x869bb7b871872b85%3A0x65cc8cefdc6b7345!2sVivero%20Las%20Magnolias!5e0!3m2!1ses!2smx!4v1678840876876!5m2!1ses!2smx" width="600" height="450" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;&lt;/div&gt;
+                        &lt;div&gt;&lt;/div&gt;
+                        &lt;p&gt;El Parque Ecoturístico undefined es una opción fantástica para tener una aventura natural en Tabasco. Su calificación promedio es de 4.7 respaldada por más de 106visitantes, así que no tenemos duda de que este lugar pertenece a la lista de los Parque Ecoturístico mejor rankeados de Tabasco y que se trata de uno de los principales atractivos naturales en la región. Así que ya sabes... ¿ganas de naturaleza?... pues el Parque Ecoturístico undefined es una grandísima opción.&lt;/p&gt;
+                        &lt;h3&gt;&lt;b&gt;¿Cómo llegar al Parque Ecoturístico Vivero Las Magnolias? &lt;/b&gt;&lt;/h3&gt;
+                            &lt;p&gt;El Parque Ecoturístico se ubica enSauca 103, Jardines de Durango, 34200 Durango, Dgo.. Para llegar, puedes símplemente colocar esta dirección en el googleMaps o Waze o apoyarte en este &lt;a href='https://www.google.com.mx/maps/place/Vivero+Las+Magnolias/@24.0374832,-104.6351623,17z/data=!3m1!4b1!4m6!3m5!1s0x869bb7b871872b85:0x65cc8cefdc6b7345!8m2!3d24.0374832!4d-104.6351623!16s%2Fg%2F11b6j5b_lw?authuser=0&amp;hl=es'&gt;Mapa del Parque Ecoturístico Vivero Las Magnolias&lt;/a&gt;&lt;/p&gt;
+                        &lt;h3&gt;&lt;b&gt;¿Cuáles son los contactos del Parque Ecoturístico Vivero Las Magnolias?&lt;/b&gt;&lt;/h3&gt;
+                            &lt;p&gt;Los contactos disponibles del Parque de Ecoturismo Vivero Las Magnolias son: &lt;/p&gt;
                             &lt;ul&gt;
                                 &lt;li&gt;&lt;b&gt;Teléfono:&lt;/b&gt;618 129 7673&lt;/li&gt;
                                 &lt;li&gt;&lt;b&gt;SitioWeb:&lt;/b&gt;web no disponible&lt;/li&gt;                                
                             &lt;/ul&gt;
-                        &lt;h3&gt;&lt;b&gt;¿En qué horarios y días se puede visitar el Parque de Ecoturismo Vivero Las Magnolias?&lt;/b&gt;&lt;/h3&gt;
-                            &lt;p&gt;Los horarios oficiales del Centro de Ecoturismo Vivero Las Magnolias son los siguientes:&lt;/p&gt;                       
-                            &lt;ul&gt;
-                                &lt;li&gt;Lunes de 09:00 a 18:00&lt;/li&gt;
+                        &lt;h3&gt;&lt;b&gt;¿En qué horarios y días se puede visitar el Sitio Ecoturístico Vivero Las Magnolias?&lt;/b&gt;&lt;/h3&gt;
+                            &lt;p&gt;Los horarios oficiales del Parque Ecoturístico Vivero Las Magnolias son los siguientes:&lt;/p&gt;                       
+                            &lt;ul&gt;
+                                &lt;li&gt;Lunes (Natalicio de Benito Juárez (feriado)) de 09:00 a 18:00 El horario podría cambiar&lt;/li&gt;
                                 &lt;li&gt;Martes de 09:00 a 18:00&lt;/li&gt;
                                 &lt;li&gt;Miércoles de 09:00 a 18:00&lt;/li&gt;
                                 &lt;li&gt;Jueves de 09:00 a 18:00&lt;/li&gt;
@@ -668,15 +683,15 @@
                                 &lt;li&gt;Sábado de 09:00 a 18:00&lt;/li&gt;
                                 &lt;li&gt;Domingo de 09:00 a 17:00&lt;/li&gt;
                             &lt;/ul&gt;
-                            &lt;p&gt;A pesar de contar con horarios oficiales, te recomendamos siempre visitar sus sitios de contacto y redes oficiales antes de ir al lugar, así podrás identificar cualquier cambio extraordinario que hayan tenido.&lt;/p&gt;                 
-                    </v>
-      </c>
-      <c r="V3" t="str" xml:space="preserve">
+                            &lt;p&gt;Aunque estos horarios están oficialmente vigentes, siempre es bueno consultar sus sitios de contacto y redes oficiales antes de visitarlos, por cualquier cambio extraordinario que pudieran tener.&lt;/p&gt;                 
+                    </v>
+      </c>
+      <c r="W3" t="str" xml:space="preserve">
         <v xml:space="preserve">
                     &lt;img src="https://rumbonaturaleza.com/wp-content/uploads/2023/03/Vivero_Las_Magnolias_1.jpg" alt="Vivero Las Magnolias"&gt;                
                 </v>
       </c>
-      <c r="W3" t="str">
+      <c r="X3" t="str">
         <v>Añadir sitio web</v>
       </c>
     </row>
@@ -700,70 +715,76 @@
         <v>Durango</v>
       </c>
       <c r="H4" t="str">
-        <v>https://www.google.com.mx/maps/place/VIVERO%C2%B4S+AVE+DE+PARAISO/data=!4m7!3m6!1s0x869bb7f0d4ea30ef:0x4cb36ed930d8acad!8m2!3d24.008504!4d-104.644488!16s%2Fg%2F11ddx2_b8h!19sChIJ7zDq1PC3m4YRrazYMNlus0w?authuser=0&amp;hl=es&amp;rclk=1</v>
+        <v>https://www.google.com.mx/maps/place/VIVERO%C2%B4S+AVE+DE+PARAISO/@24.008504,-104.644488,17z/data=!3m1!4b1!4m6!3m5!1s0x869bb7f0d4ea30ef:0x4cb36ed930d8acad!8m2!3d24.008504!4d-104.644488!16s%2Fg%2F11ddx2_b8h?authuser=0&amp;hl=es</v>
       </c>
       <c r="I4" t="str">
+        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3644.639501915154!2d-104.64448800000001!3d24.008503999999995!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x869bb7f0d4ea30ef%3A0x4cb36ed930d8acad!2sVIVERO%C2%B4S%20AVE%20DE%20PARAISO!5e0!3m2!1ses!2smx!4v1678840881035!5m2!1ses!2smx" width="600" height="450" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
+      </c>
+      <c r="J4" t="str">
         <v>2954+C6 Durango</v>
       </c>
-      <c r="J4" t="str">
+      <c r="K4" t="str">
         <v>4.3</v>
       </c>
-      <c r="K4" t="str">
+      <c r="L4" t="str">
         <v>21</v>
       </c>
-      <c r="L4" t="str">
+      <c r="M4" t="str">
         <v>Mala atención,Las nochebuenas estan hermosas, no me fui de ahí sin las mías, lastimas que el resto de plantas están muy amontonadas y no se pueden apreciar bien,Tienen una gran variedad de plantas</v>
       </c>
-      <c r="M4" t="str">
+      <c r="N4" t="str">
         <v>https://lh5.googleusercontent.com/p/AF1QipMOYk2QlPDlj4I6VmQIIolnA3Ipl8mWjdIXSvrS=w408-h725-k-no</v>
       </c>
-      <c r="N4" t="str">
+      <c r="O4" t="str">
         <v>wget --no-check-certificate https://lh5.googleusercontent.com/p/AF1QipMOYk2QlPDlj4I6VmQIIolnA3Ipl8mWjdIXSvrS=w408-h725-k-no</v>
       </c>
-      <c r="O4" t="str">
+      <c r="P4" t="str">
         <v>AF1QipMOYk2QlPDlj4I6VmQIIolnA3Ipl8mWjdIXSvrS=w408-h725-k-no</v>
       </c>
-      <c r="P4" t="str">
+      <c r="Q4" t="str">
         <v>VIVERO´S_AVE_DE_PARAISO_2</v>
       </c>
-      <c r="Q4" t="str">
+      <c r="R4" t="str">
         <v>https://rumbonaturaleza.com/wp-content/uploads/2023/03/VIVERO´S_AVE_DE_PARAISO_2.jpg</v>
       </c>
-      <c r="R4" t="str">
+      <c r="S4" t="str">
         <v>ren "AF1QipMOYk2QlPDlj4I6VmQIIolnA3Ipl8mWjdIXSvrS=w408-h725-k-no" "VIVERO´S_AVE_DE_PARAISO_2.jpg"</v>
       </c>
-      <c r="S4" t="str" xml:space="preserve">
+      <c r="T4" t="str" xml:space="preserve">
         <v xml:space="preserve">
                     &lt;p&gt; ¿Estás buscando los mejores Parques Ecoturísticos en Tabasco? ¡Estás en el lugar correcto! Pues en este artículo vamos a presentarte cuáles son los  Parque Ecoturístico que han sido mejor evaluados en este estado. 
- Para esto, realizamos consultas en un montón de fuentes oficiales, redes sociales, rankings e incluso entrevistas para poder determinar cuáles son los  Parque Ecoturístico que mejor calificación han recibido en Tabasco durante los últimos años. 
- Con esta prueba social como respaldo, hoy te daremos los Parque Ecoturístico mejor calificados y te compartiremos su ubicación, medios oficiales de contacto, horarios y cómo llegar hasta ellos, junto con la calificación promedio con la que cuenta cada lugar. 
- Así que prepárate y ¡a disfrutar del ecoturismo en Tabasco!&lt;/p&gt;                    
-                    </v>
-      </c>
-      <c r="T4" t="str" xml:space="preserve">
+ Para esto, realizamos consultas en un montón de fuentes oficiales, redes sociales, rankings e incluso entrevistas para poder determinar cuáles son los  Centro Ecoturístico que mejor calificación han recibido en Tabasco durante los últimos años. 
+ Con esta prueba social como respaldo, hoy te daremos los Parque Ecológico mejor calificados y te compartiremos su ubicación, medios oficiales de contacto, horarios y cómo llegar hasta ellos, junto con la calificación promedio con la que cuenta cada lugar. 
+ Así que prepárate y ¡a disfrutar del ecoturismo en Tabasco!&lt;/p&gt;                    
+                    </v>
+      </c>
+      <c r="U4" t="str" xml:space="preserve">
         <v xml:space="preserve">
                     &lt;p&gt; ¿Estás buscando los mejores Parques Ecoturísticos en Tabasco? ¡Estás en el lugar correcto! Pues en este artículo vamos a presentarte cuáles son los  Parque Ecoturístico que han sido mejor evaluados en este estado. 
- Para esto, realizamos consultas en un montón de fuentes oficiales, redes sociales, rankings e incluso entrevistas para poder determinar cuáles son los  Parque Ecoturístico que mejor calificación han recibido en Tabasco durante los últimos años. 
- Con esta prueba social como respaldo, hoy te daremos los Parque Ecoturístico mejor calificados y te compartiremos su ubicación, medios oficiales de contacto, horarios y cómo llegar hasta ellos, junto con la calificación promedio con la que cuenta cada lugar. 
- Así que prepárate y ¡a disfrutar del ecoturismo en Tabasco!&lt;/p&gt;                    
-                    </v>
-      </c>
-      <c r="U4" t="str" xml:space="preserve">
+ Para esto, realizamos consultas en un montón de fuentes oficiales, redes sociales, rankings e incluso entrevistas para poder determinar cuáles son los  Centro Ecoturístico que mejor calificación han recibido en Tabasco durante los últimos años. 
+ Con esta prueba social como respaldo, hoy te daremos los Parque Ecológico mejor calificados y te compartiremos su ubicación, medios oficiales de contacto, horarios y cómo llegar hasta ellos, junto con la calificación promedio con la que cuenta cada lugar. 
+ Así que prepárate y ¡a disfrutar del ecoturismo en Tabasco!&lt;/p&gt;                    
+                    </v>
+      </c>
+      <c r="V4" t="str" xml:space="preserve">
         <v xml:space="preserve">
                     &lt;h2&gt;&lt;b&gt;Parque Ecoturístico VIVERO´S AVE DE PARAISO&lt;/b&gt;&lt;/h2&gt;
-                        &lt;p&gt;El Parque Ecoturístico undefined es una opción fantástica para tener una aventura natural en Tabasco. Su calificación promedio es de 4.3 respaldada por más de 21visitantes, así que no tenemos duda de que este lugar pertenece a la lista de los Parque Ecoturístico mejor rankeados de Tabasco y que se trata de uno de los principales atractivos naturales en la región. Así que ya sabes... ¿ganas de naturaleza?... pues el Parque Ecoturístico undefined es una grandísima opción.&lt;/p&gt;
-                        &lt;h3&gt;&lt;b&gt;¿Cómo llegar al Parque Ecológico VIVERO´S AVE DE PARAISO? &lt;/b&gt;&lt;/h3&gt;
-                            &lt;p&gt;El Centro Ecoturístico se ubica enCalle Nazas 614, Los Sauces, 34078 Durango, Dgo.. Para llegar, puedes símplemente colocar esta dirección en el googleMaps o Waze o apoyarte en este &lt;a href='https://www.google.com.mx/maps/place/VIVERO%C2%B4S+AVE+DE+PARAISO/data=!4m7!3m6!1s0x869bb7f0d4ea30ef:0x4cb36ed930d8acad!8m2!3d24.008504!4d-104.644488!16s%2Fg%2F11ddx2_b8h!19sChIJ7zDq1PC3m4YRrazYMNlus0w?authuser=0&amp;hl=es&amp;rclk=1'&gt;Mapa del Parque Ecoturístico VIVERO´S AVE DE PARAISO&lt;/a&gt;&lt;/p&gt;
-                        &lt;h3&gt;&lt;b&gt;¿Cuáles son los contactos del Centro de Ecoturismo VIVERO´S AVE DE PARAISO?&lt;/b&gt;&lt;/h3&gt;
-                            &lt;p&gt;Los contactos disponibles del Sitio Ecoturístico VIVERO´S AVE DE PARAISO son: &lt;/p&gt;
+                        &lt;img src="https://rumbonaturaleza.com/wp-content/uploads/2023/03/VIVERO´S_AVE_DE_PARAISO_2.jpg" alt="VIVERO´S AVE DE PARAISO"&gt;   
+                        &lt;div&gt;&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3644.639501915154!2d-104.64448800000001!3d24.008503999999995!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x869bb7f0d4ea30ef%3A0x4cb36ed930d8acad!2sVIVERO%C2%B4S%20AVE%20DE%20PARAISO!5e0!3m2!1ses!2smx!4v1678840881035!5m2!1ses!2smx" width="600" height="450" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;&lt;/div&gt;
+                        &lt;div&gt;&lt;/div&gt;
+                        &lt;p&gt;Bueno pues si eres de quienes ama estar en contacto con la naturaleza y andas por Tabasco, entonces no puedes perderte la experiencia de visitar el Parque Ecoturístico undefined. Con una calificación promedio de 4.3 estrellas de más de Mala atención,Las nochebuenas estan hermosas, no me fui de ahí sin las mías, lastimas que el resto de plantas están muy amontonadas y no se pueden apreciar bien,Tienen una gran variedad de plantas visitantes, no tenemos duda de que se trata de un favorito de esta región. Así que nada...prepárate para sumergirte y disfrutar a tope de los paisajes naturales de Tabasco&lt;/p&gt;
+                        &lt;h3&gt;&lt;b&gt;¿Cómo llegar al Parque Ecoturístico VIVERO´S AVE DE PARAISO? &lt;/b&gt;&lt;/h3&gt;
+                            &lt;p&gt;El Parque Ecológico se ubica enCalle Nazas 614, Los Sauces, 34078 Durango, Dgo.. Puedes ir a este lugar sin problemas manejando, sólo coloca su dirección oficial en waze, google maps o equivalente, o guíate con este &lt;a href='https://www.google.com.mx/maps/place/VIVERO%C2%B4S+AVE+DE+PARAISO/@24.008504,-104.644488,17z/data=!3m1!4b1!4m6!3m5!1s0x869bb7f0d4ea30ef:0x4cb36ed930d8acad!8m2!3d24.008504!4d-104.644488!16s%2Fg%2F11ddx2_b8h?authuser=0&amp;hl=es'&gt;Mapa del Parque Ecoturístico VIVERO´S AVE DE PARAISO&lt;/a&gt;&lt;/p&gt;
+                        &lt;h3&gt;&lt;b&gt;¿Cuáles son los contactos del Parque de Ecoturismo VIVERO´S AVE DE PARAISO?&lt;/b&gt;&lt;/h3&gt;
+                            &lt;p&gt;Los contactos disponibles del Parque de Ecoturismo VIVERO´S AVE DE PARAISO son: &lt;/p&gt;
                             &lt;ul&gt;
                                 &lt;li&gt;&lt;b&gt;Teléfono:&lt;/b&gt;618 818 0964&lt;/li&gt;
                                 &lt;li&gt;&lt;b&gt;SitioWeb:&lt;/b&gt;&lt;a href="https://www.instagram.com/invites/contact/?i=1rjinh0zovkbr&amp;utm_content=myh4mm5"&gt;Web del place VIVERO´S AVE DE PARAISO&lt;/a&gt;&lt;/li&gt;                                
                             &lt;/ul&gt;
-                        &lt;h3&gt;&lt;b&gt;¿En qué horarios y días se puede visitar el Sitio Ecoturístico VIVERO´S AVE DE PARAISO?&lt;/b&gt;&lt;/h3&gt;
+                        &lt;h3&gt;&lt;b&gt;¿En qué horarios y días se puede visitar el Parque Ecoturístico VIVERO´S AVE DE PARAISO?&lt;/b&gt;&lt;/h3&gt;
                             &lt;p&gt;Los horarios oficiales del Parque Ecoturístico VIVERO´S AVE DE PARAISO son los siguientes:&lt;/p&gt;                       
                             &lt;ul&gt;
-                                &lt;li&gt;Lunes de 08:00 a 19:00&lt;/li&gt;
+                                &lt;li&gt;Lunes (Natalicio de Benito Juárez (feriado)) de 08:00 a 19:00 El horario podría cambiar&lt;/li&gt;
                                 &lt;li&gt;Martes de 08:00 a 19:00&lt;/li&gt;
                                 &lt;li&gt;Miércoles de 08:00 a 19:00&lt;/li&gt;
                                 &lt;li&gt;Jueves de 08:00 a 19:00&lt;/li&gt;
@@ -771,15 +792,15 @@
                                 &lt;li&gt;Sábado de 08:00 a 17:00&lt;/li&gt;
                                 &lt;li&gt;Domingo de 09:00 a 17:00&lt;/li&gt;
                             &lt;/ul&gt;
-                            &lt;p&gt;Aunque cuentes ya con los horarios oficiales de apertura de este lugar, siempre te recomendamos que antes de ir eches un ojito a sus redes sociales y vías de contacto, para asegurarte de que no hayan tenido algún cambio logístico de última hora&lt;/p&gt;                 
-                    </v>
-      </c>
-      <c r="V4" t="str" xml:space="preserve">
+                            &lt;p&gt;A pesar de contar con horarios oficiales, te recomendamos siempre visitar sus sitios de contacto y redes oficiales antes de ir al lugar, así podrás identificar cualquier cambio extraordinario que hayan tenido.&lt;/p&gt;                 
+                    </v>
+      </c>
+      <c r="W4" t="str" xml:space="preserve">
         <v xml:space="preserve">
                     &lt;img src="https://rumbonaturaleza.com/wp-content/uploads/2023/03/VIVERO´S_AVE_DE_PARAISO_2.jpg" alt="VIVERO´S AVE DE PARAISO"&gt;                
                 </v>
       </c>
-      <c r="W4" t="str">
+      <c r="X4" t="str">
         <v/>
       </c>
     </row>
@@ -803,72 +824,78 @@
         <v>Durango</v>
       </c>
       <c r="H5" t="str">
-        <v>https://www.google.com.mx/maps/place/Vivero+Santa+Fe/data=!4m7!3m6!1s0x869bc7de9a5a690f:0x1c9d03d9335b8bbd!8m2!3d23.9936822!4d-104.6858595!16s%2Fg%2F11b6jgmr3h!19sChIJD2lamt7Hm4YRvYtbM9kDnRw?authuser=0&amp;hl=es&amp;rclk=1</v>
+        <v>https://www.google.com.mx/maps/place/Vivero+Santa+Fe/@23.9936822,-104.6858595,17z/data=!3m1!4b1!4m6!3m5!1s0x869bc7de9a5a690f:0x1c9d03d9335b8bbd!8m2!3d23.9936822!4d-104.6858595!16s%2Fg%2F11b6jgmr3h?authuser=0&amp;hl=es</v>
       </c>
       <c r="I5" t="str">
+        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3645.059322127962!2d-104.68585949999999!3d23.993682200000002!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x869bc7de9a5a690f%3A0x1c9d03d9335b8bbd!2sVivero%20Santa%20Fe!5e0!3m2!1ses!2smx!4v1678840885276!5m2!1ses!2smx" width="600" height="450" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
+      </c>
+      <c r="J5" t="str">
         <v>X8V7+FM Durango</v>
       </c>
-      <c r="J5" t="str">
+      <c r="K5" t="str">
         <v>4.4</v>
       </c>
-      <c r="K5" t="str">
+      <c r="L5" t="str">
         <v>52</v>
       </c>
-      <c r="L5" t="str" xml:space="preserve">
+      <c r="M5" t="str" xml:space="preserve">
         <v xml:space="preserve">Gran surtido de plantas y pasto de muy buena calidad,Tiene gran variedad de plantas, pero sus precios no son nada asequibles, inclusive precios triplicados en cuanto a precios en otros viveros...,Muchas plantas muy bonitas
 Para Sol y sombra y buenos precios
 Sí lo recomiendo.</v>
       </c>
-      <c r="M5" t="str">
-        <v>no hay foto</v>
-      </c>
       <c r="N5" t="str">
-        <v>wget --no-check-certificate no hay foto</v>
+        <v>https://lh5.googleusercontent.com/p/AF1QipNrN9F6dstJ2M3M7lFIyGQEZFWkNlnH0euKP8Hi=w426-h240-k-no</v>
       </c>
       <c r="O5" t="str">
-        <v>no hay foto</v>
+        <v>wget --no-check-certificate https://lh5.googleusercontent.com/p/AF1QipNrN9F6dstJ2M3M7lFIyGQEZFWkNlnH0euKP8Hi=w426-h240-k-no</v>
       </c>
       <c r="P5" t="str">
+        <v>AF1QipNrN9F6dstJ2M3M7lFIyGQEZFWkNlnH0euKP8Hi=w426-h240-k-no</v>
+      </c>
+      <c r="Q5" t="str">
         <v>Vivero_Santa_Fe_3</v>
       </c>
-      <c r="Q5" t="str">
+      <c r="R5" t="str">
         <v>https://rumbonaturaleza.com/wp-content/uploads/2023/03/Vivero_Santa_Fe_3.jpg</v>
       </c>
-      <c r="R5" t="str">
-        <v>ren "no hay foto" "Vivero_Santa_Fe_3.jpg"</v>
-      </c>
-      <c r="S5" t="str" xml:space="preserve">
+      <c r="S5" t="str">
+        <v>ren "AF1QipNrN9F6dstJ2M3M7lFIyGQEZFWkNlnH0euKP8Hi=w426-h240-k-no" "Vivero_Santa_Fe_3.jpg"</v>
+      </c>
+      <c r="T5" t="str" xml:space="preserve">
         <v xml:space="preserve">
                     &lt;p&gt; ¿Estás buscando los mejores Parques Ecoturísticos en Tabasco? ¡Estás en el lugar correcto! Pues en este artículo vamos a presentarte cuáles son los  Parque Ecoturístico que han sido mejor evaluados en este estado. 
- Para esto, realizamos consultas en un montón de fuentes oficiales, redes sociales, rankings e incluso entrevistas para poder determinar cuáles son los  Parque Ecoturístico que mejor calificación han recibido en Tabasco durante los últimos años. 
- Con esta prueba social como respaldo, hoy te daremos los Sitio Ecoturístico mejor calificados y te compartiremos su ubicación, medios oficiales de contacto, horarios y cómo llegar hasta ellos, junto con la calificación promedio con la que cuenta cada lugar. 
- Así que prepárate y ¡a disfrutar del ecoturismo en Tabasco!&lt;/p&gt;                    
-                    </v>
-      </c>
-      <c r="T5" t="str" xml:space="preserve">
+ Para esto, realizamos consultas en un montón de fuentes oficiales, redes sociales, rankings e incluso entrevistas para poder determinar cuáles son los  Parque de Ecoturismo que mejor calificación han recibido en Tabasco durante los últimos años. 
+ Con esta prueba social como respaldo, hoy te daremos los Centro de Ecoturismo mejor calificados y te compartiremos su ubicación, medios oficiales de contacto, horarios y cómo llegar hasta ellos, junto con la calificación promedio con la que cuenta cada lugar. 
+ Así que prepárate y ¡a disfrutar del ecoturismo en Tabasco!&lt;/p&gt;                    
+                    </v>
+      </c>
+      <c r="U5" t="str" xml:space="preserve">
         <v xml:space="preserve">
                     &lt;p&gt; ¿Estás buscando los mejores Parques Ecoturísticos en Tabasco? ¡Estás en el lugar correcto! Pues en este artículo vamos a presentarte cuáles son los  Parque Ecoturístico que han sido mejor evaluados en este estado. 
- Para esto, realizamos consultas en un montón de fuentes oficiales, redes sociales, rankings e incluso entrevistas para poder determinar cuáles son los  Parque Ecoturístico que mejor calificación han recibido en Tabasco durante los últimos años. 
- Con esta prueba social como respaldo, hoy te daremos los Sitio Ecoturístico mejor calificados y te compartiremos su ubicación, medios oficiales de contacto, horarios y cómo llegar hasta ellos, junto con la calificación promedio con la que cuenta cada lugar. 
- Así que prepárate y ¡a disfrutar del ecoturismo en Tabasco!&lt;/p&gt;                    
-                    </v>
-      </c>
-      <c r="U5" t="str" xml:space="preserve">
+ Para esto, realizamos consultas en un montón de fuentes oficiales, redes sociales, rankings e incluso entrevistas para poder determinar cuáles son los  Parque de Ecoturismo que mejor calificación han recibido en Tabasco durante los últimos años. 
+ Con esta prueba social como respaldo, hoy te daremos los Centro de Ecoturismo mejor calificados y te compartiremos su ubicación, medios oficiales de contacto, horarios y cómo llegar hasta ellos, junto con la calificación promedio con la que cuenta cada lugar. 
+ Así que prepárate y ¡a disfrutar del ecoturismo en Tabasco!&lt;/p&gt;                    
+                    </v>
+      </c>
+      <c r="V5" t="str" xml:space="preserve">
         <v xml:space="preserve">
                     &lt;h2&gt;&lt;b&gt;Parque Ecoturístico Vivero Santa Fe&lt;/b&gt;&lt;/h2&gt;
+                        &lt;img src="https://rumbonaturaleza.com/wp-content/uploads/2023/03/Vivero_Santa_Fe_3.jpg" alt="Vivero Santa Fe"&gt;   
+                        &lt;div&gt;&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3645.059322127962!2d-104.68585949999999!3d23.993682200000002!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x869bc7de9a5a690f%3A0x1c9d03d9335b8bbd!2sVivero%20Santa%20Fe!5e0!3m2!1ses!2smx!4v1678840885276!5m2!1ses!2smx" width="600" height="450" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;&lt;/div&gt;
+                        &lt;div&gt;&lt;/div&gt;
                         &lt;p&gt;El Parque Ecoturístico undefined es una opción fantástica para tener una aventura natural en Tabasco. Su calificación promedio es de 4.4 respaldada por más de 52visitantes, así que no tenemos duda de que este lugar pertenece a la lista de los Parque Ecoturístico mejor rankeados de Tabasco y que se trata de uno de los principales atractivos naturales en la región. Así que ya sabes... ¿ganas de naturaleza?... pues el Parque Ecoturístico undefined es una grandísima opción.&lt;/p&gt;
                         &lt;h3&gt;&lt;b&gt;¿Cómo llegar al Parque Ecoturístico Vivero Santa Fe? &lt;/b&gt;&lt;/h3&gt;
-                            &lt;p&gt;El Parque Ecoturístico se ubica enC. Victoria 106, Arroyo Seco, 34147 Durango, Dgo.. Para ir a este parque, simplemente basta con colocar la dirección en una app de navegación o siguiendo este &lt;a href='https://www.google.com.mx/maps/place/Vivero+Santa+Fe/data=!4m7!3m6!1s0x869bc7de9a5a690f:0x1c9d03d9335b8bbd!8m2!3d23.9936822!4d-104.6858595!16s%2Fg%2F11b6jgmr3h!19sChIJD2lamt7Hm4YRvYtbM9kDnRw?authuser=0&amp;hl=es&amp;rclk=1'&gt;Mapa del Parque Ecoturístico Vivero Santa Fe&lt;/a&gt;&lt;/p&gt;
-                        &lt;h3&gt;&lt;b&gt;¿Cuáles son los contactos del Parque Ecoturístico Vivero Santa Fe?&lt;/b&gt;&lt;/h3&gt;
-                            &lt;p&gt;Los contactos disponibles del Parque de Ecoturismo Vivero Santa Fe son: &lt;/p&gt;
+                            &lt;p&gt;El Parque Ecoturístico se ubica enC. Victoria 106, Arroyo Seco, 34147 Durango, Dgo.. Para ir a este sitio, coloca esta dirección en una herramienta de navegación o apóyate con este &lt;a href='https://www.google.com.mx/maps/place/Vivero+Santa+Fe/@23.9936822,-104.6858595,17z/data=!3m1!4b1!4m6!3m5!1s0x869bc7de9a5a690f:0x1c9d03d9335b8bbd!8m2!3d23.9936822!4d-104.6858595!16s%2Fg%2F11b6jgmr3h?authuser=0&amp;hl=es'&gt;Mapa del Parque Ecoturístico Vivero Santa Fe&lt;/a&gt;&lt;/p&gt;
+                        &lt;h3&gt;&lt;b&gt;¿Cuáles son los contactos del Centro de Ecoturismo Vivero Santa Fe?&lt;/b&gt;&lt;/h3&gt;
+                            &lt;p&gt;Los contactos disponibles del Sitio Ecoturístico Vivero Santa Fe son: &lt;/p&gt;
                             &lt;ul&gt;
                                 &lt;li&gt;&lt;b&gt;Teléfono:&lt;/b&gt;618 120 0604&lt;/li&gt;
                                 &lt;li&gt;&lt;b&gt;SitioWeb:&lt;/b&gt;web no disponible&lt;/li&gt;                                
                             &lt;/ul&gt;
-                        &lt;h3&gt;&lt;b&gt;¿En qué horarios y días se puede visitar el Centro de Ecoturismo Vivero Santa Fe?&lt;/b&gt;&lt;/h3&gt;
-                            &lt;p&gt;Los horarios oficiales del Sitio Ecoturístico Vivero Santa Fe son los siguientes:&lt;/p&gt;                       
-                            &lt;ul&gt;
-                                &lt;li&gt;Lunes de 08:00 a 19:00&lt;/li&gt;
+                        &lt;h3&gt;&lt;b&gt;¿En qué horarios y días se puede visitar el Parque Ecoturístico Vivero Santa Fe?&lt;/b&gt;&lt;/h3&gt;
+                            &lt;p&gt;Los horarios oficiales del Parque Ecoturístico Vivero Santa Fe son los siguientes:&lt;/p&gt;                       
+                            &lt;ul&gt;
+                                &lt;li&gt;Lunes (Natalicio de Benito Juárez (feriado)) de 08:00 a 19:00 El horario podría cambiar&lt;/li&gt;
                                 &lt;li&gt;Martes de 08:00 a 19:00&lt;/li&gt;
                                 &lt;li&gt;Miércoles de 08:00 a 19:00&lt;/li&gt;
                                 &lt;li&gt;Jueves de 08:00 a 19:00&lt;/li&gt;
@@ -876,15 +903,15 @@
                                 &lt;li&gt;Sábado de 08:00 a 19:00&lt;/li&gt;
                                 &lt;li&gt;Domingo de 08:00 a 16:00&lt;/li&gt;
                             &lt;/ul&gt;
-                            &lt;p&gt;Aunque estos horarios sean oficialmente vigentes, nunca está de más que antes de lanzarte, revises en sus redes sociales o contactos digitales que no haya habido ningún cambio logístico extraordinario en sus horarios de apertura y cierre.&lt;/p&gt;                 
-                    </v>
-      </c>
-      <c r="V5" t="str" xml:space="preserve">
+                            &lt;p&gt;Aunque cuentes ya con los horarios oficiales de apertura de este lugar, siempre te recomendamos que antes de ir eches un ojito a sus redes sociales y vías de contacto, para asegurarte de que no hayan tenido algún cambio logístico de última hora&lt;/p&gt;                 
+                    </v>
+      </c>
+      <c r="W5" t="str" xml:space="preserve">
         <v xml:space="preserve">
                     &lt;img src="https://rumbonaturaleza.com/wp-content/uploads/2023/03/Vivero_Santa_Fe_3.jpg" alt="Vivero Santa Fe"&gt;                
                 </v>
       </c>
-      <c r="W5" t="str">
+      <c r="X5" t="str">
         <v>Añadir sitio web</v>
       </c>
     </row>
@@ -908,70 +935,76 @@
         <v>Durango</v>
       </c>
       <c r="H6" t="str">
-        <v>https://www.google.com.mx/maps/place/Vivero+Las+Palmas+De+Veracruz/data=!4m7!3m6!1s0x869bb7f86bc35165:0x2c2ed3acd58201b2!8m2!3d24.0040886!4d-104.6488795!16s%2Fg%2F11b6j9p3hk!19sChIJZVHDa_i3m4YRsgGC1azTLiw?authuser=0&amp;hl=es&amp;rclk=1</v>
+        <v>https://www.google.com.mx/maps/place/Vivero+Las+Palmas+De+Veracruz/@24.0040886,-104.6488795,17z/data=!3m1!4b1!4m6!3m5!1s0x869bb7f86bc35165:0x2c2ed3acd58201b2!8m2!3d24.0040886!4d-104.6488795!16s%2Fg%2F11b6j9p3hk?authuser=0&amp;hl=es</v>
       </c>
       <c r="I6" t="str">
+        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3644.7645914614886!2d-104.64887949999999!3d24.0040886!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x869bb7f86bc35165%3A0x2c2ed3acd58201b2!2sVivero%20Las%20Palmas%20De%20Veracruz!5e0!3m2!1ses!2smx!4v1678840889861!5m2!1ses!2smx" width="600" height="450" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
+      </c>
+      <c r="J6" t="str">
         <v>2932+JC Durango</v>
       </c>
-      <c r="J6" t="str">
+      <c r="K6" t="str">
         <v>4.6</v>
       </c>
-      <c r="K6" t="str">
+      <c r="L6" t="str">
         <v>65</v>
       </c>
-      <c r="L6" t="str">
+      <c r="M6" t="str">
         <v>En este vivero hay una gran variedad de plantas, flores 🥀, tierra, árboles etc. A muy buenos precios y una excelente atención lo recomiendo…,Muy amables, la señora que atiende es muy amable, te explica sobre las plantas, sólo que llega mucha gente y la abordan todos juntos, pero ella es muy linda y amable, además de que sus plantas super bonitas y muy cuidaditas.,Buen inventario de plantas y serviciales</v>
       </c>
-      <c r="M6" t="str">
-        <v>no hay foto</v>
-      </c>
       <c r="N6" t="str">
-        <v>wget --no-check-certificate no hay foto</v>
+        <v>https://lh3.googleusercontent.com/gps-proxy/ALm4wwme7VXgc2Weboi_HjqXsTwOoYDzDtl-7QULWTGauR_1pIM6JfwLo_H9Nol9a1_HTM3fCPFOVh7wQkl6kxAMWk5pDpL1VqQRniHWZFNj63HTU3Tj9HkhzDhZ7T3Fgkd6gg5XzmXkh3mG7bsdpm5QbMBg435MdUuWHNb4VyosQvmalS8qKv-xQwT3AFTKS3g9floAJcw=w408-h726-k-no</v>
       </c>
       <c r="O6" t="str">
-        <v>no hay foto</v>
+        <v>wget --no-check-certificate https://lh3.googleusercontent.com/gps-proxy/ALm4wwme7VXgc2Weboi_HjqXsTwOoYDzDtl-7QULWTGauR_1pIM6JfwLo_H9Nol9a1_HTM3fCPFOVh7wQkl6kxAMWk5pDpL1VqQRniHWZFNj63HTU3Tj9HkhzDhZ7T3Fgkd6gg5XzmXkh3mG7bsdpm5QbMBg435MdUuWHNb4VyosQvmalS8qKv-xQwT3AFTKS3g9floAJcw=w408-h726-k-no</v>
       </c>
       <c r="P6" t="str">
+        <v>ALm4wwme7VXgc2Weboi_HjqXsTwOoYDzDtl-7QULWTGauR_1pIM6JfwLo_H9Nol9a1_HTM3fCPFOVh7wQkl6kxAMWk5pDpL1VqQRniHWZFNj63HTU3Tj9HkhzDhZ7T3Fgkd6gg5XzmXkh3mG7bsdpm5QbMBg435MdUuWHNb4VyosQvmalS8qKv-xQwT3AFTKS3g9floAJcw=w408-h726-k-no</v>
+      </c>
+      <c r="Q6" t="str">
         <v>Vivero_Las_Palmas_De_Veracruz_4</v>
       </c>
-      <c r="Q6" t="str">
+      <c r="R6" t="str">
         <v>https://rumbonaturaleza.com/wp-content/uploads/2023/03/Vivero_Las_Palmas_De_Veracruz_4.jpg</v>
       </c>
-      <c r="R6" t="str">
-        <v>ren "no hay foto" "Vivero_Las_Palmas_De_Veracruz_4.jpg"</v>
-      </c>
-      <c r="S6" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-                    &lt;p&gt; ¿Estás buscando los mejores Parques Ecoturísticos en Tabasco? ¡Estás en el lugar correcto! Pues en este artículo vamos a presentarte cuáles son los  Centro de Ecoturismo que han sido mejor evaluados en este estado. 
- Para esto, realizamos consultas en un montón de fuentes oficiales, redes sociales, rankings e incluso entrevistas para poder determinar cuáles son los  Parque Ecoturístico que mejor calificación han recibido en Tabasco durante los últimos años. 
+      <c r="S6" t="str">
+        <v>ren "ALm4wwme7VXgc2Weboi_HjqXsTwOoYDzDtl-7QULWTGauR_1pIM6JfwLo_H9Nol9a1_HTM3fCPFOVh7wQkl6kxAMWk5pDpL1VqQRniHWZFNj63HTU3Tj9HkhzDhZ7T3Fgkd6gg5XzmXkh3mG7bsdpm5QbMBg435MdUuWHNb4VyosQvmalS8qKv-xQwT3AFTKS3g9floAJcw=w408-h726-k-no" "Vivero_Las_Palmas_De_Veracruz_4.jpg"</v>
+      </c>
+      <c r="T6" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+                    &lt;p&gt; ¿Estás buscando los mejores Parques Ecoturísticos en Tabasco? ¡Estás en el lugar correcto! Pues en este artículo vamos a presentarte cuáles son los  Parque Ecoturístico que han sido mejor evaluados en este estado. 
+ Para esto, realizamos consultas en un montón de fuentes oficiales, redes sociales, rankings e incluso entrevistas para poder determinar cuáles son los  Parque de Ecoturismo que mejor calificación han recibido en Tabasco durante los últimos años. 
  Con esta prueba social como respaldo, hoy te daremos los Parque Ecoturístico mejor calificados y te compartiremos su ubicación, medios oficiales de contacto, horarios y cómo llegar hasta ellos, junto con la calificación promedio con la que cuenta cada lugar. 
  Así que prepárate y ¡a disfrutar del ecoturismo en Tabasco!&lt;/p&gt;                    
                     </v>
       </c>
-      <c r="T6" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-                    &lt;p&gt; ¿Estás buscando los mejores Parques Ecoturísticos en Tabasco? ¡Estás en el lugar correcto! Pues en este artículo vamos a presentarte cuáles son los  Centro de Ecoturismo que han sido mejor evaluados en este estado. 
- Para esto, realizamos consultas en un montón de fuentes oficiales, redes sociales, rankings e incluso entrevistas para poder determinar cuáles son los  Parque Ecoturístico que mejor calificación han recibido en Tabasco durante los últimos años. 
+      <c r="U6" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+                    &lt;p&gt; ¿Estás buscando los mejores Parques Ecoturísticos en Tabasco? ¡Estás en el lugar correcto! Pues en este artículo vamos a presentarte cuáles son los  Parque Ecoturístico que han sido mejor evaluados en este estado. 
+ Para esto, realizamos consultas en un montón de fuentes oficiales, redes sociales, rankings e incluso entrevistas para poder determinar cuáles son los  Parque de Ecoturismo que mejor calificación han recibido en Tabasco durante los últimos años. 
  Con esta prueba social como respaldo, hoy te daremos los Parque Ecoturístico mejor calificados y te compartiremos su ubicación, medios oficiales de contacto, horarios y cómo llegar hasta ellos, junto con la calificación promedio con la que cuenta cada lugar. 
  Así que prepárate y ¡a disfrutar del ecoturismo en Tabasco!&lt;/p&gt;                    
                     </v>
       </c>
-      <c r="U6" t="str" xml:space="preserve">
+      <c r="V6" t="str" xml:space="preserve">
         <v xml:space="preserve">
                     &lt;h2&gt;&lt;b&gt;Parque Ecoturístico Vivero Las Palmas De Veracruz&lt;/b&gt;&lt;/h2&gt;
-                        &lt;p&gt;Este Parque Ecoturístico tiene 4.6 de calificación promedio, a partir de las más de 65 opiniones de sus visitantes... ¿nada mal no?. Es por eso que es parte de esta lista de los Parque Ecoturístico mejor calificados de Tabasco. Con este respaldo estamos más que seguras(os) que se trata  de un sitio que vas a disfrutar al Máximo. Así que ya sabes, si lo que buscas es naturaleza, el Parque Ecoturístico undefineden Tabasco, es sin duda una gran opción&lt;/p&gt;
-                        &lt;h3&gt;&lt;b&gt;¿Cómo llegar al Parque Ecoturístico Vivero Las Palmas De Veracruz? &lt;/b&gt;&lt;/h3&gt;
-                            &lt;p&gt;El Parque Ecoturístico se ubica enCalle Cto. Interior 208, Residencial Santa Teresa, 34166 Durango, Dgo.. Para ir a este lugar usar esa dirección en un gps o ayudarte con este &lt;a href='https://www.google.com.mx/maps/place/Vivero+Las+Palmas+De+Veracruz/data=!4m7!3m6!1s0x869bb7f86bc35165:0x2c2ed3acd58201b2!8m2!3d24.0040886!4d-104.6488795!16s%2Fg%2F11b6j9p3hk!19sChIJZVHDa_i3m4YRsgGC1azTLiw?authuser=0&amp;hl=es&amp;rclk=1'&gt;Mapa del Parque Ecoturístico Vivero Las Palmas De Veracruz&lt;/a&gt;&lt;/p&gt;
-                        &lt;h3&gt;&lt;b&gt;¿Cuáles son los contactos del Centro Ecoturístico Vivero Las Palmas De Veracruz?&lt;/b&gt;&lt;/h3&gt;
-                            &lt;p&gt;Los contactos disponibles del Parque Ecoturístico Vivero Las Palmas De Veracruz son: &lt;/p&gt;
+                        &lt;img src="https://rumbonaturaleza.com/wp-content/uploads/2023/03/Vivero_Las_Palmas_De_Veracruz_4.jpg" alt="Vivero Las Palmas De Veracruz"&gt;   
+                        &lt;div&gt;&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3644.7645914614886!2d-104.64887949999999!3d24.0040886!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x869bb7f86bc35165%3A0x2c2ed3acd58201b2!2sVivero%20Las%20Palmas%20De%20Veracruz!5e0!3m2!1ses!2smx!4v1678840889861!5m2!1ses!2smx" width="600" height="450" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;&lt;/div&gt;
+                        &lt;div&gt;&lt;/div&gt;
+                        &lt;p&gt;El Parque Ecoturístico undefined es una opción fantástica para tener una aventura natural en Tabasco. Su calificación promedio es de 4.6 respaldada por más de 65visitantes, así que no tenemos duda de que este lugar pertenece a la lista de los Parque Ecoturístico mejor rankeados de Tabasco y que se trata de uno de los principales atractivos naturales en la región. Así que ya sabes... ¿ganas de naturaleza?... pues el Parque Ecoturístico undefined es una grandísima opción.&lt;/p&gt;
+                        &lt;h3&gt;&lt;b&gt;¿Cómo llegar al Parque Ecológico Vivero Las Palmas De Veracruz? &lt;/b&gt;&lt;/h3&gt;
+                            &lt;p&gt;El Parque Ecoturístico se ubica enCalle Cto. Interior 208, Residencial Santa Teresa, 34166 Durango, Dgo.. Para ir a este centro manejando, puedes usar esta dirección oficial con tu google maps o usando este  &lt;a href='https://www.google.com.mx/maps/place/Vivero+Las+Palmas+De+Veracruz/@24.0040886,-104.6488795,17z/data=!3m1!4b1!4m6!3m5!1s0x869bb7f86bc35165:0x2c2ed3acd58201b2!8m2!3d24.0040886!4d-104.6488795!16s%2Fg%2F11b6j9p3hk?authuser=0&amp;hl=es'&gt;Mapa del Parque Ecoturístico Vivero Las Palmas De Veracruz&lt;/a&gt;&lt;/p&gt;
+                        &lt;h3&gt;&lt;b&gt;¿Cuáles son los contactos del Parque Ecoturístico Vivero Las Palmas De Veracruz?&lt;/b&gt;&lt;/h3&gt;
+                            &lt;p&gt;Los contactos disponibles del Parque de Ecoturismo Vivero Las Palmas De Veracruz son: &lt;/p&gt;
                             &lt;ul&gt;
                                 &lt;li&gt;&lt;b&gt;Teléfono:&lt;/b&gt;675 113 9208&lt;/li&gt;
                                 &lt;li&gt;&lt;b&gt;SitioWeb:&lt;/b&gt;web no disponible&lt;/li&gt;                                
                             &lt;/ul&gt;
-                        &lt;h3&gt;&lt;b&gt;¿En qué horarios y días se puede visitar el Parque Ecoturístico Vivero Las Palmas De Veracruz?&lt;/b&gt;&lt;/h3&gt;
-                            &lt;p&gt;Los horarios oficiales del Parque Ecoturístico Vivero Las Palmas De Veracruz son los siguientes:&lt;/p&gt;                       
-                            &lt;ul&gt;
-                                &lt;li&gt;Lunes de 09:00 a 20:00&lt;/li&gt;
+                        &lt;h3&gt;&lt;b&gt;¿En qué horarios y días se puede visitar el Parque Ecológico Vivero Las Palmas De Veracruz?&lt;/b&gt;&lt;/h3&gt;
+                            &lt;p&gt;Los horarios oficiales del Parque Natural Vivero Las Palmas De Veracruz son los siguientes:&lt;/p&gt;                       
+                            &lt;ul&gt;
+                                &lt;li&gt;Lunes (Natalicio de Benito Juárez (feriado)) de 09:00 a 20:00 El horario podría cambiar&lt;/li&gt;
                                 &lt;li&gt;Martes de 09:00 a 20:00&lt;/li&gt;
                                 &lt;li&gt;Miércoles de 09:00 a 20:00&lt;/li&gt;
                                 &lt;li&gt;Jueves de 09:00 a 20:00&lt;/li&gt;
@@ -979,21 +1012,568 @@
                                 &lt;li&gt;Sábado de 09:00 a 20:00&lt;/li&gt;
                                 &lt;li&gt;Domingo de 09:00 a 16:00&lt;/li&gt;
                             &lt;/ul&gt;
-                            &lt;p&gt;A pesar de contar con horarios oficiales, te recomendamos siempre visitar sus sitios de contacto y redes oficiales antes de ir al lugar, así podrás identificar cualquier cambio extraordinario que hayan tenido.&lt;/p&gt;                 
-                    </v>
-      </c>
-      <c r="V6" t="str" xml:space="preserve">
+                            &lt;p&gt;Aunque cuentes ya con los horarios oficiales de apertura de este lugar, siempre te recomendamos que antes de ir eches un ojito a sus redes sociales y vías de contacto, para asegurarte de que no hayan tenido algún cambio logístico de última hora&lt;/p&gt;                 
+                    </v>
+      </c>
+      <c r="W6" t="str" xml:space="preserve">
         <v xml:space="preserve">
                     &lt;img src="https://rumbonaturaleza.com/wp-content/uploads/2023/03/Vivero_Las_Palmas_De_Veracruz_4.jpg" alt="Vivero Las Palmas De Veracruz"&gt;                
                 </v>
       </c>
-      <c r="W6" t="str">
+      <c r="X6" t="str">
         <v>Añadir sitio web</v>
+      </c>
+    </row>
+    <row r="7" xml:space="preserve">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="str">
+        <v>Viveros Del Guadiana</v>
+      </c>
+      <c r="C7" t="str">
+        <v>Abasolo 609, Francisco González de la Vega, 34157 Durango, Dgo.</v>
+      </c>
+      <c r="D7" t="str">
+        <v>618 825 3855</v>
+      </c>
+      <c r="E7" t="str">
+        <v>http://macetasvivero.com.mx/directorio-viveros/durango/</v>
+      </c>
+      <c r="G7" t="str">
+        <v>Durango</v>
+      </c>
+      <c r="H7" t="str">
+        <v>https://www.google.com.mx/maps/place/Viveros+Del+Guadiana/@24.0106133,-104.6687241,17z/data=!3m1!4b1!4m6!3m5!1s0x869bc80512f9f577:0xa4030d2093a8b85e!8m2!3d24.0106133!4d-104.6687241!16s%2Fg%2F11b6jd0vv1?authuser=0&amp;hl=es</v>
+      </c>
+      <c r="I7" t="str">
+        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3644.5797372023844!2d-104.66872409999999!3d24.010613299999996!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x869bc80512f9f577%3A0xa4030d2093a8b85e!2sViveros%20Del%20Guadiana!5e0!3m2!1ses!2smx!4v1678840894132!5m2!1ses!2smx" width="600" height="450" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
+      </c>
+      <c r="J7" t="str">
+        <v>286J+6G Durango</v>
+      </c>
+      <c r="K7" t="str">
+        <v>5.0</v>
+      </c>
+      <c r="L7" t="str">
+        <v>4</v>
+      </c>
+      <c r="M7" t="str" xml:space="preserve">
+        <v xml:space="preserve">Bastante variedad de plantas, se adaptan en cada temporada del año, ahora para fiestas de navideñas cuentan con variedad de noche buenas, además que también ofrecen el servicio de diseño y mantenimiento para jardines.…,Me gustó este lugar, tiene variedad de plantas 🌱 ahí encontré dos gardenias hermosas que ya florecieron y huelen muy bonito. La atención es excelente. Volveré por más plantas 🌹🌸
+🌱🌱…,Gran variedad de plantas y excelente atención.</v>
+      </c>
+      <c r="N7" t="str">
+        <v>https://lh5.googleusercontent.com/p/AF1QipMrQ-GksQ-38r7UjiSPgRrkAk_jvI98IIqdsliq=w426-h240-k-no</v>
+      </c>
+      <c r="O7" t="str">
+        <v>wget --no-check-certificate https://lh5.googleusercontent.com/p/AF1QipMrQ-GksQ-38r7UjiSPgRrkAk_jvI98IIqdsliq=w426-h240-k-no</v>
+      </c>
+      <c r="P7" t="str">
+        <v>AF1QipMrQ-GksQ-38r7UjiSPgRrkAk_jvI98IIqdsliq=w426-h240-k-no</v>
+      </c>
+      <c r="Q7" t="str">
+        <v>Viveros_Del_Guadiana_5</v>
+      </c>
+      <c r="R7" t="str">
+        <v>https://rumbonaturaleza.com/wp-content/uploads/2023/03/Viveros_Del_Guadiana_5.jpg</v>
+      </c>
+      <c r="S7" t="str">
+        <v>ren "AF1QipMrQ-GksQ-38r7UjiSPgRrkAk_jvI98IIqdsliq=w426-h240-k-no" "Viveros_Del_Guadiana_5.jpg"</v>
+      </c>
+      <c r="T7" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+                    &lt;p&gt; ¿Estás buscando los mejores Parques Ecoturísticos en Tabasco? ¡Estás en el lugar correcto! Pues en este artículo vamos a presentarte cuáles son los  Parque Natural que han sido mejor evaluados en este estado. 
+ Para esto, realizamos consultas en un montón de fuentes oficiales, redes sociales, rankings e incluso entrevistas para poder determinar cuáles son los  Parque Ecoturístico que mejor calificación han recibido en Tabasco durante los últimos años. 
+ Con esta prueba social como respaldo, hoy te daremos los Parque Natural mejor calificados y te compartiremos su ubicación, medios oficiales de contacto, horarios y cómo llegar hasta ellos, junto con la calificación promedio con la que cuenta cada lugar. 
+ Así que prepárate y ¡a disfrutar del ecoturismo en Tabasco!&lt;/p&gt;                    
+                    </v>
+      </c>
+      <c r="U7" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+                    &lt;p&gt; ¿Estás buscando los mejores Parques Ecoturísticos en Tabasco? ¡Estás en el lugar correcto! Pues en este artículo vamos a presentarte cuáles son los  Parque Natural que han sido mejor evaluados en este estado. 
+ Para esto, realizamos consultas en un montón de fuentes oficiales, redes sociales, rankings e incluso entrevistas para poder determinar cuáles son los  Parque Ecoturístico que mejor calificación han recibido en Tabasco durante los últimos años. 
+ Con esta prueba social como respaldo, hoy te daremos los Parque Natural mejor calificados y te compartiremos su ubicación, medios oficiales de contacto, horarios y cómo llegar hasta ellos, junto con la calificación promedio con la que cuenta cada lugar. 
+ Así que prepárate y ¡a disfrutar del ecoturismo en Tabasco!&lt;/p&gt;                    
+                    </v>
+      </c>
+      <c r="V7" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+                    &lt;h2&gt;&lt;b&gt;Parque Ecoturístico Viveros Del Guadiana&lt;/b&gt;&lt;/h2&gt;
+                        &lt;img src="https://rumbonaturaleza.com/wp-content/uploads/2023/03/Viveros_Del_Guadiana_5.jpg" alt="Viveros Del Guadiana"&gt;   
+                        &lt;div&gt;&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3644.5797372023844!2d-104.66872409999999!3d24.010613299999996!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x869bc80512f9f577%3A0xa4030d2093a8b85e!2sViveros%20Del%20Guadiana!5e0!3m2!1ses!2smx!4v1678840894132!5m2!1ses!2smx" width="600" height="450" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;&lt;/div&gt;
+                        &lt;div&gt;&lt;/div&gt;
+                        &lt;p&gt;Este Parque Ecoturístico tiene 5.0 de calificación promedio, a partir de las más de 4 opiniones de sus visitantes... ¿nada mal no?. Es por eso que es parte de esta lista de los Parque Ecoturístico mejor calificados de Tabasco. Con este respaldo estamos más que seguras(os) que se trata  de un sitio que vas a disfrutar al Máximo. Así que ya sabes, si lo que buscas es naturaleza, el Parque Ecoturístico undefineden Tabasco, es sin duda una gran opción&lt;/p&gt;
+                        &lt;h3&gt;&lt;b&gt;¿Cómo llegar al Centro de Ecoturismo Viveros Del Guadiana? &lt;/b&gt;&lt;/h3&gt;
+                            &lt;p&gt;El Centro Ecoturístico se ubica enAbasolo 609, Francisco González de la Vega, 34157 Durango, Dgo.. Podrás llegar manejando sin ningún problema, símplemente usa la dirección en una app como waze o googleMaps, o usa este enlace al &lt;a href='https://www.google.com.mx/maps/place/Viveros+Del+Guadiana/@24.0106133,-104.6687241,17z/data=!3m1!4b1!4m6!3m5!1s0x869bc80512f9f577:0xa4030d2093a8b85e!8m2!3d24.0106133!4d-104.6687241!16s%2Fg%2F11b6jd0vv1?authuser=0&amp;hl=es'&gt;Mapa del Parque Ecoturístico Viveros Del Guadiana&lt;/a&gt;&lt;/p&gt;
+                        &lt;h3&gt;&lt;b&gt;¿Cuáles son los contactos del Parque Ecoturístico Viveros Del Guadiana?&lt;/b&gt;&lt;/h3&gt;
+                            &lt;p&gt;Los contactos disponibles del Sitio Ecoturístico Viveros Del Guadiana son: &lt;/p&gt;
+                            &lt;ul&gt;
+                                &lt;li&gt;&lt;b&gt;Teléfono:&lt;/b&gt;618 825 3855&lt;/li&gt;
+                                &lt;li&gt;&lt;b&gt;SitioWeb:&lt;/b&gt;&lt;a href="http://macetasvivero.com.mx/directorio-viveros/durango/"&gt;Web del place Viveros Del Guadiana&lt;/a&gt;&lt;/li&gt;                                
+                            &lt;/ul&gt;
+                        &lt;h3&gt;&lt;b&gt;¿En qué horarios y días se puede visitar el Parque Ecoturístico Viveros Del Guadiana?&lt;/b&gt;&lt;/h3&gt;
+                            &lt;p&gt;Los horarios oficiales del Centro de Ecoturismo Viveros Del Guadiana son los siguientes:&lt;/p&gt;                       
+                            &lt;ul&gt;
+                                &lt;li&gt;Lunes (Natalicio de Benito Juárez (feriado)) de 09:00 a 19:00 El horario podría cambiar&lt;/li&gt;
+                                &lt;li&gt;Martes de 09:00 a 19:00&lt;/li&gt;
+                                &lt;li&gt;Miércoles de 09:00 a 19:00&lt;/li&gt;
+                                &lt;li&gt;Jueves de 09:00 a 19:00&lt;/li&gt;
+                                &lt;li&gt;Viernes de 09:00 a 19:00&lt;/li&gt;
+                                &lt;li&gt;Sábado de 09:00 a 17:00&lt;/li&gt;
+                                &lt;li&gt;Domingo de 10:00 a 15:00&lt;/li&gt;
+                            &lt;/ul&gt;
+                            &lt;p&gt;Aunque estos horarios están oficialmente vigentes, siempre es bueno consultar sus sitios de contacto y redes oficiales antes de visitarlos, por cualquier cambio extraordinario que pudieran tener.&lt;/p&gt;                 
+                    </v>
+      </c>
+      <c r="W7" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+                    &lt;img src="https://rumbonaturaleza.com/wp-content/uploads/2023/03/Viveros_Del_Guadiana_5.jpg" alt="Viveros Del Guadiana"&gt;                
+                </v>
+      </c>
+      <c r="X7" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="8" xml:space="preserve">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="str">
+        <v>Vivero Santos</v>
+      </c>
+      <c r="C8" t="str">
+        <v>Blvd. Luis Donaldo Colosio M. 109, La Forestal, 34217 Durango, Dgo.</v>
+      </c>
+      <c r="D8" t="str">
+        <v>618 107 2833</v>
+      </c>
+      <c r="E8" t="str">
+        <v>Web no disponible</v>
+      </c>
+      <c r="G8" t="str">
+        <v>Durango</v>
+      </c>
+      <c r="H8" t="str">
+        <v>https://www.google.com.mx/maps/place/Vivero+Santos/@24.0385842,-104.657476,17z/data=!3m1!4b1!4m6!3m5!1s0x869bb7d6349387f9:0x5f5970606c2c7ea8!8m2!3d24.0385842!4d-104.657476!16s%2Fg%2F11b6hvymy7?authuser=0&amp;hl=es</v>
+      </c>
+      <c r="I8" t="str">
+        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3643.7867452724445!2d-104.65747599999999!3d24.0385842!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x869bb7d6349387f9%3A0x5f5970606c2c7ea8!2sVivero%20Santos!5e0!3m2!1ses!2smx!4v1678840897661!5m2!1ses!2smx" width="600" height="450" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
+      </c>
+      <c r="J8" t="str">
+        <v>28QV+C2 Durango</v>
+      </c>
+      <c r="K8" t="str">
+        <v>4.6</v>
+      </c>
+      <c r="L8" t="str">
+        <v>15</v>
+      </c>
+      <c r="M8" t="str">
+        <v>Mucho surtido excelente atención.  Bastante ayuda con la asesoría gratuita que me Proporcionaron.  en verdad te ayudan a hacer realidad tu proyecto de remodelación  de jardín.,Es un lugar muy lindo y el sr muy amable llama uno y le da informes,tienen muchas suculentas y cactus a buen precio</v>
+      </c>
+      <c r="N8" t="str">
+        <v>https://lh3.googleusercontent.com/gps-proxy/ALm4wwnmWGA_OMikXL9-T5PwzyqO2X2p_ZQytVRTBFNm7ZjGFRiUKH6xElhH4if7RzNzLQ6kbIUuIkAR-mWgQBNCz1a9TD_6qvwgEdA7FkS7iXpBe_eXXrFki1oOpICa1w_uRTztpTiqcueJ4KxG44WIfZ7x2iFv9PjrK3H2fcFMAQ7h7Tyf3UPHLGSD4075VXgLy8y7nyo=w427-h240-k-no</v>
+      </c>
+      <c r="O8" t="str">
+        <v>wget --no-check-certificate https://lh3.googleusercontent.com/gps-proxy/ALm4wwnmWGA_OMikXL9-T5PwzyqO2X2p_ZQytVRTBFNm7ZjGFRiUKH6xElhH4if7RzNzLQ6kbIUuIkAR-mWgQBNCz1a9TD_6qvwgEdA7FkS7iXpBe_eXXrFki1oOpICa1w_uRTztpTiqcueJ4KxG44WIfZ7x2iFv9PjrK3H2fcFMAQ7h7Tyf3UPHLGSD4075VXgLy8y7nyo=w427-h240-k-no</v>
+      </c>
+      <c r="P8" t="str">
+        <v>ALm4wwnmWGA_OMikXL9-T5PwzyqO2X2p_ZQytVRTBFNm7ZjGFRiUKH6xElhH4if7RzNzLQ6kbIUuIkAR-mWgQBNCz1a9TD_6qvwgEdA7FkS7iXpBe_eXXrFki1oOpICa1w_uRTztpTiqcueJ4KxG44WIfZ7x2iFv9PjrK3H2fcFMAQ7h7Tyf3UPHLGSD4075VXgLy8y7nyo=w427-h240-k-no</v>
+      </c>
+      <c r="Q8" t="str">
+        <v>Vivero_Santos_6</v>
+      </c>
+      <c r="R8" t="str">
+        <v>https://rumbonaturaleza.com/wp-content/uploads/2023/03/Vivero_Santos_6.jpg</v>
+      </c>
+      <c r="S8" t="str">
+        <v>ren "ALm4wwnmWGA_OMikXL9-T5PwzyqO2X2p_ZQytVRTBFNm7ZjGFRiUKH6xElhH4if7RzNzLQ6kbIUuIkAR-mWgQBNCz1a9TD_6qvwgEdA7FkS7iXpBe_eXXrFki1oOpICa1w_uRTztpTiqcueJ4KxG44WIfZ7x2iFv9PjrK3H2fcFMAQ7h7Tyf3UPHLGSD4075VXgLy8y7nyo=w427-h240-k-no" "Vivero_Santos_6.jpg"</v>
+      </c>
+      <c r="T8" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+                    &lt;p&gt; ¿Estás buscando los mejores Parques Ecoturísticos en Tabasco? ¡Estás en el lugar correcto! Pues en este artículo vamos a presentarte cuáles son los  Parque Ecológico que han sido mejor evaluados en este estado. 
+ Para esto, realizamos consultas en un montón de fuentes oficiales, redes sociales, rankings e incluso entrevistas para poder determinar cuáles son los  Parque de Ecoturismo que mejor calificación han recibido en Tabasco durante los últimos años. 
+ Con esta prueba social como respaldo, hoy te daremos los Parque de Ecoturismo mejor calificados y te compartiremos su ubicación, medios oficiales de contacto, horarios y cómo llegar hasta ellos, junto con la calificación promedio con la que cuenta cada lugar. 
+ Así que prepárate y ¡a disfrutar del ecoturismo en Tabasco!&lt;/p&gt;                    
+                    </v>
+      </c>
+      <c r="U8" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+                    &lt;p&gt; ¿Estás buscando los mejores Parques Ecoturísticos en Tabasco? ¡Estás en el lugar correcto! Pues en este artículo vamos a presentarte cuáles son los  Parque Ecológico que han sido mejor evaluados en este estado. 
+ Para esto, realizamos consultas en un montón de fuentes oficiales, redes sociales, rankings e incluso entrevistas para poder determinar cuáles son los  Parque de Ecoturismo que mejor calificación han recibido en Tabasco durante los últimos años. 
+ Con esta prueba social como respaldo, hoy te daremos los Parque de Ecoturismo mejor calificados y te compartiremos su ubicación, medios oficiales de contacto, horarios y cómo llegar hasta ellos, junto con la calificación promedio con la que cuenta cada lugar. 
+ Así que prepárate y ¡a disfrutar del ecoturismo en Tabasco!&lt;/p&gt;                    
+                    </v>
+      </c>
+      <c r="V8" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+                    &lt;h2&gt;&lt;b&gt;Parque Ecoturístico Vivero Santos&lt;/b&gt;&lt;/h2&gt;
+                        &lt;img src="https://rumbonaturaleza.com/wp-content/uploads/2023/03/Vivero_Santos_6.jpg" alt="Vivero Santos"&gt;   
+                        &lt;div&gt;&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3643.7867452724445!2d-104.65747599999999!3d24.0385842!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x869bb7d6349387f9%3A0x5f5970606c2c7ea8!2sVivero%20Santos!5e0!3m2!1ses!2smx!4v1678840897661!5m2!1ses!2smx" width="600" height="450" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;&lt;/div&gt;
+                        &lt;div&gt;&lt;/div&gt;
+                        &lt;p&gt;Este Parque Ecoturístico tiene 4.6 de calificación promedio, a partir de las más de 15 opiniones de sus visitantes... ¿nada mal no?. Es por eso que es parte de esta lista de los Parque Ecoturístico mejor calificados de Tabasco. Con este respaldo estamos más que seguras(os) que se trata  de un sitio que vas a disfrutar al Máximo. Así que ya sabes, si lo que buscas es naturaleza, el Parque Ecoturístico undefineden Tabasco, es sin duda una gran opción&lt;/p&gt;
+                        &lt;h3&gt;&lt;b&gt;¿Cómo llegar al Parque Natural Vivero Santos? &lt;/b&gt;&lt;/h3&gt;
+                            &lt;p&gt;El Parque Ecoturístico se ubica enBlvd. Luis Donaldo Colosio M. 109, La Forestal, 34217 Durango, Dgo.. Podrás llegar manejando sin ningún problema, símplemente usa la dirección en una app como waze o googleMaps, o usa este enlace al &lt;a href='https://www.google.com.mx/maps/place/Vivero+Santos/@24.0385842,-104.657476,17z/data=!3m1!4b1!4m6!3m5!1s0x869bb7d6349387f9:0x5f5970606c2c7ea8!8m2!3d24.0385842!4d-104.657476!16s%2Fg%2F11b6hvymy7?authuser=0&amp;hl=es'&gt;Mapa del Parque Ecoturístico Vivero Santos&lt;/a&gt;&lt;/p&gt;
+                        &lt;h3&gt;&lt;b&gt;¿Cuáles son los contactos del Centro de Ecoturismo Vivero Santos?&lt;/b&gt;&lt;/h3&gt;
+                            &lt;p&gt;Los contactos disponibles del Parque Ecoturístico Vivero Santos son: &lt;/p&gt;
+                            &lt;ul&gt;
+                                &lt;li&gt;&lt;b&gt;Teléfono:&lt;/b&gt;618 107 2833&lt;/li&gt;
+                                &lt;li&gt;&lt;b&gt;SitioWeb:&lt;/b&gt;web no disponible&lt;/li&gt;                                
+                            &lt;/ul&gt;
+                        &lt;h3&gt;&lt;b&gt;¿En qué horarios y días se puede visitar el Centro de Ecoturismo Vivero Santos?&lt;/b&gt;&lt;/h3&gt;
+                            &lt;p&gt;Los horarios oficiales del Centro de Ecoturismo Vivero Santos son los siguientes:&lt;/p&gt;                       
+                            &lt;ul&gt;
+                                &lt;li&gt;Lunes (Natalicio de Benito Juárez (feriado)) de 09:00 a 19:00 El horario podría cambiar&lt;/li&gt;
+                                &lt;li&gt;Martes de 09:00 a 19:00&lt;/li&gt;
+                                &lt;li&gt;Miércoles de 09:00 a 19:00&lt;/li&gt;
+                                &lt;li&gt;Jueves de 09:00 a 19:00&lt;/li&gt;
+                                &lt;li&gt;Viernes de 09:00 a 19:00&lt;/li&gt;
+                                &lt;li&gt;Sábado de 09:00 a 19:00&lt;/li&gt;
+                                &lt;li&gt;Domingo de 09:00 a 19:00&lt;/li&gt;
+                            &lt;/ul&gt;
+                            &lt;p&gt;Aunque cuentes ya con los horarios oficiales de apertura de este lugar, siempre te recomendamos que antes de ir eches un ojito a sus redes sociales y vías de contacto, para asegurarte de que no hayan tenido algún cambio logístico de última hora&lt;/p&gt;                 
+                    </v>
+      </c>
+      <c r="W8" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+                    &lt;img src="https://rumbonaturaleza.com/wp-content/uploads/2023/03/Vivero_Santos_6.jpg" alt="Vivero Santos"&gt;                
+                </v>
+      </c>
+      <c r="X8" t="str">
+        <v>Añadir sitio web</v>
+      </c>
+    </row>
+    <row r="9" xml:space="preserve">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="str">
+        <v>Vivero Las Nubes</v>
+      </c>
+      <c r="C9" t="str">
+        <v>Av Fidel Velázquez Sánchez, Nuevo Pedregal, Las Nubes, 34224 Durango, Dgo.</v>
+      </c>
+      <c r="D9" t="str">
+        <v>No cuenta con teléfono</v>
+      </c>
+      <c r="E9" t="str">
+        <v>Web no disponible</v>
+      </c>
+      <c r="G9" t="str">
+        <v>Durango</v>
+      </c>
+      <c r="H9" t="str">
+        <v>https://www.google.com.mx/maps/place/Vivero+Las+Nubes/@24.052367,-104.595552,17z/data=!3m1!4b1!4m6!3m5!1s0x869bb71dcf83f9bb:0x30182ba89df601ac!8m2!3d24.052367!4d-104.595552!16s%2Fg%2F11b6h_sf8h?authuser=0&amp;hl=es</v>
+      </c>
+      <c r="I9" t="str">
+        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3643.395675164008!2d-104.595552!3d24.052367!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x869bb71dcf83f9bb%3A0x30182ba89df601ac!2sVivero%20Las%20Nubes!5e0!3m2!1ses!2smx!4v1678840902756!5m2!1ses!2smx" width="600" height="450" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
+      </c>
+      <c r="J9" t="str">
+        <v>3C23+WQ Durango</v>
+      </c>
+      <c r="K9" t="str">
+        <v>4.4</v>
+      </c>
+      <c r="L9" t="str">
+        <v>117</v>
+      </c>
+      <c r="M9" t="str">
+        <v>Gran vivero con muchas opciones hermosas de plantas a un buen precio, trato muy amable. Abren los domingos y eso también es una gran ventaja ya que es cuando mucha gente tiene tiempo libre y busca opciones para decorar su hogar. ¡Recomendado!,Siempre tiene plantas muy bonitas. Más el viernes en la tarde, excelente trato y te dan tips,Tienen una excelente variedad de plantas y el señor que atendió sabe mucho de plantas.</v>
+      </c>
+      <c r="N9" t="str">
+        <v>https://lh3.googleusercontent.com/gps-proxy/ALm4wwnuNOHlzHUWJLF2TGvIIHTNpfyaszgaXNpUFrx-2ZpHPklEgneZyqU4Uw7u9r8taeR6iC3X2nvh89fjpPZvWtkMGT-xFZBD8euiWt1W4NJojLzgXeK1f2Ic_tOu4UF0z5H5h6C6C7ttcPhTGHOmLFGEZ4H0pvYl8fn_dOehOifL8g63P0B2qloOhxOTPih048hhkw=w408-h726-k-no</v>
+      </c>
+      <c r="O9" t="str">
+        <v>wget --no-check-certificate https://lh3.googleusercontent.com/gps-proxy/ALm4wwnuNOHlzHUWJLF2TGvIIHTNpfyaszgaXNpUFrx-2ZpHPklEgneZyqU4Uw7u9r8taeR6iC3X2nvh89fjpPZvWtkMGT-xFZBD8euiWt1W4NJojLzgXeK1f2Ic_tOu4UF0z5H5h6C6C7ttcPhTGHOmLFGEZ4H0pvYl8fn_dOehOifL8g63P0B2qloOhxOTPih048hhkw=w408-h726-k-no</v>
+      </c>
+      <c r="P9" t="str">
+        <v>ALm4wwnuNOHlzHUWJLF2TGvIIHTNpfyaszgaXNpUFrx-2ZpHPklEgneZyqU4Uw7u9r8taeR6iC3X2nvh89fjpPZvWtkMGT-xFZBD8euiWt1W4NJojLzgXeK1f2Ic_tOu4UF0z5H5h6C6C7ttcPhTGHOmLFGEZ4H0pvYl8fn_dOehOifL8g63P0B2qloOhxOTPih048hhkw=w408-h726-k-no</v>
+      </c>
+      <c r="Q9" t="str">
+        <v>Vivero_Las_Nubes_7</v>
+      </c>
+      <c r="R9" t="str">
+        <v>https://rumbonaturaleza.com/wp-content/uploads/2023/03/Vivero_Las_Nubes_7.jpg</v>
+      </c>
+      <c r="S9" t="str">
+        <v>ren "ALm4wwnuNOHlzHUWJLF2TGvIIHTNpfyaszgaXNpUFrx-2ZpHPklEgneZyqU4Uw7u9r8taeR6iC3X2nvh89fjpPZvWtkMGT-xFZBD8euiWt1W4NJojLzgXeK1f2Ic_tOu4UF0z5H5h6C6C7ttcPhTGHOmLFGEZ4H0pvYl8fn_dOehOifL8g63P0B2qloOhxOTPih048hhkw=w408-h726-k-no" "Vivero_Las_Nubes_7.jpg"</v>
+      </c>
+      <c r="T9" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+                    &lt;p&gt; ¿Estás buscando los mejores Parques Ecoturísticos en Tabasco? ¡Estás en el lugar correcto! Pues en este artículo vamos a presentarte cuáles son los  Parque de Ecoturismo que han sido mejor evaluados en este estado. 
+ Para esto, realizamos consultas en un montón de fuentes oficiales, redes sociales, rankings e incluso entrevistas para poder determinar cuáles son los  Parque Ecológico que mejor calificación han recibido en Tabasco durante los últimos años. 
+ Con esta prueba social como respaldo, hoy te daremos los Centro Ecoturístico mejor calificados y te compartiremos su ubicación, medios oficiales de contacto, horarios y cómo llegar hasta ellos, junto con la calificación promedio con la que cuenta cada lugar. 
+ Así que prepárate y ¡a disfrutar del ecoturismo en Tabasco!&lt;/p&gt;                    
+                    </v>
+      </c>
+      <c r="U9" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+                    &lt;p&gt; ¿Estás buscando los mejores Parques Ecoturísticos en Tabasco? ¡Estás en el lugar correcto! Pues en este artículo vamos a presentarte cuáles son los  Parque de Ecoturismo que han sido mejor evaluados en este estado. 
+ Para esto, realizamos consultas en un montón de fuentes oficiales, redes sociales, rankings e incluso entrevistas para poder determinar cuáles son los  Parque Ecológico que mejor calificación han recibido en Tabasco durante los últimos años. 
+ Con esta prueba social como respaldo, hoy te daremos los Centro Ecoturístico mejor calificados y te compartiremos su ubicación, medios oficiales de contacto, horarios y cómo llegar hasta ellos, junto con la calificación promedio con la que cuenta cada lugar. 
+ Así que prepárate y ¡a disfrutar del ecoturismo en Tabasco!&lt;/p&gt;                    
+                    </v>
+      </c>
+      <c r="V9" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+                    &lt;h2&gt;&lt;b&gt;Parque Ecoturístico Vivero Las Nubes&lt;/b&gt;&lt;/h2&gt;
+                        &lt;img src="https://rumbonaturaleza.com/wp-content/uploads/2023/03/Vivero_Las_Nubes_7.jpg" alt="Vivero Las Nubes"&gt;   
+                        &lt;div&gt;&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3643.395675164008!2d-104.595552!3d24.052367!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x869bb71dcf83f9bb%3A0x30182ba89df601ac!2sVivero%20Las%20Nubes!5e0!3m2!1ses!2smx!4v1678840902756!5m2!1ses!2smx" width="600" height="450" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;&lt;/div&gt;
+                        &lt;div&gt;&lt;/div&gt;
+                        &lt;p&gt;Bueno pues si eres de quienes ama estar en contacto con la naturaleza y andas por Tabasco, entonces no puedes perderte la experiencia de visitar el Parque Ecoturístico undefined. Con una calificación promedio de 4.4 estrellas de más de Gran vivero con muchas opciones hermosas de plantas a un buen precio, trato muy amable. Abren los domingos y eso también es una gran ventaja ya que es cuando mucha gente tiene tiempo libre y busca opciones para decorar su hogar. ¡Recomendado!,Siempre tiene plantas muy bonitas. Más el viernes en la tarde, excelente trato y te dan tips,Tienen una excelente variedad de plantas y el señor que atendió sabe mucho de plantas. visitantes, no tenemos duda de que se trata de un favorito de esta región. Así que nada...prepárate para sumergirte y disfrutar a tope de los paisajes naturales de Tabasco&lt;/p&gt;
+                        &lt;h3&gt;&lt;b&gt;¿Cómo llegar al Parque Ecoturístico Vivero Las Nubes? &lt;/b&gt;&lt;/h3&gt;
+                            &lt;p&gt;El Parque Ecoturístico se ubica enAv Fidel Velázquez Sánchez, Nuevo Pedregal, Las Nubes, 34224 Durango, Dgo.. Podrás llegar manejando sin ningún problema, símplemente usa la dirección en una app como waze o googleMaps, o usa este enlace al &lt;a href='https://www.google.com.mx/maps/place/Vivero+Las+Nubes/@24.052367,-104.595552,17z/data=!3m1!4b1!4m6!3m5!1s0x869bb71dcf83f9bb:0x30182ba89df601ac!8m2!3d24.052367!4d-104.595552!16s%2Fg%2F11b6h_sf8h?authuser=0&amp;hl=es'&gt;Mapa del Parque Ecoturístico Vivero Las Nubes&lt;/a&gt;&lt;/p&gt;
+                        &lt;h3&gt;&lt;b&gt;¿Cuáles son los contactos del Sitio Ecoturístico Vivero Las Nubes?&lt;/b&gt;&lt;/h3&gt;
+                            &lt;p&gt;Los contactos disponibles del Parque Ecoturístico Vivero Las Nubes son: &lt;/p&gt;
+                            &lt;ul&gt;
+                                &lt;li&gt;&lt;b&gt;Teléfono:&lt;/b&gt;No cuenta con teléfono&lt;/li&gt;
+                                &lt;li&gt;&lt;b&gt;SitioWeb:&lt;/b&gt;web no disponible&lt;/li&gt;                                
+                            &lt;/ul&gt;
+                        &lt;h3&gt;&lt;b&gt;¿En qué horarios y días se puede visitar el Parque Natural Vivero Las Nubes?&lt;/b&gt;&lt;/h3&gt;
+                            &lt;p&gt;Los horarios oficiales del Parque Ecológico Vivero Las Nubes son los siguientes:&lt;/p&gt;                       
+                            &lt;ul&gt;
+                                &lt;li&gt;Lunes (Natalicio de Benito Juárez (feriado)) de 09:00 a 19:00 El horario podría cambiar&lt;/li&gt;
+                                &lt;li&gt;Martes de 09:00 a 19:00&lt;/li&gt;
+                                &lt;li&gt;Miércoles de 09:00 a 19:00&lt;/li&gt;
+                                &lt;li&gt;Jueves de 09:00 a 19:00&lt;/li&gt;
+                                &lt;li&gt;Viernes de 09:00 a 19:00&lt;/li&gt;
+                                &lt;li&gt;Sábado de 09:00 a 19:00&lt;/li&gt;
+                                &lt;li&gt;Domingo de 09:30 a 16:00&lt;/li&gt;
+                            &lt;/ul&gt;
+                            &lt;p&gt;Siempre es importante -aún si cuentas con estos horarios oficiales-, revisar en sus redes sociales y medios de contacto antes de ir. Así podrás asegurarte de que no hayan tenido ningún cambio de horario o logístico de último momento.&lt;/p&gt;                 
+                    </v>
+      </c>
+      <c r="W9" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+                    &lt;img src="https://rumbonaturaleza.com/wp-content/uploads/2023/03/Vivero_Las_Nubes_7.jpg" alt="Vivero Las Nubes"&gt;                
+                </v>
+      </c>
+      <c r="X9" t="str">
+        <v>Añadir número de teléfono del sitio,Añadir sitio web</v>
+      </c>
+    </row>
+    <row r="10" xml:space="preserve">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="str">
+        <v>Vivero El Milagro Suc Los Angeles</v>
+      </c>
+      <c r="C10" t="str">
+        <v>C. Aquiles Serdan 1306, Los Ángeles, 34076 Durango, Dgo.</v>
+      </c>
+      <c r="D10" t="str">
+        <v>618 189 0754</v>
+      </c>
+      <c r="E10" t="str">
+        <v>Web no disponible</v>
+      </c>
+      <c r="G10" t="str">
+        <v>Durango</v>
+      </c>
+      <c r="H10" t="str">
+        <v>https://www.google.com.mx/maps/place/Vivero+El+Milagro+Suc+Los+Angeles/@24.0267101,-104.6794677,17z/data=!3m1!4b1!4m6!3m5!1s0x869bc83f03010ed1:0x1db0e10487ed912!8m2!3d24.0267101!4d-104.6794677!16s%2Fg%2F11b6j6cy2v?authuser=0&amp;hl=es</v>
+      </c>
+      <c r="I10" t="str">
+        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3644.123489275272!2d-104.67946769999999!3d24.0267101!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x869bc83f03010ed1%3A0x1db0e10487ed912!2sVivero%20El%20Milagro%20Suc%20Los%20Angeles!5e0!3m2!1ses!2smx!4v1678840906363!5m2!1ses!2smx" width="600" height="450" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
+      </c>
+      <c r="J10" t="str">
+        <v>28GC+M6 Durango</v>
+      </c>
+      <c r="K10" t="str">
+        <v>4.2</v>
+      </c>
+      <c r="L10" t="str">
+        <v>11</v>
+      </c>
+      <c r="M10" t="str" xml:space="preserve">
+        <v xml:space="preserve">Muy bonito lugar, precios moderados,  buenas bebidas y snacks,La comida estuvo buena.
+El servicio a cliente es pésimo, las chicas son muy groseras e incómodan con su actitud. Problemas al tomar la orden.,Hay muy poca variedad de maceta floral</v>
+      </c>
+      <c r="N10" t="str">
+        <v>https://lh3.googleusercontent.com/gps-proxy/ALm4wwlhoCICLNrCakBRbJ52KABdnQK1nKhuotM0pNYzS7emK1HStPexrEFEtHyXqM6bDlhgivruwFg1uQ8Pk1V_bURU_NkNU6vxwFrbCv4WLzlRK-9Tlk0yFhLDC4ke5PGQLnW_qgErq8ChHcchLH_anc1cZAaajn6B3GYglaBwPSZBXxs78jDzmdog2ufU5WoSUSdY3A=w427-h240-k-no</v>
+      </c>
+      <c r="O10" t="str">
+        <v>wget --no-check-certificate https://lh3.googleusercontent.com/gps-proxy/ALm4wwlhoCICLNrCakBRbJ52KABdnQK1nKhuotM0pNYzS7emK1HStPexrEFEtHyXqM6bDlhgivruwFg1uQ8Pk1V_bURU_NkNU6vxwFrbCv4WLzlRK-9Tlk0yFhLDC4ke5PGQLnW_qgErq8ChHcchLH_anc1cZAaajn6B3GYglaBwPSZBXxs78jDzmdog2ufU5WoSUSdY3A=w427-h240-k-no</v>
+      </c>
+      <c r="P10" t="str">
+        <v>ALm4wwlhoCICLNrCakBRbJ52KABdnQK1nKhuotM0pNYzS7emK1HStPexrEFEtHyXqM6bDlhgivruwFg1uQ8Pk1V_bURU_NkNU6vxwFrbCv4WLzlRK-9Tlk0yFhLDC4ke5PGQLnW_qgErq8ChHcchLH_anc1cZAaajn6B3GYglaBwPSZBXxs78jDzmdog2ufU5WoSUSdY3A=w427-h240-k-no</v>
+      </c>
+      <c r="Q10" t="str">
+        <v>Vivero_El_Milagro_Suc_Los_Angeles_8</v>
+      </c>
+      <c r="R10" t="str">
+        <v>https://rumbonaturaleza.com/wp-content/uploads/2023/03/Vivero_El_Milagro_Suc_Los_Angeles_8.jpg</v>
+      </c>
+      <c r="S10" t="str">
+        <v>ren "ALm4wwlhoCICLNrCakBRbJ52KABdnQK1nKhuotM0pNYzS7emK1HStPexrEFEtHyXqM6bDlhgivruwFg1uQ8Pk1V_bURU_NkNU6vxwFrbCv4WLzlRK-9Tlk0yFhLDC4ke5PGQLnW_qgErq8ChHcchLH_anc1cZAaajn6B3GYglaBwPSZBXxs78jDzmdog2ufU5WoSUSdY3A=w427-h240-k-no" "Vivero_El_Milagro_Suc_Los_Angeles_8.jpg"</v>
+      </c>
+      <c r="T10" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+                    &lt;p&gt; ¿Estás buscando los mejores Parques Ecoturísticos en Tabasco? ¡Estás en el lugar correcto! Pues en este artículo vamos a presentarte cuáles son los  Parque Ecoturístico que han sido mejor evaluados en este estado. 
+ Para esto, realizamos consultas en un montón de fuentes oficiales, redes sociales, rankings e incluso entrevistas para poder determinar cuáles son los  Parque Ecoturístico que mejor calificación han recibido en Tabasco durante los últimos años. 
+ Con esta prueba social como respaldo, hoy te daremos los Parque Ecoturístico mejor calificados y te compartiremos su ubicación, medios oficiales de contacto, horarios y cómo llegar hasta ellos, junto con la calificación promedio con la que cuenta cada lugar. 
+ Así que prepárate y ¡a disfrutar del ecoturismo en Tabasco!&lt;/p&gt;                    
+                    </v>
+      </c>
+      <c r="U10" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+                    &lt;p&gt; ¿Estás buscando los mejores Parques Ecoturísticos en Tabasco? ¡Estás en el lugar correcto! Pues en este artículo vamos a presentarte cuáles son los  Parque Ecoturístico que han sido mejor evaluados en este estado. 
+ Para esto, realizamos consultas en un montón de fuentes oficiales, redes sociales, rankings e incluso entrevistas para poder determinar cuáles son los  Parque Ecoturístico que mejor calificación han recibido en Tabasco durante los últimos años. 
+ Con esta prueba social como respaldo, hoy te daremos los Parque Ecoturístico mejor calificados y te compartiremos su ubicación, medios oficiales de contacto, horarios y cómo llegar hasta ellos, junto con la calificación promedio con la que cuenta cada lugar. 
+ Así que prepárate y ¡a disfrutar del ecoturismo en Tabasco!&lt;/p&gt;                    
+                    </v>
+      </c>
+      <c r="V10" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+                    &lt;h2&gt;&lt;b&gt;Parque Ecoturístico Vivero El Milagro Suc Los Angeles&lt;/b&gt;&lt;/h2&gt;
+                        &lt;img src="https://rumbonaturaleza.com/wp-content/uploads/2023/03/Vivero_El_Milagro_Suc_Los_Angeles_8.jpg" alt="Vivero El Milagro Suc Los Angeles"&gt;   
+                        &lt;div&gt;&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3644.123489275272!2d-104.67946769999999!3d24.0267101!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x869bc83f03010ed1%3A0x1db0e10487ed912!2sVivero%20El%20Milagro%20Suc%20Los%20Angeles!5e0!3m2!1ses!2smx!4v1678840906363!5m2!1ses!2smx" width="600" height="450" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;&lt;/div&gt;
+                        &lt;div&gt;&lt;/div&gt;
+                        &lt;p&gt;Este Parque Ecoturístico tiene 4.2 de calificación promedio, a partir de las más de 11 opiniones de sus visitantes... ¿nada mal no?. Es por eso que es parte de esta lista de los Parque Ecoturístico mejor calificados de Tabasco. Con este respaldo estamos más que seguras(os) que se trata  de un sitio que vas a disfrutar al Máximo. Así que ya sabes, si lo que buscas es naturaleza, el Parque Ecoturístico undefineden Tabasco, es sin duda una gran opción&lt;/p&gt;
+                        &lt;h3&gt;&lt;b&gt;¿Cómo llegar al Parque Ecoturístico Vivero El Milagro Suc Los Angeles? &lt;/b&gt;&lt;/h3&gt;
+                            &lt;p&gt;El Sitio Ecoturístico se ubica enC. Aquiles Serdan 1306, Los Ángeles, 34076 Durango, Dgo.. Para llegar, puedes símplemente colocar esta dirección en el googleMaps o Waze o apoyarte en este &lt;a href='https://www.google.com.mx/maps/place/Vivero+El+Milagro+Suc+Los+Angeles/@24.0267101,-104.6794677,17z/data=!3m1!4b1!4m6!3m5!1s0x869bc83f03010ed1:0x1db0e10487ed912!8m2!3d24.0267101!4d-104.6794677!16s%2Fg%2F11b6j6cy2v?authuser=0&amp;hl=es'&gt;Mapa del Parque Ecoturístico Vivero El Milagro Suc Los Angeles&lt;/a&gt;&lt;/p&gt;
+                        &lt;h3&gt;&lt;b&gt;¿Cuáles son los contactos del Parque de Ecoturismo Vivero El Milagro Suc Los Angeles?&lt;/b&gt;&lt;/h3&gt;
+                            &lt;p&gt;Los contactos disponibles del Centro Ecoturístico Vivero El Milagro Suc Los Angeles son: &lt;/p&gt;
+                            &lt;ul&gt;
+                                &lt;li&gt;&lt;b&gt;Teléfono:&lt;/b&gt;618 189 0754&lt;/li&gt;
+                                &lt;li&gt;&lt;b&gt;SitioWeb:&lt;/b&gt;web no disponible&lt;/li&gt;                                
+                            &lt;/ul&gt;
+                        &lt;h3&gt;&lt;b&gt;¿En qué horarios y días se puede visitar el Parque de Ecoturismo Vivero El Milagro Suc Los Angeles?&lt;/b&gt;&lt;/h3&gt;
+                            &lt;p&gt;Los horarios oficiales del Parque de Ecoturismo Vivero El Milagro Suc Los Angeles son los siguientes:&lt;/p&gt;                       
+                            &lt;ul&gt;
+                                &lt;li&gt;Lunes (Natalicio de Benito Juárez (feriado)) de 08:00 a 19:00 El horario podría cambiar&lt;/li&gt;
+                                &lt;li&gt;Martes de 08:00 a 19:00&lt;/li&gt;
+                                &lt;li&gt;Miércoles de 08:00 a 19:00&lt;/li&gt;
+                                &lt;li&gt;Jueves de 08:00 a 19:00&lt;/li&gt;
+                                &lt;li&gt;Viernes de 08:00 a 19:00&lt;/li&gt;
+                                &lt;li&gt;Sábado de 08:00 a 23:00&lt;/li&gt;
+                                &lt;li&gt;Domingo de 08:00 a 23:00&lt;/li&gt;
+                            &lt;/ul&gt;
+                            &lt;p&gt;Aunque estos horarios sean oficialmente vigentes, nunca está de más que antes de lanzarte, revises en sus redes sociales o contactos digitales que no haya habido ningún cambio logístico extraordinario en sus horarios de apertura y cierre.&lt;/p&gt;                 
+                    </v>
+      </c>
+      <c r="W10" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+                    &lt;img src="https://rumbonaturaleza.com/wp-content/uploads/2023/03/Vivero_El_Milagro_Suc_Los_Angeles_8.jpg" alt="Vivero El Milagro Suc Los Angeles"&gt;                
+                </v>
+      </c>
+      <c r="X10" t="str">
+        <v>Añadir sitio web</v>
+      </c>
+    </row>
+    <row r="11" xml:space="preserve">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="str">
+        <v>Vivero Victoria</v>
+      </c>
+      <c r="C11" t="str">
+        <v>Av. del Factor 906, Casa Redonda, 35158 Durango, Dgo.</v>
+      </c>
+      <c r="D11" t="str">
+        <v>No cuenta con teléfono</v>
+      </c>
+      <c r="E11" t="str">
+        <v>Web no disponible</v>
+      </c>
+      <c r="G11" t="str">
+        <v>Durango</v>
+      </c>
+      <c r="H11" t="str">
+        <v>https://www.google.com.mx/maps/place/Vivero+Victoria/@24.0391699,-104.6661015,17z/data=!3m1!4b1!4m6!3m5!1s0x869bc82f1e35ef4b:0x28ac0bb71cd10463!8m2!3d24.0391699!4d-104.6661015!16s%2Fg%2F11b6j5hybg?authuser=0&amp;hl=es</v>
+      </c>
+      <c r="I11" t="str">
+        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3643.7701310402113!2d-104.6661015!3d24.039169899999997!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x869bc82f1e35ef4b%3A0x28ac0bb71cd10463!2sVivero%20Victoria!5e0!3m2!1ses!2smx!4v1678840910783!5m2!1ses!2smx" width="600" height="450" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
+      </c>
+      <c r="J11" t="str">
+        <v>28QM+MH Durango</v>
+      </c>
+      <c r="K11" t="str">
+        <v>4.3</v>
+      </c>
+      <c r="L11" t="str">
+        <v>7</v>
+      </c>
+      <c r="M11" t="str">
+        <v>Cuando fui no sabían que veriedad eran los árboles, aún que tenían de muchos tipos, los dan muy económicos.,Mucha variedad de plantas,Buen servicio</v>
+      </c>
+      <c r="N11" t="str">
+        <v>https://lh3.googleusercontent.com/gps-proxy/ALm4wwlIxtyo1B_aI5fW_-j28M2U6kwbnPZmpcWWw1fESbw5AxS813poPcupGTN3aCJGpI1FEzmkNN1zZUPofuwIYeXBS8Pct4vuUMtAunxUZB4gYW-TY8Edz-p2nSQKebAAQGxduiv5-8nN0tn2vcLotAzsnMxvj-N1bexMbh6y5GF1OwlgXDmbMg80lrwkH1-l1kOFnbs=w427-h240-k-no</v>
+      </c>
+      <c r="O11" t="str">
+        <v>wget --no-check-certificate https://lh3.googleusercontent.com/gps-proxy/ALm4wwlIxtyo1B_aI5fW_-j28M2U6kwbnPZmpcWWw1fESbw5AxS813poPcupGTN3aCJGpI1FEzmkNN1zZUPofuwIYeXBS8Pct4vuUMtAunxUZB4gYW-TY8Edz-p2nSQKebAAQGxduiv5-8nN0tn2vcLotAzsnMxvj-N1bexMbh6y5GF1OwlgXDmbMg80lrwkH1-l1kOFnbs=w427-h240-k-no</v>
+      </c>
+      <c r="P11" t="str">
+        <v>ALm4wwlIxtyo1B_aI5fW_-j28M2U6kwbnPZmpcWWw1fESbw5AxS813poPcupGTN3aCJGpI1FEzmkNN1zZUPofuwIYeXBS8Pct4vuUMtAunxUZB4gYW-TY8Edz-p2nSQKebAAQGxduiv5-8nN0tn2vcLotAzsnMxvj-N1bexMbh6y5GF1OwlgXDmbMg80lrwkH1-l1kOFnbs=w427-h240-k-no</v>
+      </c>
+      <c r="Q11" t="str">
+        <v>Vivero_Victoria_9</v>
+      </c>
+      <c r="R11" t="str">
+        <v>https://rumbonaturaleza.com/wp-content/uploads/2023/03/Vivero_Victoria_9.jpg</v>
+      </c>
+      <c r="S11" t="str">
+        <v>ren "ALm4wwlIxtyo1B_aI5fW_-j28M2U6kwbnPZmpcWWw1fESbw5AxS813poPcupGTN3aCJGpI1FEzmkNN1zZUPofuwIYeXBS8Pct4vuUMtAunxUZB4gYW-TY8Edz-p2nSQKebAAQGxduiv5-8nN0tn2vcLotAzsnMxvj-N1bexMbh6y5GF1OwlgXDmbMg80lrwkH1-l1kOFnbs=w427-h240-k-no" "Vivero_Victoria_9.jpg"</v>
+      </c>
+      <c r="T11" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+                    &lt;p&gt; ¿Estás buscando los mejores Parques Ecoturísticos en Tabasco? ¡Estás en el lugar correcto! Pues en este artículo vamos a presentarte cuáles son los  Parque Ecológico que han sido mejor evaluados en este estado. 
+ Para esto, realizamos consultas en un montón de fuentes oficiales, redes sociales, rankings e incluso entrevistas para poder determinar cuáles son los  Parque de Ecoturismo que mejor calificación han recibido en Tabasco durante los últimos años. 
+ Con esta prueba social como respaldo, hoy te daremos los Parque de Ecoturismo mejor calificados y te compartiremos su ubicación, medios oficiales de contacto, horarios y cómo llegar hasta ellos, junto con la calificación promedio con la que cuenta cada lugar. 
+ Así que prepárate y ¡a disfrutar del ecoturismo en Tabasco!&lt;/p&gt;                    
+                    </v>
+      </c>
+      <c r="U11" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+                    &lt;p&gt; ¿Estás buscando los mejores Parques Ecoturísticos en Tabasco? ¡Estás en el lugar correcto! Pues en este artículo vamos a presentarte cuáles son los  Parque Ecológico que han sido mejor evaluados en este estado. 
+ Para esto, realizamos consultas en un montón de fuentes oficiales, redes sociales, rankings e incluso entrevistas para poder determinar cuáles son los  Parque de Ecoturismo que mejor calificación han recibido en Tabasco durante los últimos años. 
+ Con esta prueba social como respaldo, hoy te daremos los Parque de Ecoturismo mejor calificados y te compartiremos su ubicación, medios oficiales de contacto, horarios y cómo llegar hasta ellos, junto con la calificación promedio con la que cuenta cada lugar. 
+ Así que prepárate y ¡a disfrutar del ecoturismo en Tabasco!&lt;/p&gt;                    
+                    </v>
+      </c>
+      <c r="V11" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+                    &lt;h2&gt;&lt;b&gt;Parque Ecoturístico Vivero Victoria&lt;/b&gt;&lt;/h2&gt;
+                        &lt;img src="https://rumbonaturaleza.com/wp-content/uploads/2023/03/Vivero_Victoria_9.jpg" alt="Vivero Victoria"&gt;   
+                        &lt;div&gt;&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3643.7701310402113!2d-104.6661015!3d24.039169899999997!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x869bc82f1e35ef4b%3A0x28ac0bb71cd10463!2sVivero%20Victoria!5e0!3m2!1ses!2smx!4v1678840910783!5m2!1ses!2smx" width="600" height="450" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;&lt;/div&gt;
+                        &lt;div&gt;&lt;/div&gt;
+                        &lt;p&gt;El Parque Ecoturístico undefined es una opción fantástica para tener una aventura natural en Tabasco. Su calificación promedio es de 4.3 respaldada por más de 7visitantes, así que no tenemos duda de que este lugar pertenece a la lista de los Parque Ecoturístico mejor rankeados de Tabasco y que se trata de uno de los principales atractivos naturales en la región. Así que ya sabes... ¿ganas de naturaleza?... pues el Parque Ecoturístico undefined es una grandísima opción.&lt;/p&gt;
+                        &lt;h3&gt;&lt;b&gt;¿Cómo llegar al Centro Ecoturístico Vivero Victoria? &lt;/b&gt;&lt;/h3&gt;
+                            &lt;p&gt;El Parque Ecoturístico se ubica enAv. del Factor 906, Casa Redonda, 35158 Durango, Dgo.. Puedes ir a este lugar sin problemas manejando, sólo coloca su dirección oficial en waze, google maps o equivalente, o guíate con este &lt;a href='https://www.google.com.mx/maps/place/Vivero+Victoria/@24.0391699,-104.6661015,17z/data=!3m1!4b1!4m6!3m5!1s0x869bc82f1e35ef4b:0x28ac0bb71cd10463!8m2!3d24.0391699!4d-104.6661015!16s%2Fg%2F11b6j5hybg?authuser=0&amp;hl=es'&gt;Mapa del Parque Ecoturístico Vivero Victoria&lt;/a&gt;&lt;/p&gt;
+                        &lt;h3&gt;&lt;b&gt;¿Cuáles son los contactos del Parque Natural Vivero Victoria?&lt;/b&gt;&lt;/h3&gt;
+                            &lt;p&gt;Los contactos disponibles del Sitio Ecoturístico Vivero Victoria son: &lt;/p&gt;
+                            &lt;ul&gt;
+                                &lt;li&gt;&lt;b&gt;Teléfono:&lt;/b&gt;No cuenta con teléfono&lt;/li&gt;
+                                &lt;li&gt;&lt;b&gt;SitioWeb:&lt;/b&gt;web no disponible&lt;/li&gt;                                
+                            &lt;/ul&gt;
+                        &lt;h3&gt;&lt;b&gt;¿En qué horarios y días se puede visitar el Parque Ecoturístico Vivero Victoria?&lt;/b&gt;&lt;/h3&gt;
+                            &lt;p&gt;Los horarios oficiales del Centro Ecoturístico Vivero Victoria son los siguientes:&lt;/p&gt;                       
+                            &lt;ul&gt;
+                                &lt;li&gt;Lunes (Natalicio de Benito Juárez (feriado)) de 09:00 a 19:00 El horario podría cambiar&lt;/li&gt;
+                                &lt;li&gt;Martes de 09:00 a 19:00&lt;/li&gt;
+                                &lt;li&gt;Miércoles de 09:00 a 19:00&lt;/li&gt;
+                                &lt;li&gt;Jueves de 09:00 a 19:00&lt;/li&gt;
+                                &lt;li&gt;Viernes de 09:00 a 19:00&lt;/li&gt;
+                                &lt;li&gt;Sábado de 09:00 a 19:00&lt;/li&gt;
+                                &lt;li&gt;Domingo de 09:00 a 19:00&lt;/li&gt;
+                            &lt;/ul&gt;
+                            &lt;p&gt;Aunque cuentes ya con los horarios oficiales de apertura de este lugar, siempre te recomendamos que antes de ir eches un ojito a sus redes sociales y vías de contacto, para asegurarte de que no hayan tenido algún cambio logístico de última hora&lt;/p&gt;                 
+                    </v>
+      </c>
+      <c r="W11" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+                    &lt;img src="https://rumbonaturaleza.com/wp-content/uploads/2023/03/Vivero_Victoria_9.jpg" alt="Vivero Victoria"&gt;                
+                </v>
+      </c>
+      <c r="X11" t="str">
+        <v>Añadir número de teléfono del sitio,Añadir sitio web</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:W6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:X11"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
WIP_Horario Bug detectado_version Pre intentos de corrección
</commit_message>
<xml_diff>
--- a/testingAllImports.xlsx
+++ b/testingAllImports.xlsx
@@ -520,7 +520,7 @@
         <v>https://www.google.com/maps/place/Centro+Ecoturistico+El+Nuevo+Mundo+-+Estoracon/@16.8505798,-93.7933739,17z/data=!3m1!4b1!4m6!3m5!1s0x85eca6200d7617bb:0x7498371825377da6!8m2!3d16.8505798!4d-93.7933739!16s%2Fg%2F11dxpchfty?authuser=0&amp;hl=es</v>
       </c>
       <c r="L2" t="str">
-        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3818.5113687598837!2d-93.79337389999999!3d16.8505798!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x85eca6200d7617bb%3A0x7498371825377da6!2sCentro%20Ecoturistico%20El%20Nuevo%20Mundo%20-%20Estoracon!5e0!3m2!1ses!2smx!4v1679086801983!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
+        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3818.5113687598837!2d-93.79337389999999!3d16.8505798!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x85eca6200d7617bb%3A0x7498371825377da6!2sCentro%20Ecoturistico%20El%20Nuevo%20Mundo%20-%20Estoracon!5e0!3m2!1ses!2smx!4v1679155875054!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
       </c>
       <c r="M2" t="str">
         <v>V624+6M Estoracón, Chiapas</v>
@@ -560,29 +560,30 @@
       </c>
       <c r="Y2" t="str" xml:space="preserve">
         <v xml:space="preserve">
-                    &lt;p&gt; ¿Estás buscando los mejores parques ecoturísticos en undefined? Entonces sin duda ¡estás en el lugar correcto!. Hoy en este artículo vamos a presentarte cuáles son los  parque ecoturístico que han sido mejor evaluados en este estado. 
- Para poder definir esta listade los mejores, realizamos consultas en un montón de fuentes oficiales, redes sociales, rankings e incluso algunas entrevistas que nos permitieron determinar cuáles son y dónde se ubican los parque natural que mejores experiencias han brindado a sus visitantes, y que mayor calificación han recibido en undefined durante los últimos años. 
- Con esta prueba social como respaldo, hoy te compartimos la lista de los parque ecológico mejor calificados en undefined en function getFullYear() { [native code] } junto con su ubicación, medios oficiales de contacto, horarios y cómo llegar hasta ellos; así como la calificación promedio con la que cuenta cada lugar. 
- Prepárate con esto y ¡a disfrutar del ecoturismo en undefined!&lt;/p&gt;                    
+                    &lt;p&gt; ¿Estás buscando los mejores parques ecoturísticos en Chiapas? Entonces sin duda ¡estás en el lugar correcto!. Hoy en este artículo vamos a presentarte cuáles son los  parques ecoturísticos que han sido mejor evaluados en este estado. 
+ Para poder definir esta listade los mejores, realizamos consultas en un montón de fuentes oficiales, redes sociales, rankings e incluso algunas entrevistas que nos permitieron determinar cuáles son y dónde se ubican los parques de ecoturismo que mejores experiencias han brindado a sus visitantes, y que mayor calificación han recibido en Chiapas durante los últimos años. 
+ Con esta prueba social como respaldo, hoy te compartimos la lista de los parque ecológico mejor calificados en Chiapas en function getFullYear() { [native code] } junto con su ubicación, medios oficiales de contacto, horarios y cómo llegar hasta ellos; así como la calificación promedio con la que cuenta cada lugar. 
+ Prepárate con esto y ¡a disfrutar del ecoturismo en Chiapas!&lt;/p&gt;                    
                     </v>
       </c>
       <c r="Z2" t="str" xml:space="preserve">
         <v xml:space="preserve">
-                    &lt;h2&gt;&lt;b&gt;Centro Ecoturístico Centro Ecoturistico El Nuevo Mundo - Estoracon&lt;/b&gt;&lt;/h2&gt;
+                    &lt;h2&gt;&lt;b&gt;Sitio Ecoturístico Centro Ecoturistico El Nuevo Mundo - Estoracon&lt;/b&gt;&lt;/h2&gt;
                         &lt;img src="https://rumbonaturaleza.com/wp-content/uploads/2023/03/Centro_Ecoturistico_El_Nuevo_Mundo_-_Estoracon_0.jpg" alt="Centro Ecoturistico El Nuevo Mundo - Estoracon"&gt;   
-                        &lt;div&gt;&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3818.5113687598837!2d-93.79337389999999!3d16.8505798!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x85eca6200d7617bb%3A0x7498371825377da6!2sCentro%20Ecoturistico%20El%20Nuevo%20Mundo%20-%20Estoracon!5e0!3m2!1ses!2smx!4v1679086801983!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;&lt;/div&gt;
+                        &lt;div&gt;&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3818.5113687598837!2d-93.79337389999999!3d16.8505798!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x85eca6200d7617bb%3A0x7498371825377da6!2sCentro%20Ecoturistico%20El%20Nuevo%20Mundo%20-%20Estoracon!5e0!3m2!1ses!2smx!4v1679155875054!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;&lt;/div&gt;
                         &lt;div&gt;&lt;/div&gt;
-                        &lt;p&gt;Si andas en búsca de experiencias únicas en la naturaleza, entonces el parque natural undefined en undefined tiene que ser parte de tu lista. Este es un parque ecoturístico con más de undefined opiniones de visitantes y que ha sido de manera consistente calificado con hasta undefined estrellas, es por eso que aunque pueda tener algunas áreas de mejora, es sin duda uno de los mejores lugares para disfrutar de la naturaleza en la región. Así que no lo pienses mucho más y ¡a visitar undefined!&lt;/p&gt;
-                        &lt;h3&gt;&lt;b&gt;¿Cómo llegar al Parque Ecológico "Centro Ecoturistico El Nuevo Mundo - Estoracon"? &lt;/b&gt;&lt;/h3&gt;
-                            &lt;p&gt;El parque de ecoturismo se ubica enCarretera Sayula S/N, Francisco I. Madero, 30400 Cintalapa, Chis.. Si necesitas llegar a este destino, basta con que ingreses la dirección en una app de navegación o sigas este&lt;a href='https://www.google.com/maps/place/Centro+Ecoturistico+El+Nuevo+Mundo+-+Estoracon/@16.8505798,-93.7933739,17z/data=!3m1!4b1!4m6!3m5!1s0x85eca6200d7617bb:0x7498371825377da6!8m2!3d16.8505798!4d-93.7933739!16s%2Fg%2F11dxpchfty?authuser=0&amp;hl=es'&gt;Mapa del Parque Ecoturístico,Centro Ecoturístico,Parque Ecoturístico,Sitio Ecoturístico,Parque Ecológico,Parque Ecoturístico,Parque Natural,Parque Ecoturístico,Centro de Ecoturismo,Parque de Ecoturismo Centro Ecoturistico El Nuevo Mundo - Estoracon&lt;/a&gt;&lt;/p&gt;
-                        &lt;h3&gt;&lt;b&gt;¿Cuáles son los contactos del centro ecoturístico Centro Ecoturistico El Nuevo Mundo - Estoracon?&lt;/b&gt;&lt;/h3&gt;
-                            &lt;p&gt;Los contactos disponibles del Parque Ecológico Centro Ecoturistico El Nuevo Mundo - Estoracon son: &lt;/p&gt;
+                        &lt;p&gt;Bueno... pues ya que andas buscando salir de lo cotidiano... ¿Qué tal disfrutar de algunos de los paisajes más bonitos y naturales de undefined?. Pues eso es lo que centro de ecoturismo undefined te ofrece. Este sitio tiene una calificación promedio de undefined estrellas, a partir de opiniones de al menos undefined visitantes previos a ti, y es por eso que se considera uno de los top de este estado. Así que nada... sin excusas y ¡a vivir esta experiencia en la naturaleza!&lt;/p&gt;
+                        &lt;h3&gt;&lt;b&gt;¿Cómo llegar al Centro de Ecoturismo "Centro Ecoturistico El Nuevo Mundo - Estoracon"? &lt;/b&gt;&lt;/h3&gt;
+                            &lt;p&gt;Este parque natural se ubica en Carretera Sayula S/N, Francisco I. Madero, 30400 Cintalapa, Chis.
+ Puedes llegar a este centro facilmente manejando apoyándote en una aplicación de navegación (ej. maps) o consultando este &lt;a href='https://www.google.com/maps/place/Centro+Ecoturistico+El+Nuevo+Mundo+-+Estoracon/@16.8505798,-93.7933739,17z/data=!3m1!4b1!4m6!3m5!1s0x85eca6200d7617bb:0x7498371825377da6!8m2!3d16.8505798!4d-93.7933739!16s%2Fg%2F11dxpchfty?authuser=0&amp;hl=es'&gt;Mapa del Parque Ecoturístico Centro Ecoturistico El Nuevo Mundo - Estoracon&lt;/a&gt;&lt;/p&gt;
+                        &lt;h3&gt;&lt;b&gt;¿Cuáles son los contactos del parque ecoturístico Centro Ecoturistico El Nuevo Mundo - Estoracon?&lt;/b&gt;&lt;/h3&gt;
+                            &lt;p&gt;Los contactos disponibles del Centro Ecoturístico Centro Ecoturistico El Nuevo Mundo - Estoracon son: &lt;/p&gt;
                             &lt;ul&gt;
                                 &lt;li&gt;&lt;b&gt;Teléfono:&lt;/b&gt;961 284 4705&lt;/li&gt;
                                 &lt;li&gt;&lt;b&gt;SitioWeb:&lt;/b&gt;web no disponible&lt;/li&gt;                                
                             &lt;/ul&gt;
-                        &lt;h3&gt;&lt;b&gt;¿En qué horarios y días se puede visitar el sitio ecoturístico Centro Ecoturistico El Nuevo Mundo - Estoracon?&lt;/b&gt;&lt;/h3&gt;
-                            &lt;p&gt;Los horarios oficiales del parque ecoturístico Centro Ecoturistico El Nuevo Mundo - Estoracon son los siguientes:&lt;/p&gt;                       
+                        &lt;h3&gt;&lt;b&gt;¿En qué horarios y días se puede visitar el centro ecoturístico Centro Ecoturistico El Nuevo Mundo - Estoracon?&lt;/b&gt;&lt;/h3&gt;
+                            &lt;p&gt;Los horarios oficiales del centro de ecoturismo Centro Ecoturistico El Nuevo Mundo - Estoracon son los siguientes:&lt;/p&gt;                       
                             &lt;ul&gt;
                                 &lt;li&gt;Lunes de 10:00 a 19:00&lt;/li&gt;
                                 &lt;li&gt;Martes de 10:00 a 19:00&lt;/li&gt;
@@ -592,7 +593,7 @@
                                 &lt;li&gt;Sábado de 10:00 a 19:00&lt;/li&gt;
                                 &lt;li&gt;Domingo de 10:00 a 19:00&lt;/li&gt;
                             &lt;/ul&gt;
-                            &lt;p&gt;A pesar de contar con horarios oficiales, te recomendamos siempre visitar sus sitios de contacto y redes oficiales antes de ir al lugar, así podrás identificar cualquier cambio extraordinario que hayan tenido.&lt;/p&gt;                 
+                            &lt;p&gt;Antes de visitar el lugar, es una buena idea verificar sus sitios de contacto digitales y redes sociales, aún si ya cuentas con los horarios oficiales, para evitar cualquier cambio inesperado o sorpresas ya que estés ahí (por ej. cambio por días feriados)&lt;/p&gt;                 
                     </v>
       </c>
       <c r="AA2" t="str" xml:space="preserve">
@@ -636,7 +637,7 @@
         <v>https://www.google.com/maps/place/Siempre+Verde+Chiapas,+Centro+Ecotur%C3%ADstico/@17.143827,-92.888084,17z/data=!3m1!4b1!4m6!3m5!1s0x85ed0ee58c29248b:0xcdab59d265c14ddf!8m2!3d17.143827!4d-92.888084!16s%2Fg%2F11bvv4whms?authuser=0&amp;hl=es</v>
       </c>
       <c r="L3" t="str">
-        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3812.5419796816677!2d-92.88808399999999!3d17.143826999999998!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x85ed0ee58c29248b%3A0xcdab59d265c14ddf!2sSiempre%20Verde%20Chiapas%2C%20Centro%20Ecotur%C3%ADstico!5e0!3m2!1ses!2smx!4v1679086807159!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
+        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3812.5419796816677!2d-92.88808399999999!3d17.143826999999998!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x85ed0ee58c29248b%3A0xcdab59d265c14ddf!2sSiempre%20Verde%20Chiapas%2C%20Centro%20Ecotur%C3%ADstico!5e0!3m2!1ses!2smx!4v1679155880397!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
       </c>
       <c r="M3" t="str">
         <v>44V6+GQ Jitotol, Chiapas</v>
@@ -676,22 +677,23 @@
       </c>
       <c r="Y3" t="str" xml:space="preserve">
         <v xml:space="preserve">
-                    &lt;p&gt; ¿Estás buscando los mejores parques ecoturísticos en undefined? Entonces sin duda ¡estás en el lugar correcto!. Hoy en este artículo vamos a presentarte cuáles son los  sitio ecoturístico que han sido mejor evaluados en este estado. 
- Para poder definir esta listade los mejores, realizamos consultas en un montón de fuentes oficiales, redes sociales, rankings e incluso algunas entrevistas que nos permitieron determinar cuáles son y dónde se ubican los parque ecoturístico que mejores experiencias han brindado a sus visitantes, y que mayor calificación han recibido en undefined durante los últimos años. 
- Con esta prueba social como respaldo, hoy te compartimos la lista de los parque ecoturístico mejor calificados en undefined en function getFullYear() { [native code] } junto con su ubicación, medios oficiales de contacto, horarios y cómo llegar hasta ellos; así como la calificación promedio con la que cuenta cada lugar. 
- Prepárate con esto y ¡a disfrutar del ecoturismo en undefined!&lt;/p&gt;                    
+                    &lt;p&gt; ¿Estás buscando los mejores parques ecoturísticos en Chiapas? Entonces sin duda ¡estás en el lugar correcto!. Hoy en este artículo vamos a presentarte cuáles son los  parques ecoturísticos que han sido mejor evaluados en este estado. 
+ Para poder definir esta listade los mejores, realizamos consultas en un montón de fuentes oficiales, redes sociales, rankings e incluso algunas entrevistas que nos permitieron determinar cuáles son y dónde se ubican los parques de ecoturismo que mejores experiencias han brindado a sus visitantes, y que mayor calificación han recibido en Chiapas durante los últimos años. 
+ Con esta prueba social como respaldo, hoy te compartimos la lista de los parque ecológico mejor calificados en Chiapas en function getFullYear() { [native code] } junto con su ubicación, medios oficiales de contacto, horarios y cómo llegar hasta ellos; así como la calificación promedio con la que cuenta cada lugar. 
+ Prepárate con esto y ¡a disfrutar del ecoturismo en Chiapas!&lt;/p&gt;                    
                     </v>
       </c>
       <c r="Z3" t="str" xml:space="preserve">
         <v xml:space="preserve">
-                    &lt;h2&gt;&lt;b&gt;Parque Ecoturístico Siempre Verde Chiapas, Centro Ecoturístico&lt;/b&gt;&lt;/h2&gt;
+                    &lt;h2&gt;&lt;b&gt;Parque de Ecoturismo Siempre Verde Chiapas, Centro Ecoturístico&lt;/b&gt;&lt;/h2&gt;
                         &lt;img src="https://rumbonaturaleza.com/wp-content/uploads/2023/03/Siempre_Verde_Chiapas,_Centro_Ecoturístico_1.jpg" alt="Siempre Verde Chiapas, Centro Ecoturístico"&gt;   
-                        &lt;div&gt;&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3812.5419796816677!2d-92.88808399999999!3d17.143826999999998!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x85ed0ee58c29248b%3A0xcdab59d265c14ddf!2sSiempre%20Verde%20Chiapas%2C%20Centro%20Ecotur%C3%ADstico!5e0!3m2!1ses!2smx!4v1679086807159!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;&lt;/div&gt;
+                        &lt;div&gt;&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3812.5419796816677!2d-92.88808399999999!3d17.143826999999998!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x85ed0ee58c29248b%3A0xcdab59d265c14ddf!2sSiempre%20Verde%20Chiapas%2C%20Centro%20Ecotur%C3%ADstico!5e0!3m2!1ses!2smx!4v1679155880397!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;&lt;/div&gt;
                         &lt;div&gt;&lt;/div&gt;
-                        &lt;p&gt;Si estás en busca de un lugar para conectarte con la naturaleza, el parque ecoturístico undefined es una de tus mejores apuestas. Este sitio forma parte de esta lista de los mejores parques ecoturísticos de undefined gracias al respaldo y opiniones de más de undefined visitantes y que le han otorgado una calificación de más de undefined estrellas en promedio. Este lugar es sin duda uno de los mejores para disfrutar del entorno natural y paisajes de undefined y practicar el ecoturismo y la aventura en la región&lt;/p&gt;
-                        &lt;h3&gt;&lt;b&gt;¿Cómo llegar al Parque Natural "Siempre Verde Chiapas, Centro Ecoturístico"? &lt;/b&gt;&lt;/h3&gt;
-                            &lt;p&gt;El parque ecoturístico se ubica enCarretera Escopetazo Pichucalco Kilometro 81 S/N, El Campanario, 29760 Jitotol, Chis.. Si ya estás con todo listo para irte a este lugar entonces ¡no se diga más!, puedes ir siguiendo directamente la ruta de googleMaps mediante este &lt;a href='https://www.google.com/maps/place/Siempre+Verde+Chiapas,+Centro+Ecotur%C3%ADstico/@17.143827,-92.888084,17z/data=!3m1!4b1!4m6!3m5!1s0x85ed0ee58c29248b:0xcdab59d265c14ddf!8m2!3d17.143827!4d-92.888084!16s%2Fg%2F11bvv4whms?authuser=0&amp;hl=es'&gt;Mapa del Parque Ecoturístico,Centro Ecoturístico,Parque Ecoturístico,Sitio Ecoturístico,Parque Ecológico,Parque Ecoturístico,Parque Natural,Parque Ecoturístico,Centro de Ecoturismo,Parque de Ecoturismo Siempre Verde Chiapas, Centro Ecoturístico&lt;/a&gt;&lt;/p&gt;
-                        &lt;h3&gt;&lt;b&gt;¿Cuáles son los contactos del parque ecológico Siempre Verde Chiapas, Centro Ecoturístico?&lt;/b&gt;&lt;/h3&gt;
+                        &lt;p&gt;Si te apasiona la naturaleza y andas en busca de aventuras ¡pues no se diga más! porque sin duda el parque ecoturístico undefined es una opción en undefined que no debes dejar pasar. Este parque ecoturístico tiene una calificación promedio de undefined estrellas, basada en las opiniones de más de undefined visitantes, motivo por el que forma parte de este rank. Así es que... siendo uno de los parques ecoturísticos mejores calificados en undefined  ¿qué esperas para visitarlo?&lt;/p&gt;
+                        &lt;h3&gt;&lt;b&gt;¿Cómo llegar al Centro Ecoturístico "Siempre Verde Chiapas, Centro Ecoturístico"? &lt;/b&gt;&lt;/h3&gt;
+                            &lt;p&gt;Este parque de ecoturismo se ubica en Carretera Escopetazo Pichucalco Kilometro 81 S/N, El Campanario, 29760 Jitotol, Chis.
+ Si necesitas ir a este sitio manejando puedes apoyarte poniendo la dirección en un navegador tipo waze o googleMaps o siguiendo directamente este &lt;a href='https://www.google.com/maps/place/Siempre+Verde+Chiapas,+Centro+Ecotur%C3%ADstico/@17.143827,-92.888084,17z/data=!3m1!4b1!4m6!3m5!1s0x85ed0ee58c29248b:0xcdab59d265c14ddf!8m2!3d17.143827!4d-92.888084!16s%2Fg%2F11bvv4whms?authuser=0&amp;hl=es'&gt;Mapa del Parque Natural Siempre Verde Chiapas, Centro Ecoturístico&lt;/a&gt;&lt;/p&gt;
+                        &lt;h3&gt;&lt;b&gt;¿Cuáles son los contactos del parque de ecoturismo Siempre Verde Chiapas, Centro Ecoturístico?&lt;/b&gt;&lt;/h3&gt;
                             &lt;p&gt;Los contactos disponibles del Parque Ecoturístico Siempre Verde Chiapas, Centro Ecoturístico son: &lt;/p&gt;
                             &lt;ul&gt;
                                 &lt;li&gt;&lt;b&gt;Teléfono:&lt;/b&gt;919 104 9970&lt;/li&gt;
@@ -708,7 +710,7 @@
                                 &lt;li&gt;undefined&lt;/li&gt;
                                 &lt;li&gt;undefined&lt;/li&gt;
                             &lt;/ul&gt;
-                            &lt;p&gt;Antes de visitar el lugar, es importante revisar sus sitios digitales y redes sociales, así te aseguras de detectar cualquier cambio que hayan tenido de última hora por cuestiones de fechas especiales, vacaciones, temporadas altas, etc&lt;/p&gt;                 
+                            &lt;p&gt;A pesar de contar con horarios oficiales, te recomendamos siempre visitar sus sitios de contacto y redes oficiales antes de ir al lugar, así podrás identificar cualquier cambio extraordinario que hayan tenido.&lt;/p&gt;                 
                     </v>
       </c>
       <c r="AA3" t="str" xml:space="preserve">
@@ -725,116 +727,116 @@
         <v>3</v>
       </c>
       <c r="B4" t="str">
-        <v>Centro Ecoturístico "El Aguacero"</v>
+        <v>Parque Ecoturistico Tzimbac</v>
       </c>
       <c r="C4" t="str">
-        <v>Centro Ecoturístico "el Aguacero"</v>
+        <v>Parque Ecoturistico Tzimbac</v>
       </c>
       <c r="D4" t="str">
-        <v>centro ecoturístico "el aguacero"</v>
+        <v>parque ecoturistico tzimbac</v>
       </c>
       <c r="E4" t="str">
-        <v>Unnamed Road, Chis.</v>
+        <v>Carretera a Monterrey Km. 2.2, Villarreal, 29125 Chis.</v>
       </c>
       <c r="F4" t="str">
-        <v>968 106 9019</v>
+        <v>961 286 8575</v>
       </c>
       <c r="G4" t="str">
-        <v>http://www.cascadaelaguacero.com/</v>
+        <v>Web no disponible</v>
       </c>
       <c r="I4" t="str">
-        <v>El Recuerdo, Chiapas</v>
+        <v>Santa Rita, Chiapas</v>
       </c>
       <c r="J4" t="str">
         <v>Chiapas</v>
       </c>
       <c r="K4" t="str">
-        <v>https://www.google.com/maps/place/Centro+Ecotur%C3%ADstico+%22El+Aguacero%22/@16.7591291,-93.5246499,17z/data=!3m1!4b1!4m6!3m5!1s0x85ecbbbeb75d1b1f:0x70f4450b76c6d0b!8m2!3d16.7591291!4d-93.5246499!16s%2Fg%2F11g6mr_n7p?authuser=0&amp;hl=es</v>
+        <v>https://www.google.com/maps/place/Parque+Ecoturistico+Tzimbac/@16.8998672,-93.2289146,17z/data=!3m1!4b1!4m6!3m5!1s0x85ece790120fdba7:0xf3cf8d4d73cd7595!8m2!3d16.8998672!4d-93.2289146!16s%2Fg%2F12hm176_z?authuser=0&amp;hl=es</v>
       </c>
       <c r="L4" t="str">
-        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3820.352500879553!2d-93.5246499!3d16.7591291!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x85ecbbbeb75d1b1f%3A0x70f4450b76c6d0b!2sCentro%20Ecotur%C3%ADstico%20%22El%20Aguacero%22!5e0!3m2!1ses!2smx!4v1679086811873!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
+        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3817.515055110652!2d-93.2289146!3d16.8998672!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x85ece790120fdba7%3A0xf3cf8d4d73cd7595!2sParque%20Ecoturistico%20Tzimbac!5e0!3m2!1ses!2smx!4v1679155885639!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
       </c>
       <c r="M4" t="str">
-        <v>QF5G+M4 El Recuerdo, Chiapas</v>
+        <v>VQXC+WC Santa Rita, Chiapas</v>
       </c>
       <c r="N4" t="str">
-        <v>4.6</v>
+        <v>4.2</v>
       </c>
       <c r="O4" t="str">
-        <v>318</v>
-      </c>
-      <c r="P4" t="str" xml:space="preserve">
-        <v xml:space="preserve">Un lugar maravilloso para visitar, te exige mucha condición (ir preparados con calzado para escalar o senderismo) y llevar ropa cómoda.
-La comida del restaurante es excelente y con un sazón único!…,Increible lugar, antes de ir necesitas saber que para llegar a la cascada hay que caminar 30 minutos aproximadamente, escaleras hacia abajo, son más de 700 escalones más una caminata de unos 200 metros sobre el río. No hay partes ondas y hay mucho lugar para montar un picnic.,Es un lugar increíble!! Si no tienes coche el acceso esta algo complicado pero vale la pena, es mas para pasar el día llevar de comer o incluso acampar, la altura del río es pequeña así que no es tanto para nadar pero bastante agradable, cobran una entrada de aproximadamente 60 pesos</v>
+        <v>46</v>
+      </c>
+      <c r="P4" t="str">
+        <v>Si te gusta la naturaleza visítalo, si esperas muchas comodidades no es un sitio para ti. No hay señal, los baños están módicamente cómodos (si vas a la naturaleza no esperes lujos), hay área para acampar, muy limpio. Fuimos y nos tocó…,Buen lugar para descansar y rejarte un rato, sin embargo podría mejorar en muchos detalles, porque en época de lluvia es imposible disfrutar de la naturaleza, tener más sanitarios o en áreas más comunes.,Exelente lugar para ir con la familia y amigos. Podras acampar, explorar, senderismo, rappel, tirolesa, montar a caballo. Todo esto rodeo de magia y naturaleza respirando aire puro, fuera de la cantaminacion de la ciudad; puedes realozar…</v>
       </c>
       <c r="Q4" t="str">
-        <v>https://lh5.googleusercontent.com/p/AF1QipPtbKPypMyq7Ne_R7EO2WsnKqRywG7IpYIsf5Im=w408-h544-k-no</v>
+        <v>https://lh5.googleusercontent.com/p/AF1QipNYYHKIZRIqOhYXADcr3o_zu4-ho3SpnynhRZrw=w408-h306-k-no</v>
       </c>
       <c r="R4" t="str">
-        <v>wget --no-check-certificate https://lh5.googleusercontent.com/p/AF1QipPtbKPypMyq7Ne_R7EO2WsnKqRywG7IpYIsf5Im=w408-h544-k-no</v>
+        <v>wget --no-check-certificate https://lh5.googleusercontent.com/p/AF1QipNYYHKIZRIqOhYXADcr3o_zu4-ho3SpnynhRZrw=w408-h306-k-no</v>
       </c>
       <c r="S4" t="str">
-        <v>AF1QipPtbKPypMyq7Ne_R7EO2WsnKqRywG7IpYIsf5Im=w408-h544-k-no</v>
+        <v>AF1QipNYYHKIZRIqOhYXADcr3o_zu4-ho3SpnynhRZrw=w408-h306-k-no</v>
       </c>
       <c r="T4" t="str">
-        <v>Centro_Ecoturístico_"El_Aguacero"_2</v>
+        <v>Parque_Ecoturistico_Tzimbac_2</v>
       </c>
       <c r="U4" t="str">
-        <v>Centro_Ecoturístico_"El_Aguacero"_2.jpg</v>
+        <v>Parque_Ecoturistico_Tzimbac_2.jpg</v>
       </c>
       <c r="V4" t="str">
-        <v>https://rumbonaturaleza.com/wp-content/uploads/2023/03/Centro_Ecoturístico_"El_Aguacero"_2.jpg</v>
+        <v>https://rumbonaturaleza.com/wp-content/uploads/2023/03/Parque_Ecoturistico_Tzimbac_2.jpg</v>
       </c>
       <c r="W4" t="str">
-        <v>ren "AF1QipPtbKPypMyq7Ne_R7EO2WsnKqRywG7IpYIsf5Im=w408-h544-k-no" "Centro_Ecoturístico_"El_Aguacero"_2.jpg"</v>
+        <v>ren "AF1QipNYYHKIZRIqOhYXADcr3o_zu4-ho3SpnynhRZrw=w408-h306-k-no" "Parque_Ecoturistico_Tzimbac_2.jpg"</v>
       </c>
       <c r="X4" t="str">
         <v>parques-ecoturismo-en-chiapas</v>
       </c>
       <c r="Y4" t="str" xml:space="preserve">
         <v xml:space="preserve">
-                    &lt;p&gt; ¿Estás buscando los mejores parques ecoturísticos en undefined? Entonces sin duda ¡estás en el lugar correcto!. Hoy en este artículo vamos a presentarte cuáles son los  parque ecoturístico que han sido mejor evaluados en este estado. 
- Para poder definir esta listade los mejores, realizamos consultas en un montón de fuentes oficiales, redes sociales, rankings e incluso algunas entrevistas que nos permitieron determinar cuáles son y dónde se ubican los centro ecoturístico que mejores experiencias han brindado a sus visitantes, y que mayor calificación han recibido en undefined durante los últimos años. 
- Con esta prueba social como respaldo, hoy te compartimos la lista de los parque ecoturístico mejor calificados en undefined en function getFullYear() { [native code] } junto con su ubicación, medios oficiales de contacto, horarios y cómo llegar hasta ellos; así como la calificación promedio con la que cuenta cada lugar. 
- Prepárate con esto y ¡a disfrutar del ecoturismo en undefined!&lt;/p&gt;                    
+                    &lt;p&gt; ¿Estás buscando los mejores parques ecoturísticos en Chiapas? Entonces sin duda ¡estás en el lugar correcto!. Hoy en este artículo vamos a presentarte cuáles son los  parques ecoturísticos que han sido mejor evaluados en este estado. 
+ Para poder definir esta listade los mejores, realizamos consultas en un montón de fuentes oficiales, redes sociales, rankings e incluso algunas entrevistas que nos permitieron determinar cuáles son y dónde se ubican los parques ecoturísticos que mejores experiencias han brindado a sus visitantes, y que mayor calificación han recibido en Chiapas durante los últimos años. 
+ Con esta prueba social como respaldo, hoy te compartimos la lista de los centro ecoturístico mejor calificados en Chiapas en function getFullYear() { [native code] } junto con su ubicación, medios oficiales de contacto, horarios y cómo llegar hasta ellos; así como la calificación promedio con la que cuenta cada lugar. 
+ Prepárate con esto y ¡a disfrutar del ecoturismo en Chiapas!&lt;/p&gt;                    
                     </v>
       </c>
       <c r="Z4" t="str" xml:space="preserve">
         <v xml:space="preserve">
-                    &lt;h2&gt;&lt;b&gt;Parque Natural Centro Ecoturístico "el Aguacero"&lt;/b&gt;&lt;/h2&gt;
-                        &lt;img src="https://rumbonaturaleza.com/wp-content/uploads/2023/03/Centro_Ecoturístico_"El_Aguacero"_2.jpg" alt="Centro Ecoturístico "El Aguacero""&gt;   
-                        &lt;div&gt;&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3820.352500879553!2d-93.5246499!3d16.7591291!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x85ecbbbeb75d1b1f%3A0x70f4450b76c6d0b!2sCentro%20Ecotur%C3%ADstico%20%22El%20Aguacero%22!5e0!3m2!1ses!2smx!4v1679086811873!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;&lt;/div&gt;
+                    &lt;h2&gt;&lt;b&gt;Centro Ecoturístico Parque Ecoturistico Tzimbac&lt;/b&gt;&lt;/h2&gt;
+                        &lt;img src="https://rumbonaturaleza.com/wp-content/uploads/2023/03/Parque_Ecoturistico_Tzimbac_2.jpg" alt="Parque Ecoturistico Tzimbac"&gt;   
+                        &lt;div&gt;&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3817.515055110652!2d-93.2289146!3d16.8998672!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x85ece790120fdba7%3A0xf3cf8d4d73cd7595!2sParque%20Ecoturistico%20Tzimbac!5e0!3m2!1ses!2smx!4v1679155885639!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;&lt;/div&gt;
                         &lt;div&gt;&lt;/div&gt;
-                        &lt;p&gt;Uno de los sitios naturales más memorables de undefined es sin duda alguna el parque ecoturístico undefined. Este lugar está respaldado por un montón de visitantes previos y más de undefined evaluaciones promedio que rondan las undefined estrellas, lo que lo hace un favorito de esta región. Es por eso que forma parte de esta lista de los mejores centros ecoturísticos de undefined, y es por eso también que nos parece una recomendación imperdible para ti.&lt;/p&gt;
-                        &lt;h3&gt;&lt;b&gt;¿Cómo llegar al Parque Ecoturístico "Centro Ecoturístico "el Aguacero""? &lt;/b&gt;&lt;/h3&gt;
-                            &lt;p&gt;El parque de ecoturismo se ubica enUnnamed Road, Chis.. Para llegar a este lugar, simplemente ingresa la dirección en una app de navegación o utiliza este enlace al&lt;a href='https://www.google.com/maps/place/Centro+Ecotur%C3%ADstico+%22El+Aguacero%22/@16.7591291,-93.5246499,17z/data=!3m1!4b1!4m6!3m5!1s0x85ecbbbeb75d1b1f:0x70f4450b76c6d0b!8m2!3d16.7591291!4d-93.5246499!16s%2Fg%2F11g6mr_n7p?authuser=0&amp;hl=es'&gt;Mapa del Parque Ecoturístico,Centro Ecoturístico,Parque Ecoturístico,Sitio Ecoturístico,Parque Ecológico,Parque Ecoturístico,Parque Natural,Parque Ecoturístico,Centro de Ecoturismo,Parque de Ecoturismo Centro Ecoturístico "el Aguacero"&lt;/a&gt;&lt;/p&gt;
-                        &lt;h3&gt;&lt;b&gt;¿Cuáles son los contactos del centro ecoturístico Centro Ecoturístico "el Aguacero"?&lt;/b&gt;&lt;/h3&gt;
-                            &lt;p&gt;Los contactos disponibles del Parque Ecológico Centro Ecoturístico "el Aguacero" son: &lt;/p&gt;
+                        &lt;p&gt;Este sitio ecoturístico tiene undefined estrellas de calificación promedio, a partir de las más de undefined opiniones de sus visitantes... ¿nada mal no?. Es por esto que undefined es parte de esta lista de los parques naturales mejor calificados de undefined. Con este respaldo estamos más que seguras(os) que se trata  de un sitio que vas a disfrutar al Máximo. Así que ya sabes, si lo que buscas es naturaleza, el parque ecoturístico undefined en undefined es sin duda una gran opción&lt;/p&gt;
+                        &lt;h3&gt;&lt;b&gt;¿Cómo llegar al Centro Ecoturístico "Parque Ecoturistico Tzimbac"? &lt;/b&gt;&lt;/h3&gt;
+                            &lt;p&gt;Este centro ecoturístico se ubica en Carretera a Monterrey Km. 2.2, Villarreal, 29125 Chis.
+ Para llegar a este lugar, simplemente ingresa la dirección en una app de navegación o utiliza este enlace al&lt;a href='https://www.google.com/maps/place/Parque+Ecoturistico+Tzimbac/@16.8998672,-93.2289146,17z/data=!3m1!4b1!4m6!3m5!1s0x85ece790120fdba7:0xf3cf8d4d73cd7595!8m2!3d16.8998672!4d-93.2289146!16s%2Fg%2F12hm176_z?authuser=0&amp;hl=es'&gt;Mapa del Parque Ecoturístico Parque Ecoturistico Tzimbac&lt;/a&gt;&lt;/p&gt;
+                        &lt;h3&gt;&lt;b&gt;¿Cuáles son los contactos del centro de ecoturismo Parque Ecoturistico Tzimbac?&lt;/b&gt;&lt;/h3&gt;
+                            &lt;p&gt;Los contactos disponibles del Centro Ecoturístico Parque Ecoturistico Tzimbac son: &lt;/p&gt;
                             &lt;ul&gt;
-                                &lt;li&gt;&lt;b&gt;Teléfono:&lt;/b&gt;968 106 9019&lt;/li&gt;
-                                &lt;li&gt;&lt;b&gt;SitioWeb:&lt;/b&gt;&lt;a href="http://www.cascadaelaguacero.com/"&gt;Web del place Centro Ecoturístico "El Aguacero"&lt;/a&gt;&lt;/li&gt;                                
+                                &lt;li&gt;&lt;b&gt;Teléfono:&lt;/b&gt;961 286 8575&lt;/li&gt;
+                                &lt;li&gt;&lt;b&gt;SitioWeb:&lt;/b&gt;web no disponible&lt;/li&gt;                                
                             &lt;/ul&gt;
-                        &lt;h3&gt;&lt;b&gt;¿En qué horarios y días se puede visitar el centro de ecoturismo Centro Ecoturístico "el Aguacero"?&lt;/b&gt;&lt;/h3&gt;
-                            &lt;p&gt;Los horarios oficiales del parque ecoturístico Centro Ecoturístico "el Aguacero" son los siguientes:&lt;/p&gt;                       
+                        &lt;h3&gt;&lt;b&gt;¿En qué horarios y días se puede visitar el sitio ecoturístico Parque Ecoturistico Tzimbac?&lt;/b&gt;&lt;/h3&gt;
+                            &lt;p&gt;Los horarios oficiales del centro de ecoturismo Parque Ecoturistico Tzimbac son los siguientes:&lt;/p&gt;                       
                             &lt;ul&gt;
-                                &lt;li&gt;Lunes de 07:00 a 17:00&lt;/li&gt;
-                                &lt;li&gt;Martes de 07:00 a 17:00&lt;/li&gt;
-                                &lt;li&gt;Miércoles de 07:00 a 17:00&lt;/li&gt;
-                                &lt;li&gt;Jueves de 07:00 a 17:00&lt;/li&gt;
-                                &lt;li&gt;Viernes de 07:00 a 17:00&lt;/li&gt;
-                                &lt;li&gt;Sábado de 07:00 a 17:00&lt;/li&gt;
-                                &lt;li&gt;Domingo de 07:00 a 17:00&lt;/li&gt;
+                                &lt;li&gt;undefined&lt;/li&gt;
+                                &lt;li&gt;undefined&lt;/li&gt;
+                                &lt;li&gt;undefined&lt;/li&gt;
+                                &lt;li&gt;undefined&lt;/li&gt;
+                                &lt;li&gt;undefined&lt;/li&gt;
+                                &lt;li&gt;undefined&lt;/li&gt;
+                                &lt;li&gt;undefined&lt;/li&gt;
                             &lt;/ul&gt;
-                            &lt;p&gt;Te recomendamos  igual siempre revisar sus redes sociales y contactos digitales antes de ir, pues aunque este horario es oficial, pueden haber cambios en fechas especiales, épocas vacacionales y demás&lt;/p&gt;                 
+                            &lt;p&gt;A pesar de que los horarios sean oficiales, es buena idea que antes ir, revises siempre cómo están las cosas en sus redes sociales y contactos digitales, esto te permitirá asegurarte de que no haya cambios de horario o logística antes de tu arribo al lugar&lt;/p&gt;                 
                     </v>
       </c>
       <c r="AA4" t="str" xml:space="preserve">
         <v xml:space="preserve">
-                    &lt;img src="https://rumbonaturaleza.com/wp-content/uploads/2023/03/Centro_Ecoturístico_"El_Aguacero"_2.jpg" alt="Centro Ecoturístico "El Aguacero""&gt;                
+                    &lt;img src="https://rumbonaturaleza.com/wp-content/uploads/2023/03/Parque_Ecoturistico_Tzimbac_2.jpg" alt="Parque Ecoturistico Tzimbac"&gt;                
                 </v>
       </c>
       <c r="AB4" t="str">
-        <v/>
+        <v>Añadir sitio web</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
WIP_Horario bug corregido para mostrar horario string en resultado excel_Completed :)
</commit_message>
<xml_diff>
--- a/testingAllImports.xlsx
+++ b/testingAllImports.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB4"/>
+  <dimension ref="A1:AC4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -428,63 +428,66 @@
         <v>horario</v>
       </c>
       <c r="I1" t="str">
+        <v>horarioText</v>
+      </c>
+      <c r="J1" t="str">
         <v>cityClean</v>
       </c>
-      <c r="J1" t="str">
+      <c r="K1" t="str">
         <v>state</v>
       </c>
-      <c r="K1" t="str">
+      <c r="L1" t="str">
         <v>urlgMaps</v>
       </c>
-      <c r="L1" t="str">
+      <c r="M1" t="str">
         <v>iframeMap</v>
       </c>
-      <c r="M1" t="str">
+      <c r="N1" t="str">
         <v>city</v>
       </c>
-      <c r="N1" t="str">
+      <c r="O1" t="str">
         <v>stars</v>
       </c>
-      <c r="O1" t="str">
+      <c r="P1" t="str">
         <v>cantidadResenas</v>
       </c>
-      <c r="P1" t="str">
+      <c r="Q1" t="str">
         <v>opiniones</v>
       </c>
-      <c r="Q1" t="str">
+      <c r="R1" t="str">
         <v>photoOriginalURL</v>
       </c>
-      <c r="R1" t="str">
+      <c r="S1" t="str">
         <v>photoDownloadScript</v>
       </c>
-      <c r="S1" t="str">
+      <c r="T1" t="str">
         <v>photoFileName</v>
       </c>
-      <c r="T1" t="str">
+      <c r="U1" t="str">
         <v>photoNewName</v>
       </c>
-      <c r="U1" t="str">
+      <c r="V1" t="str">
         <v>photoNewFullFileName</v>
       </c>
-      <c r="V1" t="str">
+      <c r="W1" t="str">
         <v>photoNewURL</v>
       </c>
-      <c r="W1" t="str">
+      <c r="X1" t="str">
         <v>fileNameConversionScript</v>
       </c>
-      <c r="X1" t="str">
+      <c r="Y1" t="str">
         <v>slug</v>
       </c>
-      <c r="Y1" t="str">
+      <c r="Z1" t="str">
         <v>articleIntro</v>
       </c>
-      <c r="Z1" t="str">
+      <c r="AA1" t="str">
         <v>structuredData</v>
       </c>
-      <c r="AA1" t="str">
+      <c r="AB1" t="str">
         <v>photoLocal</v>
       </c>
-      <c r="AB1" t="str">
+      <c r="AC1" t="str">
         <v>missingData</v>
       </c>
     </row>
@@ -511,79 +514,82 @@
         <v>Web no disponible</v>
       </c>
       <c r="I2" t="str">
+        <v>Sábado de 10:00 a 19:00,Domingo de 10:00 a 19:00,Lunes de 10:00 a 19:00,Martes de 10:00 a 19:00,Miércoles de 10:00 a 19:00,Jueves de 10:00 a 19:00,Viernes de 10:00 a 19:00</v>
+      </c>
+      <c r="J2" t="str">
         <v>Estoracón, Chiapas</v>
       </c>
-      <c r="J2" t="str">
+      <c r="K2" t="str">
         <v>Chiapas</v>
       </c>
-      <c r="K2" t="str">
+      <c r="L2" t="str">
         <v>https://www.google.com/maps/place/Centro+Ecoturistico+El+Nuevo+Mundo+-+Estoracon/@16.8505798,-93.7933739,17z/data=!3m1!4b1!4m6!3m5!1s0x85eca6200d7617bb:0x7498371825377da6!8m2!3d16.8505798!4d-93.7933739!16s%2Fg%2F11dxpchfty?authuser=0&amp;hl=es</v>
       </c>
-      <c r="L2" t="str">
-        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3818.5113687598837!2d-93.79337389999999!3d16.8505798!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x85eca6200d7617bb%3A0x7498371825377da6!2sCentro%20Ecoturistico%20El%20Nuevo%20Mundo%20-%20Estoracon!5e0!3m2!1ses!2smx!4v1679155875054!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
-      </c>
       <c r="M2" t="str">
+        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3818.5113687598837!2d-93.79337389999999!3d16.8505798!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x85eca6200d7617bb%3A0x7498371825377da6!2sCentro%20Ecoturistico%20El%20Nuevo%20Mundo%20-%20Estoracon!5e0!3m2!1ses!2smx!4v1679160007861!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
+      </c>
+      <c r="N2" t="str">
         <v>V624+6M Estoracón, Chiapas</v>
       </c>
-      <c r="N2" t="str">
+      <c r="O2" t="str">
         <v>4.5</v>
       </c>
-      <c r="O2" t="str">
+      <c r="P2" t="str">
         <v>31</v>
       </c>
-      <c r="P2" t="str">
+      <c r="Q2" t="str">
         <v>Hermoso día de excursión en familia a este sitio remoto con 4 cascadas en plena naturaleza con piscina y una comida riquísima con buena atención, los Tucanes con muchi acercamiento, salimos de Cintalapa Chiapas,Muy bonita reserva recomendable,Se puede acampar ($180 por tienda de campaña), hay cabañas (sencilla $400, doble $800), rentan hamacas, tienda de campaña, venden refrescos, cervezas, sabritas, buena comida(camarones empanizado, en ensalada , mojarras, carne asada, pollo,…</v>
       </c>
-      <c r="Q2" t="str">
+      <c r="R2" t="str">
         <v>https://lh5.googleusercontent.com/p/AF1QipPOgfBL_SMdx6bZCZHeZCe150jGe-GqwXaX7lE=w408-h306-k-no</v>
       </c>
-      <c r="R2" t="str">
+      <c r="S2" t="str">
         <v>wget --no-check-certificate https://lh5.googleusercontent.com/p/AF1QipPOgfBL_SMdx6bZCZHeZCe150jGe-GqwXaX7lE=w408-h306-k-no</v>
       </c>
-      <c r="S2" t="str">
+      <c r="T2" t="str">
         <v>AF1QipPOgfBL_SMdx6bZCZHeZCe150jGe-GqwXaX7lE=w408-h306-k-no</v>
       </c>
-      <c r="T2" t="str">
+      <c r="U2" t="str">
         <v>Centro_Ecoturistico_El_Nuevo_Mundo_-_Estoracon_0</v>
       </c>
-      <c r="U2" t="str">
+      <c r="V2" t="str">
         <v>Centro_Ecoturistico_El_Nuevo_Mundo_-_Estoracon_0.jpg</v>
       </c>
-      <c r="V2" t="str">
+      <c r="W2" t="str">
         <v>https://rumbonaturaleza.com/wp-content/uploads/2023/03/Centro_Ecoturistico_El_Nuevo_Mundo_-_Estoracon_0.jpg</v>
       </c>
-      <c r="W2" t="str">
+      <c r="X2" t="str">
         <v>ren "AF1QipPOgfBL_SMdx6bZCZHeZCe150jGe-GqwXaX7lE=w408-h306-k-no" "Centro_Ecoturistico_El_Nuevo_Mundo_-_Estoracon_0.jpg"</v>
       </c>
-      <c r="X2" t="str">
+      <c r="Y2" t="str">
         <v>parques-ecoturismo-en-chiapas</v>
       </c>
-      <c r="Y2" t="str" xml:space="preserve">
+      <c r="Z2" t="str" xml:space="preserve">
         <v xml:space="preserve">
-                    &lt;p&gt; ¿Estás buscando los mejores parques ecoturísticos en Chiapas? Entonces sin duda ¡estás en el lugar correcto!. Hoy en este artículo vamos a presentarte cuáles son los  parques ecoturísticos que han sido mejor evaluados en este estado. 
- Para poder definir esta listade los mejores, realizamos consultas en un montón de fuentes oficiales, redes sociales, rankings e incluso algunas entrevistas que nos permitieron determinar cuáles son y dónde se ubican los parques de ecoturismo que mejores experiencias han brindado a sus visitantes, y que mayor calificación han recibido en Chiapas durante los últimos años. 
- Con esta prueba social como respaldo, hoy te compartimos la lista de los parque ecológico mejor calificados en Chiapas en function getFullYear() { [native code] } junto con su ubicación, medios oficiales de contacto, horarios y cómo llegar hasta ellos; así como la calificación promedio con la que cuenta cada lugar. 
+                    &lt;p&gt; ¿Estás buscando los mejores parques ecoturísticos en Chiapas? Entonces sin duda ¡estás en el lugar correcto!. Hoy en este artículo vamos a presentarte cuáles son los  centros de ecoturismo que han sido mejor evaluados en este estado. 
+ Para poder definir esta listade los mejores, realizamos consultas en un montón de fuentes oficiales, redes sociales, rankings e incluso algunas entrevistas que nos permitieron determinar cuáles son y dónde se ubican los centros ecoturísticos que mejores experiencias han brindado a sus visitantes, y que mayor calificación han recibido en Chiapas durante los últimos años. 
+ Con esta prueba social como respaldo, hoy te compartimos la lista de los parque natural mejor calificados en Chiapas en function getFullYear() { [native code] } junto con su ubicación, medios oficiales de contacto, horarios y cómo llegar hasta ellos; así como la calificación promedio con la que cuenta cada lugar. 
  Prepárate con esto y ¡a disfrutar del ecoturismo en Chiapas!&lt;/p&gt;                    
                     </v>
       </c>
-      <c r="Z2" t="str" xml:space="preserve">
+      <c r="AA2" t="str" xml:space="preserve">
         <v xml:space="preserve">
-                    &lt;h2&gt;&lt;b&gt;Sitio Ecoturístico Centro Ecoturistico El Nuevo Mundo - Estoracon&lt;/b&gt;&lt;/h2&gt;
+                    &lt;h2&gt;&lt;b&gt;Parque Ecoturístico Centro Ecoturistico El Nuevo Mundo - Estoracon&lt;/b&gt;&lt;/h2&gt;
                         &lt;img src="https://rumbonaturaleza.com/wp-content/uploads/2023/03/Centro_Ecoturistico_El_Nuevo_Mundo_-_Estoracon_0.jpg" alt="Centro Ecoturistico El Nuevo Mundo - Estoracon"&gt;   
-                        &lt;div&gt;&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3818.5113687598837!2d-93.79337389999999!3d16.8505798!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x85eca6200d7617bb%3A0x7498371825377da6!2sCentro%20Ecoturistico%20El%20Nuevo%20Mundo%20-%20Estoracon!5e0!3m2!1ses!2smx!4v1679155875054!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;&lt;/div&gt;
+                        &lt;div&gt;&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3818.5113687598837!2d-93.79337389999999!3d16.8505798!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x85eca6200d7617bb%3A0x7498371825377da6!2sCentro%20Ecoturistico%20El%20Nuevo%20Mundo%20-%20Estoracon!5e0!3m2!1ses!2smx!4v1679160007861!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;&lt;/div&gt;
                         &lt;div&gt;&lt;/div&gt;
-                        &lt;p&gt;Bueno... pues ya que andas buscando salir de lo cotidiano... ¿Qué tal disfrutar de algunos de los paisajes más bonitos y naturales de undefined?. Pues eso es lo que centro de ecoturismo undefined te ofrece. Este sitio tiene una calificación promedio de undefined estrellas, a partir de opiniones de al menos undefined visitantes previos a ti, y es por eso que se considera uno de los top de este estado. Así que nada... sin excusas y ¡a vivir esta experiencia en la naturaleza!&lt;/p&gt;
-                        &lt;h3&gt;&lt;b&gt;¿Cómo llegar al Centro de Ecoturismo "Centro Ecoturistico El Nuevo Mundo - Estoracon"? &lt;/b&gt;&lt;/h3&gt;
-                            &lt;p&gt;Este parque natural se ubica en Carretera Sayula S/N, Francisco I. Madero, 30400 Cintalapa, Chis.
- Puedes llegar a este centro facilmente manejando apoyándote en una aplicación de navegación (ej. maps) o consultando este &lt;a href='https://www.google.com/maps/place/Centro+Ecoturistico+El+Nuevo+Mundo+-+Estoracon/@16.8505798,-93.7933739,17z/data=!3m1!4b1!4m6!3m5!1s0x85eca6200d7617bb:0x7498371825377da6!8m2!3d16.8505798!4d-93.7933739!16s%2Fg%2F11dxpchfty?authuser=0&amp;hl=es'&gt;Mapa del Parque Ecoturístico Centro Ecoturistico El Nuevo Mundo - Estoracon&lt;/a&gt;&lt;/p&gt;
+                        &lt;p&gt;¿Quieres vivir un paseo increible en contacto con la naturaleza? entonces no puedes dejar de considerar una visita al centro de ecoturismo undefined en undefined. Con una calificación promedio de undefined estrellas y más de undefined opiniones de visitantes, este lugar es una de las mejores opciones para los amantes del ecoturismo en esta región. Así es que ¡toma nota  de todo lo requerido para tu visita a continuación!&lt;/p&gt;
+                        &lt;h3&gt;&lt;b&gt;¿Cómo llegar al Parque Natural "Centro Ecoturistico El Nuevo Mundo - Estoracon"? &lt;/b&gt;&lt;/h3&gt;
+                            &lt;p&gt;Este parque ecoturístico se ubica en Carretera Sayula S/N, Francisco I. Madero, 30400 Cintalapa, Chis.
+ La verdad es que llegar a este Centro no tiene gran dificultad. Puedes encontrar la dirección de un lugar siguiendo cualquier aplicación de navegación que se te facilite o siguiendo esta liga al &lt;a href='https://www.google.com/maps/place/Centro+Ecoturistico+El+Nuevo+Mundo+-+Estoracon/@16.8505798,-93.7933739,17z/data=!3m1!4b1!4m6!3m5!1s0x85eca6200d7617bb:0x7498371825377da6!8m2!3d16.8505798!4d-93.7933739!16s%2Fg%2F11dxpchfty?authuser=0&amp;hl=es'&gt;Mapa del Parque Ecoturístico Centro Ecoturistico El Nuevo Mundo - Estoracon&lt;/a&gt;&lt;/p&gt;
                         &lt;h3&gt;&lt;b&gt;¿Cuáles son los contactos del parque ecoturístico Centro Ecoturistico El Nuevo Mundo - Estoracon?&lt;/b&gt;&lt;/h3&gt;
-                            &lt;p&gt;Los contactos disponibles del Centro Ecoturístico Centro Ecoturistico El Nuevo Mundo - Estoracon son: &lt;/p&gt;
+                            &lt;p&gt;Los contactos disponibles del Parque de Ecoturismo Centro Ecoturistico El Nuevo Mundo - Estoracon son: &lt;/p&gt;
                             &lt;ul&gt;
                                 &lt;li&gt;&lt;b&gt;Teléfono:&lt;/b&gt;961 284 4705&lt;/li&gt;
                                 &lt;li&gt;&lt;b&gt;SitioWeb:&lt;/b&gt;web no disponible&lt;/li&gt;                                
                             &lt;/ul&gt;
-                        &lt;h3&gt;&lt;b&gt;¿En qué horarios y días se puede visitar el centro ecoturístico Centro Ecoturistico El Nuevo Mundo - Estoracon?&lt;/b&gt;&lt;/h3&gt;
-                            &lt;p&gt;Los horarios oficiales del centro de ecoturismo Centro Ecoturistico El Nuevo Mundo - Estoracon son los siguientes:&lt;/p&gt;                       
+                        &lt;h3&gt;&lt;b&gt;¿En qué horarios y días se puede visitar el parque ecoturístico Centro Ecoturistico El Nuevo Mundo - Estoracon?&lt;/b&gt;&lt;/h3&gt;
+                        &lt;p&gt;Los horarios oficiales del parque ecoturístico Centro Ecoturistico El Nuevo Mundo - Estoracon son los siguientes:&lt;/p&gt;                       
                             &lt;ul&gt;
                                 &lt;li&gt;Lunes de 10:00 a 19:00&lt;/li&gt;
                                 &lt;li&gt;Martes de 10:00 a 19:00&lt;/li&gt;
@@ -593,15 +599,14 @@
                                 &lt;li&gt;Sábado de 10:00 a 19:00&lt;/li&gt;
                                 &lt;li&gt;Domingo de 10:00 a 19:00&lt;/li&gt;
                             &lt;/ul&gt;
-                            &lt;p&gt;Antes de visitar el lugar, es una buena idea verificar sus sitios de contacto digitales y redes sociales, aún si ya cuentas con los horarios oficiales, para evitar cualquier cambio inesperado o sorpresas ya que estés ahí (por ej. cambio por días feriados)&lt;/p&gt;                 
-                    </v>
-      </c>
-      <c r="AA2" t="str" xml:space="preserve">
+                            &lt;p&gt;Antes de visitar el lugar, es importante revisar sus sitios digitales y redes sociales, así te aseguras de detectar cualquier cambio que hayan tenido de última hora por cuestiones de fechas especiales, vacaciones, temporadas altas, etc&lt;/p&gt;</v>
+      </c>
+      <c r="AB2" t="str" xml:space="preserve">
         <v xml:space="preserve">
                     &lt;img src="https://rumbonaturaleza.com/wp-content/uploads/2023/03/Centro_Ecoturistico_El_Nuevo_Mundo_-_Estoracon_0.jpg" alt="Centro Ecoturistico El Nuevo Mundo - Estoracon"&gt;                
                 </v>
       </c>
-      <c r="AB2" t="str">
+      <c r="AC2" t="str">
         <v>Añadir sitio web</v>
       </c>
     </row>
@@ -627,172 +632,61 @@
       <c r="G3" t="str">
         <v>Web no disponible</v>
       </c>
+      <c r="H3" t="str">
+        <v>No se cuenta con horario oficial</v>
+      </c>
       <c r="I3" t="str">
+        <v>No se cuenta con horario oficial</v>
+      </c>
+      <c r="J3" t="str">
         <v>Jitotol, Chiapas</v>
       </c>
-      <c r="J3" t="str">
+      <c r="K3" t="str">
         <v>Chiapas</v>
       </c>
-      <c r="K3" t="str">
+      <c r="L3" t="str">
         <v>https://www.google.com/maps/place/Siempre+Verde+Chiapas,+Centro+Ecotur%C3%ADstico/@17.143827,-92.888084,17z/data=!3m1!4b1!4m6!3m5!1s0x85ed0ee58c29248b:0xcdab59d265c14ddf!8m2!3d17.143827!4d-92.888084!16s%2Fg%2F11bvv4whms?authuser=0&amp;hl=es</v>
       </c>
-      <c r="L3" t="str">
-        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3812.5419796816677!2d-92.88808399999999!3d17.143826999999998!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x85ed0ee58c29248b%3A0xcdab59d265c14ddf!2sSiempre%20Verde%20Chiapas%2C%20Centro%20Ecotur%C3%ADstico!5e0!3m2!1ses!2smx!4v1679155880397!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
-      </c>
       <c r="M3" t="str">
+        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3812.5419796816677!2d-92.88808399999999!3d17.143826999999998!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x85ed0ee58c29248b%3A0xcdab59d265c14ddf!2sSiempre%20Verde%20Chiapas%2C%20Centro%20Ecotur%C3%ADstico!5e0!3m2!1ses!2smx!4v1679160012658!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
+      </c>
+      <c r="N3" t="str">
         <v>44V6+GQ Jitotol, Chiapas</v>
       </c>
-      <c r="N3" t="str">
+      <c r="O3" t="str">
         <v>4.4</v>
       </c>
-      <c r="O3" t="str">
+      <c r="P3" t="str">
         <v>555</v>
       </c>
-      <c r="P3" t="str">
+      <c r="Q3" t="str">
         <v>Hermoso lugar para realizar senderismo, manejar cuatrimotos y para pasar unos días de relajamiento, todo el lugar es magnifico, las cabañas con chimeneas y balcones enormes desde donde puedes admirar el bosque, el lugar cuenta con…,El lugar es espectacular para estar alejado de la ciudad. Descansar, delicioso clima. Cómodo y limpio. No esperes un lugar de lujo pero si un lugar acogedor.,Un lugar muy bello para pasar un fin de semana en familia, el clima súper agradable y la vegetación maravillosa. Amo mi chiapas</v>
       </c>
-      <c r="Q3" t="str">
+      <c r="R3" t="str">
         <v>https://lh5.googleusercontent.com/p/AF1QipPeHN3i2PWxhWxToRs-k5bKZZRwHphpyIy-yf-L=w426-h240-k-no</v>
       </c>
-      <c r="R3" t="str">
+      <c r="S3" t="str">
         <v>wget --no-check-certificate https://lh5.googleusercontent.com/p/AF1QipPeHN3i2PWxhWxToRs-k5bKZZRwHphpyIy-yf-L=w426-h240-k-no</v>
       </c>
-      <c r="S3" t="str">
+      <c r="T3" t="str">
         <v>AF1QipPeHN3i2PWxhWxToRs-k5bKZZRwHphpyIy-yf-L=w426-h240-k-no</v>
       </c>
-      <c r="T3" t="str">
+      <c r="U3" t="str">
         <v>Siempre_Verde_Chiapas,_Centro_Ecoturístico_1</v>
       </c>
-      <c r="U3" t="str">
+      <c r="V3" t="str">
         <v>Siempre_Verde_Chiapas,_Centro_Ecoturístico_1.jpg</v>
       </c>
-      <c r="V3" t="str">
+      <c r="W3" t="str">
         <v>https://rumbonaturaleza.com/wp-content/uploads/2023/03/Siempre_Verde_Chiapas,_Centro_Ecoturístico_1.jpg</v>
       </c>
-      <c r="W3" t="str">
+      <c r="X3" t="str">
         <v>ren "AF1QipPeHN3i2PWxhWxToRs-k5bKZZRwHphpyIy-yf-L=w426-h240-k-no" "Siempre_Verde_Chiapas,_Centro_Ecoturístico_1.jpg"</v>
       </c>
-      <c r="X3" t="str">
+      <c r="Y3" t="str">
         <v>parques-ecoturismo-en-chiapas</v>
       </c>
-      <c r="Y3" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-                    &lt;p&gt; ¿Estás buscando los mejores parques ecoturísticos en Chiapas? Entonces sin duda ¡estás en el lugar correcto!. Hoy en este artículo vamos a presentarte cuáles son los  parques ecoturísticos que han sido mejor evaluados en este estado. 
- Para poder definir esta listade los mejores, realizamos consultas en un montón de fuentes oficiales, redes sociales, rankings e incluso algunas entrevistas que nos permitieron determinar cuáles son y dónde se ubican los parques de ecoturismo que mejores experiencias han brindado a sus visitantes, y que mayor calificación han recibido en Chiapas durante los últimos años. 
- Con esta prueba social como respaldo, hoy te compartimos la lista de los parque ecológico mejor calificados en Chiapas en function getFullYear() { [native code] } junto con su ubicación, medios oficiales de contacto, horarios y cómo llegar hasta ellos; así como la calificación promedio con la que cuenta cada lugar. 
- Prepárate con esto y ¡a disfrutar del ecoturismo en Chiapas!&lt;/p&gt;                    
-                    </v>
-      </c>
       <c r="Z3" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-                    &lt;h2&gt;&lt;b&gt;Parque de Ecoturismo Siempre Verde Chiapas, Centro Ecoturístico&lt;/b&gt;&lt;/h2&gt;
-                        &lt;img src="https://rumbonaturaleza.com/wp-content/uploads/2023/03/Siempre_Verde_Chiapas,_Centro_Ecoturístico_1.jpg" alt="Siempre Verde Chiapas, Centro Ecoturístico"&gt;   
-                        &lt;div&gt;&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3812.5419796816677!2d-92.88808399999999!3d17.143826999999998!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x85ed0ee58c29248b%3A0xcdab59d265c14ddf!2sSiempre%20Verde%20Chiapas%2C%20Centro%20Ecotur%C3%ADstico!5e0!3m2!1ses!2smx!4v1679155880397!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;&lt;/div&gt;
-                        &lt;div&gt;&lt;/div&gt;
-                        &lt;p&gt;Si te apasiona la naturaleza y andas en busca de aventuras ¡pues no se diga más! porque sin duda el parque ecoturístico undefined es una opción en undefined que no debes dejar pasar. Este parque ecoturístico tiene una calificación promedio de undefined estrellas, basada en las opiniones de más de undefined visitantes, motivo por el que forma parte de este rank. Así es que... siendo uno de los parques ecoturísticos mejores calificados en undefined  ¿qué esperas para visitarlo?&lt;/p&gt;
-                        &lt;h3&gt;&lt;b&gt;¿Cómo llegar al Centro Ecoturístico "Siempre Verde Chiapas, Centro Ecoturístico"? &lt;/b&gt;&lt;/h3&gt;
-                            &lt;p&gt;Este parque de ecoturismo se ubica en Carretera Escopetazo Pichucalco Kilometro 81 S/N, El Campanario, 29760 Jitotol, Chis.
- Si necesitas ir a este sitio manejando puedes apoyarte poniendo la dirección en un navegador tipo waze o googleMaps o siguiendo directamente este &lt;a href='https://www.google.com/maps/place/Siempre+Verde+Chiapas,+Centro+Ecotur%C3%ADstico/@17.143827,-92.888084,17z/data=!3m1!4b1!4m6!3m5!1s0x85ed0ee58c29248b:0xcdab59d265c14ddf!8m2!3d17.143827!4d-92.888084!16s%2Fg%2F11bvv4whms?authuser=0&amp;hl=es'&gt;Mapa del Parque Natural Siempre Verde Chiapas, Centro Ecoturístico&lt;/a&gt;&lt;/p&gt;
-                        &lt;h3&gt;&lt;b&gt;¿Cuáles son los contactos del parque de ecoturismo Siempre Verde Chiapas, Centro Ecoturístico?&lt;/b&gt;&lt;/h3&gt;
-                            &lt;p&gt;Los contactos disponibles del Parque Ecoturístico Siempre Verde Chiapas, Centro Ecoturístico son: &lt;/p&gt;
-                            &lt;ul&gt;
-                                &lt;li&gt;&lt;b&gt;Teléfono:&lt;/b&gt;919 104 9970&lt;/li&gt;
-                                &lt;li&gt;&lt;b&gt;SitioWeb:&lt;/b&gt;web no disponible&lt;/li&gt;                                
-                            &lt;/ul&gt;
-                        &lt;h3&gt;&lt;b&gt;¿En qué horarios y días se puede visitar el parque ecoturístico Siempre Verde Chiapas, Centro Ecoturístico?&lt;/b&gt;&lt;/h3&gt;
-                            &lt;p&gt;Los horarios oficiales del parque ecoturístico Siempre Verde Chiapas, Centro Ecoturístico son los siguientes:&lt;/p&gt;                       
-                            &lt;ul&gt;
-                                &lt;li&gt;undefined&lt;/li&gt;
-                                &lt;li&gt;undefined&lt;/li&gt;
-                                &lt;li&gt;undefined&lt;/li&gt;
-                                &lt;li&gt;undefined&lt;/li&gt;
-                                &lt;li&gt;undefined&lt;/li&gt;
-                                &lt;li&gt;undefined&lt;/li&gt;
-                                &lt;li&gt;undefined&lt;/li&gt;
-                            &lt;/ul&gt;
-                            &lt;p&gt;A pesar de contar con horarios oficiales, te recomendamos siempre visitar sus sitios de contacto y redes oficiales antes de ir al lugar, así podrás identificar cualquier cambio extraordinario que hayan tenido.&lt;/p&gt;                 
-                    </v>
-      </c>
-      <c r="AA3" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-                    &lt;img src="https://rumbonaturaleza.com/wp-content/uploads/2023/03/Siempre_Verde_Chiapas,_Centro_Ecoturístico_1.jpg" alt="Siempre Verde Chiapas, Centro Ecoturístico"&gt;                
-                </v>
-      </c>
-      <c r="AB3" t="str">
-        <v>Añadir sitio web</v>
-      </c>
-    </row>
-    <row r="4" xml:space="preserve">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="str">
-        <v>Parque Ecoturistico Tzimbac</v>
-      </c>
-      <c r="C4" t="str">
-        <v>Parque Ecoturistico Tzimbac</v>
-      </c>
-      <c r="D4" t="str">
-        <v>parque ecoturistico tzimbac</v>
-      </c>
-      <c r="E4" t="str">
-        <v>Carretera a Monterrey Km. 2.2, Villarreal, 29125 Chis.</v>
-      </c>
-      <c r="F4" t="str">
-        <v>961 286 8575</v>
-      </c>
-      <c r="G4" t="str">
-        <v>Web no disponible</v>
-      </c>
-      <c r="I4" t="str">
-        <v>Santa Rita, Chiapas</v>
-      </c>
-      <c r="J4" t="str">
-        <v>Chiapas</v>
-      </c>
-      <c r="K4" t="str">
-        <v>https://www.google.com/maps/place/Parque+Ecoturistico+Tzimbac/@16.8998672,-93.2289146,17z/data=!3m1!4b1!4m6!3m5!1s0x85ece790120fdba7:0xf3cf8d4d73cd7595!8m2!3d16.8998672!4d-93.2289146!16s%2Fg%2F12hm176_z?authuser=0&amp;hl=es</v>
-      </c>
-      <c r="L4" t="str">
-        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3817.515055110652!2d-93.2289146!3d16.8998672!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x85ece790120fdba7%3A0xf3cf8d4d73cd7595!2sParque%20Ecoturistico%20Tzimbac!5e0!3m2!1ses!2smx!4v1679155885639!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
-      </c>
-      <c r="M4" t="str">
-        <v>VQXC+WC Santa Rita, Chiapas</v>
-      </c>
-      <c r="N4" t="str">
-        <v>4.2</v>
-      </c>
-      <c r="O4" t="str">
-        <v>46</v>
-      </c>
-      <c r="P4" t="str">
-        <v>Si te gusta la naturaleza visítalo, si esperas muchas comodidades no es un sitio para ti. No hay señal, los baños están módicamente cómodos (si vas a la naturaleza no esperes lujos), hay área para acampar, muy limpio. Fuimos y nos tocó…,Buen lugar para descansar y rejarte un rato, sin embargo podría mejorar en muchos detalles, porque en época de lluvia es imposible disfrutar de la naturaleza, tener más sanitarios o en áreas más comunes.,Exelente lugar para ir con la familia y amigos. Podras acampar, explorar, senderismo, rappel, tirolesa, montar a caballo. Todo esto rodeo de magia y naturaleza respirando aire puro, fuera de la cantaminacion de la ciudad; puedes realozar…</v>
-      </c>
-      <c r="Q4" t="str">
-        <v>https://lh5.googleusercontent.com/p/AF1QipNYYHKIZRIqOhYXADcr3o_zu4-ho3SpnynhRZrw=w408-h306-k-no</v>
-      </c>
-      <c r="R4" t="str">
-        <v>wget --no-check-certificate https://lh5.googleusercontent.com/p/AF1QipNYYHKIZRIqOhYXADcr3o_zu4-ho3SpnynhRZrw=w408-h306-k-no</v>
-      </c>
-      <c r="S4" t="str">
-        <v>AF1QipNYYHKIZRIqOhYXADcr3o_zu4-ho3SpnynhRZrw=w408-h306-k-no</v>
-      </c>
-      <c r="T4" t="str">
-        <v>Parque_Ecoturistico_Tzimbac_2</v>
-      </c>
-      <c r="U4" t="str">
-        <v>Parque_Ecoturistico_Tzimbac_2.jpg</v>
-      </c>
-      <c r="V4" t="str">
-        <v>https://rumbonaturaleza.com/wp-content/uploads/2023/03/Parque_Ecoturistico_Tzimbac_2.jpg</v>
-      </c>
-      <c r="W4" t="str">
-        <v>ren "AF1QipNYYHKIZRIqOhYXADcr3o_zu4-ho3SpnynhRZrw=w408-h306-k-no" "Parque_Ecoturistico_Tzimbac_2.jpg"</v>
-      </c>
-      <c r="X4" t="str">
-        <v>parques-ecoturismo-en-chiapas</v>
-      </c>
-      <c r="Y4" t="str" xml:space="preserve">
         <v xml:space="preserve">
                     &lt;p&gt; ¿Estás buscando los mejores parques ecoturísticos en Chiapas? Entonces sin duda ¡estás en el lugar correcto!. Hoy en este artículo vamos a presentarte cuáles son los  parques ecoturísticos que han sido mejor evaluados en este estado. 
  Para poder definir esta listade los mejores, realizamos consultas en un montón de fuentes oficiales, redes sociales, rankings e incluso algunas entrevistas que nos permitieron determinar cuáles son y dónde se ubican los parques ecoturísticos que mejores experiencias han brindado a sus visitantes, y que mayor calificación han recibido en Chiapas durante los últimos años. 
@@ -800,48 +694,151 @@
  Prepárate con esto y ¡a disfrutar del ecoturismo en Chiapas!&lt;/p&gt;                    
                     </v>
       </c>
+      <c r="AA3" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+                    &lt;h2&gt;&lt;b&gt;Centro de Ecoturismo Siempre Verde Chiapas, Centro Ecoturístico&lt;/b&gt;&lt;/h2&gt;
+                        &lt;img src="https://rumbonaturaleza.com/wp-content/uploads/2023/03/Siempre_Verde_Chiapas,_Centro_Ecoturístico_1.jpg" alt="Siempre Verde Chiapas, Centro Ecoturístico"&gt;   
+                        &lt;div&gt;&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3812.5419796816677!2d-92.88808399999999!3d17.143826999999998!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x85ed0ee58c29248b%3A0xcdab59d265c14ddf!2sSiempre%20Verde%20Chiapas%2C%20Centro%20Ecotur%C3%ADstico!5e0!3m2!1ses!2smx!4v1679160012658!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;&lt;/div&gt;
+                        &lt;div&gt;&lt;/div&gt;
+                        &lt;p&gt;El parque ecoturístico undefined es una opción fantástica para tener una aventura natural en undefined. Su calificación promedio es de undefined estrellas respaldada por más de undefined visitantes, así que no tenemos duda de que este lugar pertenece a la lista de los parques ecoturísticos mejor rankeados de de undefined y que se trata de uno de los principales atractivos naturales en la región. Así que ya sabes... ¿ganas de naturaleza?... pues entonces el parque natural undefined es una grandísima opción&lt;/p&gt;
+                        &lt;h3&gt;&lt;b&gt;¿Cómo llegar al Sitio Ecoturístico "Siempre Verde Chiapas, Centro Ecoturístico"? &lt;/b&gt;&lt;/h3&gt;
+                            &lt;p&gt;Este parque natural se ubica en Carretera Escopetazo Pichucalco Kilometro 81 S/N, El Campanario, 29760 Jitotol, Chis.
+ Si necesitas ir a este sitio manejando puedes apoyarte poniendo la dirección en un navegador tipo waze o googleMaps o siguiendo directamente este &lt;a href='https://www.google.com/maps/place/Siempre+Verde+Chiapas,+Centro+Ecotur%C3%ADstico/@17.143827,-92.888084,17z/data=!3m1!4b1!4m6!3m5!1s0x85ed0ee58c29248b:0xcdab59d265c14ddf!8m2!3d17.143827!4d-92.888084!16s%2Fg%2F11bvv4whms?authuser=0&amp;hl=es'&gt;Mapa del Parque Ecoturístico Siempre Verde Chiapas, Centro Ecoturístico&lt;/a&gt;&lt;/p&gt;
+                        &lt;h3&gt;&lt;b&gt;¿Cuáles son los contactos del parque de ecoturismo Siempre Verde Chiapas, Centro Ecoturístico?&lt;/b&gt;&lt;/h3&gt;
+                            &lt;p&gt;Los contactos disponibles del Centro Ecoturístico Siempre Verde Chiapas, Centro Ecoturístico son: &lt;/p&gt;
+                            &lt;ul&gt;
+                                &lt;li&gt;&lt;b&gt;Teléfono:&lt;/b&gt;919 104 9970&lt;/li&gt;
+                                &lt;li&gt;&lt;b&gt;SitioWeb:&lt;/b&gt;web no disponible&lt;/li&gt;                                
+                            &lt;/ul&gt;
+                        &lt;h3&gt;&lt;b&gt;¿En qué horarios y días se puede visitar el centro ecoturístico Siempre Verde Chiapas, Centro Ecoturístico?&lt;/b&gt;&lt;/h3&gt;
+                        &lt;p&gt; Lamentablemente este sitio no cuenta con horarios publicados oficialmente, posiblemente debido a que existen variaciones frecuentes en sus horarios de operación. 
+ Por este motivo, te recomendamos consultar sus sitios oficiales en una fecha cercana a tu visita o contactarlos directamente para pedir la actualización más reciente de sus días y horas de operación.</v>
+      </c>
+      <c r="AB3" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+                    &lt;img src="https://rumbonaturaleza.com/wp-content/uploads/2023/03/Siempre_Verde_Chiapas,_Centro_Ecoturístico_1.jpg" alt="Siempre Verde Chiapas, Centro Ecoturístico"&gt;                
+                </v>
+      </c>
+      <c r="AC3" t="str">
+        <v>Añadir sitio web</v>
+      </c>
+    </row>
+    <row r="4" xml:space="preserve">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Parque Ecoturistico Tzimbac</v>
+      </c>
+      <c r="C4" t="str">
+        <v>Parque Ecoturistico Tzimbac</v>
+      </c>
+      <c r="D4" t="str">
+        <v>parque ecoturistico tzimbac</v>
+      </c>
+      <c r="E4" t="str">
+        <v>Carretera a Monterrey Km. 2.2, Villarreal, 29125 Chis.</v>
+      </c>
+      <c r="F4" t="str">
+        <v>961 286 8575</v>
+      </c>
+      <c r="G4" t="str">
+        <v>Web no disponible</v>
+      </c>
+      <c r="H4" t="str">
+        <v>No se cuenta con horario oficial</v>
+      </c>
+      <c r="I4" t="str">
+        <v>No se cuenta con horario oficial</v>
+      </c>
+      <c r="J4" t="str">
+        <v>Santa Rita, Chiapas</v>
+      </c>
+      <c r="K4" t="str">
+        <v>Chiapas</v>
+      </c>
+      <c r="L4" t="str">
+        <v>https://www.google.com/maps/place/Parque+Ecoturistico+Tzimbac/@16.8998672,-93.2289146,17z/data=!3m1!4b1!4m6!3m5!1s0x85ece790120fdba7:0xf3cf8d4d73cd7595!8m2!3d16.8998672!4d-93.2289146!16s%2Fg%2F12hm176_z?authuser=0&amp;hl=es</v>
+      </c>
+      <c r="M4" t="str">
+        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3817.515055110652!2d-93.2289146!3d16.8998672!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x85ece790120fdba7%3A0xf3cf8d4d73cd7595!2sParque%20Ecoturistico%20Tzimbac!5e0!3m2!1ses!2smx!4v1679160017598!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
+      </c>
+      <c r="N4" t="str">
+        <v>VQXC+WC Santa Rita, Chiapas</v>
+      </c>
+      <c r="O4" t="str">
+        <v>4.2</v>
+      </c>
+      <c r="P4" t="str">
+        <v>46</v>
+      </c>
+      <c r="Q4" t="str">
+        <v>Si te gusta la naturaleza visítalo, si esperas muchas comodidades no es un sitio para ti. No hay señal, los baños están módicamente cómodos (si vas a la naturaleza no esperes lujos), hay área para acampar, muy limpio. Fuimos y nos tocó…,Buen lugar para descansar y rejarte un rato, sin embargo podría mejorar en muchos detalles, porque en época de lluvia es imposible disfrutar de la naturaleza, tener más sanitarios o en áreas más comunes.,Exelente lugar para ir con la familia y amigos. Podras acampar, explorar, senderismo, rappel, tirolesa, montar a caballo. Todo esto rodeo de magia y naturaleza respirando aire puro, fuera de la cantaminacion de la ciudad; puedes realozar…</v>
+      </c>
+      <c r="R4" t="str">
+        <v>https://lh5.googleusercontent.com/p/AF1QipNYYHKIZRIqOhYXADcr3o_zu4-ho3SpnynhRZrw=w408-h306-k-no</v>
+      </c>
+      <c r="S4" t="str">
+        <v>wget --no-check-certificate https://lh5.googleusercontent.com/p/AF1QipNYYHKIZRIqOhYXADcr3o_zu4-ho3SpnynhRZrw=w408-h306-k-no</v>
+      </c>
+      <c r="T4" t="str">
+        <v>AF1QipNYYHKIZRIqOhYXADcr3o_zu4-ho3SpnynhRZrw=w408-h306-k-no</v>
+      </c>
+      <c r="U4" t="str">
+        <v>Parque_Ecoturistico_Tzimbac_2</v>
+      </c>
+      <c r="V4" t="str">
+        <v>Parque_Ecoturistico_Tzimbac_2.jpg</v>
+      </c>
+      <c r="W4" t="str">
+        <v>https://rumbonaturaleza.com/wp-content/uploads/2023/03/Parque_Ecoturistico_Tzimbac_2.jpg</v>
+      </c>
+      <c r="X4" t="str">
+        <v>ren "AF1QipNYYHKIZRIqOhYXADcr3o_zu4-ho3SpnynhRZrw=w408-h306-k-no" "Parque_Ecoturistico_Tzimbac_2.jpg"</v>
+      </c>
+      <c r="Y4" t="str">
+        <v>parques-ecoturismo-en-chiapas</v>
+      </c>
       <c r="Z4" t="str" xml:space="preserve">
         <v xml:space="preserve">
-                    &lt;h2&gt;&lt;b&gt;Centro Ecoturístico Parque Ecoturistico Tzimbac&lt;/b&gt;&lt;/h2&gt;
+                    &lt;p&gt; ¿Estás buscando los mejores parques ecoturísticos en Chiapas? Entonces sin duda ¡estás en el lugar correcto!. Hoy en este artículo vamos a presentarte cuáles son los  parques ecológicos que han sido mejor evaluados en este estado. 
+ Para poder definir esta listade los mejores, realizamos consultas en un montón de fuentes oficiales, redes sociales, rankings e incluso algunas entrevistas que nos permitieron determinar cuáles son y dónde se ubican los parques naturales que mejores experiencias han brindado a sus visitantes, y que mayor calificación han recibido en Chiapas durante los últimos años. 
+ Con esta prueba social como respaldo, hoy te compartimos la lista de los parque ecoturístico mejor calificados en Chiapas en function getFullYear() { [native code] } junto con su ubicación, medios oficiales de contacto, horarios y cómo llegar hasta ellos; así como la calificación promedio con la que cuenta cada lugar. 
+ Prepárate con esto y ¡a disfrutar del ecoturismo en Chiapas!&lt;/p&gt;                    
+                    </v>
+      </c>
+      <c r="AA4" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+                    &lt;h2&gt;&lt;b&gt;Parque Ecoturístico Parque Ecoturistico Tzimbac&lt;/b&gt;&lt;/h2&gt;
                         &lt;img src="https://rumbonaturaleza.com/wp-content/uploads/2023/03/Parque_Ecoturistico_Tzimbac_2.jpg" alt="Parque Ecoturistico Tzimbac"&gt;   
-                        &lt;div&gt;&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3817.515055110652!2d-93.2289146!3d16.8998672!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x85ece790120fdba7%3A0xf3cf8d4d73cd7595!2sParque%20Ecoturistico%20Tzimbac!5e0!3m2!1ses!2smx!4v1679155885639!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;&lt;/div&gt;
+                        &lt;div&gt;&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3817.515055110652!2d-93.2289146!3d16.8998672!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x85ece790120fdba7%3A0xf3cf8d4d73cd7595!2sParque%20Ecoturistico%20Tzimbac!5e0!3m2!1ses!2smx!4v1679160017598!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;&lt;/div&gt;
                         &lt;div&gt;&lt;/div&gt;
-                        &lt;p&gt;Este sitio ecoturístico tiene undefined estrellas de calificación promedio, a partir de las más de undefined opiniones de sus visitantes... ¿nada mal no?. Es por esto que undefined es parte de esta lista de los parques naturales mejor calificados de undefined. Con este respaldo estamos más que seguras(os) que se trata  de un sitio que vas a disfrutar al Máximo. Así que ya sabes, si lo que buscas es naturaleza, el parque ecoturístico undefined en undefined es sin duda una gran opción&lt;/p&gt;
-                        &lt;h3&gt;&lt;b&gt;¿Cómo llegar al Centro Ecoturístico "Parque Ecoturistico Tzimbac"? &lt;/b&gt;&lt;/h3&gt;
-                            &lt;p&gt;Este centro ecoturístico se ubica en Carretera a Monterrey Km. 2.2, Villarreal, 29125 Chis.
- Para llegar a este lugar, simplemente ingresa la dirección en una app de navegación o utiliza este enlace al&lt;a href='https://www.google.com/maps/place/Parque+Ecoturistico+Tzimbac/@16.8998672,-93.2289146,17z/data=!3m1!4b1!4m6!3m5!1s0x85ece790120fdba7:0xf3cf8d4d73cd7595!8m2!3d16.8998672!4d-93.2289146!16s%2Fg%2F12hm176_z?authuser=0&amp;hl=es'&gt;Mapa del Parque Ecoturístico Parque Ecoturistico Tzimbac&lt;/a&gt;&lt;/p&gt;
-                        &lt;h3&gt;&lt;b&gt;¿Cuáles son los contactos del centro de ecoturismo Parque Ecoturistico Tzimbac?&lt;/b&gt;&lt;/h3&gt;
+                        &lt;p&gt;Si estás en undefined en búsqueda de algo de ecoturismo y aventura entonces el parque ecoturístico undefined no se te puede escapar. Hemos decidido incluir este parque ecoturístico en esta lista de los mejores de undefined gracias al respaldo y opiniones de más de undefined visitantes que lo han evaluado públicamente por lo menos con undefined estrellas de calificación (de las más altas para este estado del país). Así que chécate todos lo detalles necesarios para tu visita y ¡no se diga más! ¡a vivir el ecoturismo en undefined en undefined!&lt;/p&gt;
+                        &lt;h3&gt;&lt;b&gt;¿Cómo llegar al Parque Ecoturístico "Parque Ecoturistico Tzimbac"? &lt;/b&gt;&lt;/h3&gt;
+                            &lt;p&gt;Este sitio ecoturístico se ubica en Carretera a Monterrey Km. 2.2, Villarreal, 29125 Chis.
+ Para llegar a este parque, simplemente sigue las indicaciones de tu aplicación de navegación preferida o utiliza este link al &lt;a href='https://www.google.com/maps/place/Parque+Ecoturistico+Tzimbac/@16.8998672,-93.2289146,17z/data=!3m1!4b1!4m6!3m5!1s0x85ece790120fdba7:0xf3cf8d4d73cd7595!8m2!3d16.8998672!4d-93.2289146!16s%2Fg%2F12hm176_z?authuser=0&amp;hl=es'&gt;Mapa del Parque Ecoturístico Parque Ecoturistico Tzimbac&lt;/a&gt;&lt;/p&gt;
+                        &lt;h3&gt;&lt;b&gt;¿Cuáles son los contactos del parque ecoturístico Parque Ecoturistico Tzimbac?&lt;/b&gt;&lt;/h3&gt;
                             &lt;p&gt;Los contactos disponibles del Centro Ecoturístico Parque Ecoturistico Tzimbac son: &lt;/p&gt;
                             &lt;ul&gt;
                                 &lt;li&gt;&lt;b&gt;Teléfono:&lt;/b&gt;961 286 8575&lt;/li&gt;
                                 &lt;li&gt;&lt;b&gt;SitioWeb:&lt;/b&gt;web no disponible&lt;/li&gt;                                
                             &lt;/ul&gt;
-                        &lt;h3&gt;&lt;b&gt;¿En qué horarios y días se puede visitar el sitio ecoturístico Parque Ecoturistico Tzimbac?&lt;/b&gt;&lt;/h3&gt;
-                            &lt;p&gt;Los horarios oficiales del centro de ecoturismo Parque Ecoturistico Tzimbac son los siguientes:&lt;/p&gt;                       
-                            &lt;ul&gt;
-                                &lt;li&gt;undefined&lt;/li&gt;
-                                &lt;li&gt;undefined&lt;/li&gt;
-                                &lt;li&gt;undefined&lt;/li&gt;
-                                &lt;li&gt;undefined&lt;/li&gt;
-                                &lt;li&gt;undefined&lt;/li&gt;
-                                &lt;li&gt;undefined&lt;/li&gt;
-                                &lt;li&gt;undefined&lt;/li&gt;
-                            &lt;/ul&gt;
-                            &lt;p&gt;A pesar de que los horarios sean oficiales, es buena idea que antes ir, revises siempre cómo están las cosas en sus redes sociales y contactos digitales, esto te permitirá asegurarte de que no haya cambios de horario o logística antes de tu arribo al lugar&lt;/p&gt;                 
-                    </v>
-      </c>
-      <c r="AA4" t="str" xml:space="preserve">
+                        &lt;h3&gt;&lt;b&gt;¿En qué horarios y días se puede visitar el parque natural Parque Ecoturistico Tzimbac?&lt;/b&gt;&lt;/h3&gt;
+                        &lt;p&gt; Lamentablemente este sitio no cuenta con horarios publicados oficialmente, posiblemente debido a que existen variaciones frecuentes en sus horarios de operación. 
+ Por este motivo, te recomendamos consultar sus sitios oficiales en una fecha cercana a tu visita o contactarlos directamente para pedir la actualización más reciente de sus días y horas de operación.</v>
+      </c>
+      <c r="AB4" t="str" xml:space="preserve">
         <v xml:space="preserve">
                     &lt;img src="https://rumbonaturaleza.com/wp-content/uploads/2023/03/Parque_Ecoturistico_Tzimbac_2.jpg" alt="Parque Ecoturistico Tzimbac"&gt;                
                 </v>
       </c>
-      <c r="AB4" t="str">
+      <c r="AC4" t="str">
         <v>Añadir sitio web</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:AB4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:AC4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
WIP_Creación de script para maquilacion de proceso offchain (download xls, upload de top15xls y creacion de objeto final para allImports)
</commit_message>
<xml_diff>
--- a/testingAllImports.xlsx
+++ b/testingAllImports.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC4"/>
+  <dimension ref="A1:AG4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -479,158 +479,131 @@
         <v>slug</v>
       </c>
       <c r="Z1" t="str">
-        <v>articleIntro</v>
+        <v>missingData</v>
       </c>
       <c r="AA1" t="str">
-        <v>structuredData</v>
+        <v>horarioLunes</v>
       </c>
       <c r="AB1" t="str">
-        <v>photoLocal</v>
+        <v>horarioMartes</v>
       </c>
       <c r="AC1" t="str">
-        <v>missingData</v>
+        <v>horarioMiercoles</v>
+      </c>
+      <c r="AD1" t="str">
+        <v>horarioJueves</v>
+      </c>
+      <c r="AE1" t="str">
+        <v>horarioViernes</v>
+      </c>
+      <c r="AF1" t="str">
+        <v>horarioSabado</v>
+      </c>
+      <c r="AG1" t="str">
+        <v>horarioDomingo</v>
       </c>
     </row>
-    <row r="2" xml:space="preserve">
+    <row r="2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="str">
-        <v>Centro Ecoturistico El Nuevo Mundo - Estoracon</v>
+        <v>Cissus Hotel Boutique</v>
       </c>
       <c r="C2" t="str">
-        <v>Centro Ecoturistico El Nuevo Mundo - Estoracon</v>
+        <v>Cissus Hotel Boutique</v>
       </c>
       <c r="D2" t="str">
-        <v>centro ecoturistico el nuevo mundo - estoracon</v>
+        <v>cissus hotel boutique</v>
       </c>
       <c r="E2" t="str">
-        <v>Carretera Sayula S/N, Francisco I. Madero, 30400 Cintalapa, Chis.</v>
+        <v>6a Calle Poniente 41, Antigua Guatemala 03001, Guatemala</v>
       </c>
       <c r="F2" t="str">
-        <v>961 284 4705</v>
+        <v>+502 7832 7938</v>
       </c>
       <c r="G2" t="str">
-        <v>Web no disponible</v>
+        <v>http://cissushotel.com/contact.htm</v>
+      </c>
+      <c r="H2" t="str">
+        <v>No se cuenta con horario oficial</v>
       </c>
       <c r="I2" t="str">
-        <v>Sábado de 10:00 a 19:00,Domingo de 10:00 a 19:00,Lunes de 10:00 a 19:00,Martes de 10:00 a 19:00,Miércoles de 10:00 a 19:00,Jueves de 10:00 a 19:00,Viernes de 10:00 a 19:00</v>
+        <v>No se cuenta con horario oficial</v>
       </c>
       <c r="J2" t="str">
-        <v>Estoracón, Chiapas</v>
+        <v>Antigua Guatemala, Guatemala</v>
       </c>
       <c r="K2" t="str">
         <v>Chiapas</v>
       </c>
       <c r="L2" t="str">
-        <v>https://www.google.com/maps/place/Centro+Ecoturistico+El+Nuevo+Mundo+-+Estoracon/@16.8505798,-93.7933739,17z/data=!3m1!4b1!4m6!3m5!1s0x85eca6200d7617bb:0x7498371825377da6!8m2!3d16.8505798!4d-93.7933739!16s%2Fg%2F11dxpchfty?authuser=0&amp;hl=es</v>
+        <v>https://www.google.com/maps/place/Cissus+Hotel+Boutique/@14.5550625,-90.7367743,17z/data=!3m1!4b1!4m9!3m8!1s0x85890e0da9ac8f23:0xfa13c2f77ffda111!5m2!4m1!1i2!8m2!3d14.5550625!4d-90.7367743!16s%2Fg%2F1x5qt333?authuser=0&amp;hl=es</v>
       </c>
       <c r="M2" t="str">
-        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3818.5113687598837!2d-93.79337389999999!3d16.8505798!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x85eca6200d7617bb%3A0x7498371825377da6!2sCentro%20Ecoturistico%20El%20Nuevo%20Mundo%20-%20Estoracon!5e0!3m2!1ses!2smx!4v1679160007861!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
+        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3861.7713760208194!2d-90.7367743!3d14.5550625!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x85890e0da9ac8f23%3A0xfa13c2f77ffda111!2sCissus%20Hotel%20Boutique!5e0!3m2!1ses!2smx!4v1679356385475!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
       </c>
       <c r="N2" t="str">
-        <v>V624+6M Estoracón, Chiapas</v>
+        <v>H747+27 Antigua Guatemala, Guatemala</v>
       </c>
       <c r="O2" t="str">
-        <v>4.5</v>
+        <v>0.0</v>
       </c>
       <c r="P2" t="str">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="Q2" t="str">
-        <v>Hermoso día de excursión en familia a este sitio remoto con 4 cascadas en plena naturaleza con piscina y una comida riquísima con buena atención, los Tucanes con muchi acercamiento, salimos de Cintalapa Chiapas,Muy bonita reserva recomendable,Se puede acampar ($180 por tienda de campaña), hay cabañas (sencilla $400, doble $800), rentan hamacas, tienda de campaña, venden refrescos, cervezas, sabritas, buena comida(camarones empanizado, en ensalada , mojarras, carne asada, pollo,…</v>
+        <v>no hay opiniones</v>
       </c>
       <c r="R2" t="str">
-        <v>https://lh5.googleusercontent.com/p/AF1QipPOgfBL_SMdx6bZCZHeZCe150jGe-GqwXaX7lE=w408-h306-k-no</v>
+        <v>https://lh3.googleusercontent.com/gps-proxy/ALm4wwk3xkUshr8k33AOb87SS2U8vY-xgum2k-aTyRpdHOZ86C2pvPVGUC1IDtcfUFT5iemKTdvVyI5bhNQDs9ZlL6OXC5XkEa1HlEWst2JOZOJ1qOw__lmzs9lvJp-jHdrIJK2RLDghJOmcCy-t-boSoU26t7tW8tfDJGyG9ZCa_U8-9wedBh1pN0kd=w437-h240-k-no</v>
       </c>
       <c r="S2" t="str">
-        <v>wget --no-check-certificate https://lh5.googleusercontent.com/p/AF1QipPOgfBL_SMdx6bZCZHeZCe150jGe-GqwXaX7lE=w408-h306-k-no</v>
+        <v>wget --no-check-certificate https://lh3.googleusercontent.com/gps-proxy/ALm4wwk3xkUshr8k33AOb87SS2U8vY-xgum2k-aTyRpdHOZ86C2pvPVGUC1IDtcfUFT5iemKTdvVyI5bhNQDs9ZlL6OXC5XkEa1HlEWst2JOZOJ1qOw__lmzs9lvJp-jHdrIJK2RLDghJOmcCy-t-boSoU26t7tW8tfDJGyG9ZCa_U8-9wedBh1pN0kd=w437-h240-k-no</v>
       </c>
       <c r="T2" t="str">
-        <v>AF1QipPOgfBL_SMdx6bZCZHeZCe150jGe-GqwXaX7lE=w408-h306-k-no</v>
+        <v>ALm4wwk3xkUshr8k33AOb87SS2U8vY-xgum2k-aTyRpdHOZ86C2pvPVGUC1IDtcfUFT5iemKTdvVyI5bhNQDs9ZlL6OXC5XkEa1HlEWst2JOZOJ1qOw__lmzs9lvJp-jHdrIJK2RLDghJOmcCy-t-boSoU26t7tW8tfDJGyG9ZCa_U8-9wedBh1pN0kd=w437-h240-k-no</v>
       </c>
       <c r="U2" t="str">
-        <v>Centro_Ecoturistico_El_Nuevo_Mundo_-_Estoracon_0</v>
+        <v>Cissus_Hotel_Boutique_0</v>
       </c>
       <c r="V2" t="str">
-        <v>Centro_Ecoturistico_El_Nuevo_Mundo_-_Estoracon_0.jpg</v>
+        <v>Cissus_Hotel_Boutique_0.jpg</v>
       </c>
       <c r="W2" t="str">
-        <v>https://rumbonaturaleza.com/wp-content/uploads/2023/03/Centro_Ecoturistico_El_Nuevo_Mundo_-_Estoracon_0.jpg</v>
+        <v>https://rumbonaturaleza.com/wp-content/uploads/2023/03/Cissus_Hotel_Boutique_0.jpg</v>
       </c>
       <c r="X2" t="str">
-        <v>ren "AF1QipPOgfBL_SMdx6bZCZHeZCe150jGe-GqwXaX7lE=w408-h306-k-no" "Centro_Ecoturistico_El_Nuevo_Mundo_-_Estoracon_0.jpg"</v>
+        <v>ren "ALm4wwk3xkUshr8k33AOb87SS2U8vY-xgum2k-aTyRpdHOZ86C2pvPVGUC1IDtcfUFT5iemKTdvVyI5bhNQDs9ZlL6OXC5XkEa1HlEWst2JOZOJ1qOw__lmzs9lvJp-jHdrIJK2RLDghJOmcCy-t-boSoU26t7tW8tfDJGyG9ZCa_U8-9wedBh1pN0kd=w437-h240-k-no" "Cissus_Hotel_Boutique_0.jpg"</v>
       </c>
       <c r="Y2" t="str">
         <v>parques-ecoturismo-en-chiapas</v>
       </c>
-      <c r="Z2" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-                    &lt;p&gt; ¿Estás buscando los mejores parques ecoturísticos en Chiapas? Entonces sin duda ¡estás en el lugar correcto!. Hoy en este artículo vamos a presentarte cuáles son los  centros de ecoturismo que han sido mejor evaluados en este estado. 
- Para poder definir esta listade los mejores, realizamos consultas en un montón de fuentes oficiales, redes sociales, rankings e incluso algunas entrevistas que nos permitieron determinar cuáles son y dónde se ubican los centros ecoturísticos que mejores experiencias han brindado a sus visitantes, y que mayor calificación han recibido en Chiapas durante los últimos años. 
- Con esta prueba social como respaldo, hoy te compartimos la lista de los parque natural mejor calificados en Chiapas en function getFullYear() { [native code] } junto con su ubicación, medios oficiales de contacto, horarios y cómo llegar hasta ellos; así como la calificación promedio con la que cuenta cada lugar. 
- Prepárate con esto y ¡a disfrutar del ecoturismo en Chiapas!&lt;/p&gt;                    
-                    </v>
-      </c>
-      <c r="AA2" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-                    &lt;h2&gt;&lt;b&gt;Parque Ecoturístico Centro Ecoturistico El Nuevo Mundo - Estoracon&lt;/b&gt;&lt;/h2&gt;
-                        &lt;img src="https://rumbonaturaleza.com/wp-content/uploads/2023/03/Centro_Ecoturistico_El_Nuevo_Mundo_-_Estoracon_0.jpg" alt="Centro Ecoturistico El Nuevo Mundo - Estoracon"&gt;   
-                        &lt;div&gt;&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3818.5113687598837!2d-93.79337389999999!3d16.8505798!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x85eca6200d7617bb%3A0x7498371825377da6!2sCentro%20Ecoturistico%20El%20Nuevo%20Mundo%20-%20Estoracon!5e0!3m2!1ses!2smx!4v1679160007861!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;&lt;/div&gt;
-                        &lt;div&gt;&lt;/div&gt;
-                        &lt;p&gt;¿Quieres vivir un paseo increible en contacto con la naturaleza? entonces no puedes dejar de considerar una visita al centro de ecoturismo undefined en undefined. Con una calificación promedio de undefined estrellas y más de undefined opiniones de visitantes, este lugar es una de las mejores opciones para los amantes del ecoturismo en esta región. Así es que ¡toma nota  de todo lo requerido para tu visita a continuación!&lt;/p&gt;
-                        &lt;h3&gt;&lt;b&gt;¿Cómo llegar al Parque Natural "Centro Ecoturistico El Nuevo Mundo - Estoracon"? &lt;/b&gt;&lt;/h3&gt;
-                            &lt;p&gt;Este parque ecoturístico se ubica en Carretera Sayula S/N, Francisco I. Madero, 30400 Cintalapa, Chis.
- La verdad es que llegar a este Centro no tiene gran dificultad. Puedes encontrar la dirección de un lugar siguiendo cualquier aplicación de navegación que se te facilite o siguiendo esta liga al &lt;a href='https://www.google.com/maps/place/Centro+Ecoturistico+El+Nuevo+Mundo+-+Estoracon/@16.8505798,-93.7933739,17z/data=!3m1!4b1!4m6!3m5!1s0x85eca6200d7617bb:0x7498371825377da6!8m2!3d16.8505798!4d-93.7933739!16s%2Fg%2F11dxpchfty?authuser=0&amp;hl=es'&gt;Mapa del Parque Ecoturístico Centro Ecoturistico El Nuevo Mundo - Estoracon&lt;/a&gt;&lt;/p&gt;
-                        &lt;h3&gt;&lt;b&gt;¿Cuáles son los contactos del parque ecoturístico Centro Ecoturistico El Nuevo Mundo - Estoracon?&lt;/b&gt;&lt;/h3&gt;
-                            &lt;p&gt;Los contactos disponibles del Parque de Ecoturismo Centro Ecoturistico El Nuevo Mundo - Estoracon son: &lt;/p&gt;
-                            &lt;ul&gt;
-                                &lt;li&gt;&lt;b&gt;Teléfono:&lt;/b&gt;961 284 4705&lt;/li&gt;
-                                &lt;li&gt;&lt;b&gt;SitioWeb:&lt;/b&gt;web no disponible&lt;/li&gt;                                
-                            &lt;/ul&gt;
-                        &lt;h3&gt;&lt;b&gt;¿En qué horarios y días se puede visitar el parque ecoturístico Centro Ecoturistico El Nuevo Mundo - Estoracon?&lt;/b&gt;&lt;/h3&gt;
-                        &lt;p&gt;Los horarios oficiales del parque ecoturístico Centro Ecoturistico El Nuevo Mundo - Estoracon son los siguientes:&lt;/p&gt;                       
-                            &lt;ul&gt;
-                                &lt;li&gt;Lunes de 10:00 a 19:00&lt;/li&gt;
-                                &lt;li&gt;Martes de 10:00 a 19:00&lt;/li&gt;
-                                &lt;li&gt;Miércoles de 10:00 a 19:00&lt;/li&gt;
-                                &lt;li&gt;Jueves de 10:00 a 19:00&lt;/li&gt;
-                                &lt;li&gt;Viernes de 10:00 a 19:00&lt;/li&gt;
-                                &lt;li&gt;Sábado de 10:00 a 19:00&lt;/li&gt;
-                                &lt;li&gt;Domingo de 10:00 a 19:00&lt;/li&gt;
-                            &lt;/ul&gt;
-                            &lt;p&gt;Antes de visitar el lugar, es importante revisar sus sitios digitales y redes sociales, así te aseguras de detectar cualquier cambio que hayan tenido de última hora por cuestiones de fechas especiales, vacaciones, temporadas altas, etc&lt;/p&gt;</v>
-      </c>
-      <c r="AB2" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-                    &lt;img src="https://rumbonaturaleza.com/wp-content/uploads/2023/03/Centro_Ecoturistico_El_Nuevo_Mundo_-_Estoracon_0.jpg" alt="Centro Ecoturistico El Nuevo Mundo - Estoracon"&gt;                
-                </v>
-      </c>
-      <c r="AC2" t="str">
-        <v>Añadir sitio web</v>
+      <c r="Z2" t="str">
+        <v/>
       </c>
     </row>
-    <row r="3" xml:space="preserve">
+    <row r="3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="str">
-        <v>Siempre Verde Chiapas, Centro Ecoturístico</v>
+        <v>Hotel Posada de Don Rodrigo Antigua</v>
       </c>
       <c r="C3" t="str">
-        <v>Siempre Verde Chiapas, Centro Ecoturístico</v>
+        <v>Hotel Posada De Don Rodrigo Antigua</v>
       </c>
       <c r="D3" t="str">
-        <v>siempre verde chiapas, centro ecoturístico</v>
+        <v>hotel posada de don rodrigo antigua</v>
       </c>
       <c r="E3" t="str">
-        <v>Carretera Escopetazo Pichucalco Kilometro 81 S/N, El Campanario, 29760 Jitotol, Chis.</v>
+        <v>Calle del Arco, 5a Avenida Norte, Antigua Guatemala 00502, Guatemala</v>
       </c>
       <c r="F3" t="str">
-        <v>919 104 9970</v>
+        <v>+502 7832 0387</v>
       </c>
       <c r="G3" t="str">
-        <v>Web no disponible</v>
+        <v>https://hotels.cloudbeds.com/reservation/HbWTDr</v>
       </c>
       <c r="H3" t="str">
         <v>No se cuenta con horario oficial</v>
@@ -639,206 +612,158 @@
         <v>No se cuenta con horario oficial</v>
       </c>
       <c r="J3" t="str">
-        <v>Jitotol, Chiapas</v>
+        <v>Antigua Guatemala, Guatemala</v>
       </c>
       <c r="K3" t="str">
         <v>Chiapas</v>
       </c>
       <c r="L3" t="str">
-        <v>https://www.google.com/maps/place/Siempre+Verde+Chiapas,+Centro+Ecotur%C3%ADstico/@17.143827,-92.888084,17z/data=!3m1!4b1!4m6!3m5!1s0x85ed0ee58c29248b:0xcdab59d265c14ddf!8m2!3d17.143827!4d-92.888084!16s%2Fg%2F11bvv4whms?authuser=0&amp;hl=es</v>
+        <v>https://www.google.com/maps/place/Hotel+Posada+de+Don+Rodrigo+Antigua/@14.5586234,-90.7341365,17z/data=!3m1!4b1!4m9!3m8!1s0x8589a1b94f5fae91:0xe3f57f9559045d14!5m2!4m1!1i2!8m2!3d14.5586234!4d-90.7341365!16s%2Fg%2F1td6yfpn?authuser=0&amp;hl=es</v>
       </c>
       <c r="M3" t="str">
-        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3812.5419796816677!2d-92.88808399999999!3d17.143826999999998!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x85ed0ee58c29248b%3A0xcdab59d265c14ddf!2sSiempre%20Verde%20Chiapas%2C%20Centro%20Ecotur%C3%ADstico!5e0!3m2!1ses!2smx!4v1679160012658!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
+        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3861.7090524214746!2d-90.73413649999999!3d14.558623399999998!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x8589a1b94f5fae91%3A0xe3f57f9559045d14!2sHotel%20Posada%20de%20Don%20Rodrigo%20Antigua!5e0!3m2!1ses!2smx!4v1679356390798!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
       </c>
       <c r="N3" t="str">
-        <v>44V6+GQ Jitotol, Chiapas</v>
+        <v>H758+C8 Antigua Guatemala, Guatemala</v>
       </c>
       <c r="O3" t="str">
-        <v>4.4</v>
+        <v>0.0</v>
       </c>
       <c r="P3" t="str">
-        <v>555</v>
+        <v>0</v>
       </c>
       <c r="Q3" t="str">
-        <v>Hermoso lugar para realizar senderismo, manejar cuatrimotos y para pasar unos días de relajamiento, todo el lugar es magnifico, las cabañas con chimeneas y balcones enormes desde donde puedes admirar el bosque, el lugar cuenta con…,El lugar es espectacular para estar alejado de la ciudad. Descansar, delicioso clima. Cómodo y limpio. No esperes un lugar de lujo pero si un lugar acogedor.,Un lugar muy bello para pasar un fin de semana en familia, el clima súper agradable y la vegetación maravillosa. Amo mi chiapas</v>
+        <v>no hay opiniones</v>
       </c>
       <c r="R3" t="str">
-        <v>https://lh5.googleusercontent.com/p/AF1QipPeHN3i2PWxhWxToRs-k5bKZZRwHphpyIy-yf-L=w426-h240-k-no</v>
+        <v>https://lh5.googleusercontent.com/p/AF1QipO409lNwbTr2Y-iGrirW9z7r6jqxvgW6x7GCpRP=w408-h272-k-no</v>
       </c>
       <c r="S3" t="str">
-        <v>wget --no-check-certificate https://lh5.googleusercontent.com/p/AF1QipPeHN3i2PWxhWxToRs-k5bKZZRwHphpyIy-yf-L=w426-h240-k-no</v>
+        <v>wget --no-check-certificate https://lh5.googleusercontent.com/p/AF1QipO409lNwbTr2Y-iGrirW9z7r6jqxvgW6x7GCpRP=w408-h272-k-no</v>
       </c>
       <c r="T3" t="str">
-        <v>AF1QipPeHN3i2PWxhWxToRs-k5bKZZRwHphpyIy-yf-L=w426-h240-k-no</v>
+        <v>AF1QipO409lNwbTr2Y-iGrirW9z7r6jqxvgW6x7GCpRP=w408-h272-k-no</v>
       </c>
       <c r="U3" t="str">
-        <v>Siempre_Verde_Chiapas,_Centro_Ecoturístico_1</v>
+        <v>Hotel_Posada_de_Don_Rodrigo_Antigua_1</v>
       </c>
       <c r="V3" t="str">
-        <v>Siempre_Verde_Chiapas,_Centro_Ecoturístico_1.jpg</v>
+        <v>Hotel_Posada_de_Don_Rodrigo_Antigua_1.jpg</v>
       </c>
       <c r="W3" t="str">
-        <v>https://rumbonaturaleza.com/wp-content/uploads/2023/03/Siempre_Verde_Chiapas,_Centro_Ecoturístico_1.jpg</v>
+        <v>https://rumbonaturaleza.com/wp-content/uploads/2023/03/Hotel_Posada_de_Don_Rodrigo_Antigua_1.jpg</v>
       </c>
       <c r="X3" t="str">
-        <v>ren "AF1QipPeHN3i2PWxhWxToRs-k5bKZZRwHphpyIy-yf-L=w426-h240-k-no" "Siempre_Verde_Chiapas,_Centro_Ecoturístico_1.jpg"</v>
+        <v>ren "AF1QipO409lNwbTr2Y-iGrirW9z7r6jqxvgW6x7GCpRP=w408-h272-k-no" "Hotel_Posada_de_Don_Rodrigo_Antigua_1.jpg"</v>
       </c>
       <c r="Y3" t="str">
         <v>parques-ecoturismo-en-chiapas</v>
       </c>
-      <c r="Z3" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-                    &lt;p&gt; ¿Estás buscando los mejores parques ecoturísticos en Chiapas? Entonces sin duda ¡estás en el lugar correcto!. Hoy en este artículo vamos a presentarte cuáles son los  parques ecoturísticos que han sido mejor evaluados en este estado. 
- Para poder definir esta listade los mejores, realizamos consultas en un montón de fuentes oficiales, redes sociales, rankings e incluso algunas entrevistas que nos permitieron determinar cuáles son y dónde se ubican los parques ecoturísticos que mejores experiencias han brindado a sus visitantes, y que mayor calificación han recibido en Chiapas durante los últimos años. 
- Con esta prueba social como respaldo, hoy te compartimos la lista de los centro ecoturístico mejor calificados en Chiapas en function getFullYear() { [native code] } junto con su ubicación, medios oficiales de contacto, horarios y cómo llegar hasta ellos; así como la calificación promedio con la que cuenta cada lugar. 
- Prepárate con esto y ¡a disfrutar del ecoturismo en Chiapas!&lt;/p&gt;                    
-                    </v>
-      </c>
-      <c r="AA3" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-                    &lt;h2&gt;&lt;b&gt;Centro de Ecoturismo Siempre Verde Chiapas, Centro Ecoturístico&lt;/b&gt;&lt;/h2&gt;
-                        &lt;img src="https://rumbonaturaleza.com/wp-content/uploads/2023/03/Siempre_Verde_Chiapas,_Centro_Ecoturístico_1.jpg" alt="Siempre Verde Chiapas, Centro Ecoturístico"&gt;   
-                        &lt;div&gt;&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3812.5419796816677!2d-92.88808399999999!3d17.143826999999998!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x85ed0ee58c29248b%3A0xcdab59d265c14ddf!2sSiempre%20Verde%20Chiapas%2C%20Centro%20Ecotur%C3%ADstico!5e0!3m2!1ses!2smx!4v1679160012658!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;&lt;/div&gt;
-                        &lt;div&gt;&lt;/div&gt;
-                        &lt;p&gt;El parque ecoturístico undefined es una opción fantástica para tener una aventura natural en undefined. Su calificación promedio es de undefined estrellas respaldada por más de undefined visitantes, así que no tenemos duda de que este lugar pertenece a la lista de los parques ecoturísticos mejor rankeados de de undefined y que se trata de uno de los principales atractivos naturales en la región. Así que ya sabes... ¿ganas de naturaleza?... pues entonces el parque natural undefined es una grandísima opción&lt;/p&gt;
-                        &lt;h3&gt;&lt;b&gt;¿Cómo llegar al Sitio Ecoturístico "Siempre Verde Chiapas, Centro Ecoturístico"? &lt;/b&gt;&lt;/h3&gt;
-                            &lt;p&gt;Este parque natural se ubica en Carretera Escopetazo Pichucalco Kilometro 81 S/N, El Campanario, 29760 Jitotol, Chis.
- Si necesitas ir a este sitio manejando puedes apoyarte poniendo la dirección en un navegador tipo waze o googleMaps o siguiendo directamente este &lt;a href='https://www.google.com/maps/place/Siempre+Verde+Chiapas,+Centro+Ecotur%C3%ADstico/@17.143827,-92.888084,17z/data=!3m1!4b1!4m6!3m5!1s0x85ed0ee58c29248b:0xcdab59d265c14ddf!8m2!3d17.143827!4d-92.888084!16s%2Fg%2F11bvv4whms?authuser=0&amp;hl=es'&gt;Mapa del Parque Ecoturístico Siempre Verde Chiapas, Centro Ecoturístico&lt;/a&gt;&lt;/p&gt;
-                        &lt;h3&gt;&lt;b&gt;¿Cuáles son los contactos del parque de ecoturismo Siempre Verde Chiapas, Centro Ecoturístico?&lt;/b&gt;&lt;/h3&gt;
-                            &lt;p&gt;Los contactos disponibles del Centro Ecoturístico Siempre Verde Chiapas, Centro Ecoturístico son: &lt;/p&gt;
-                            &lt;ul&gt;
-                                &lt;li&gt;&lt;b&gt;Teléfono:&lt;/b&gt;919 104 9970&lt;/li&gt;
-                                &lt;li&gt;&lt;b&gt;SitioWeb:&lt;/b&gt;web no disponible&lt;/li&gt;                                
-                            &lt;/ul&gt;
-                        &lt;h3&gt;&lt;b&gt;¿En qué horarios y días se puede visitar el centro ecoturístico Siempre Verde Chiapas, Centro Ecoturístico?&lt;/b&gt;&lt;/h3&gt;
-                        &lt;p&gt; Lamentablemente este sitio no cuenta con horarios publicados oficialmente, posiblemente debido a que existen variaciones frecuentes en sus horarios de operación. 
- Por este motivo, te recomendamos consultar sus sitios oficiales en una fecha cercana a tu visita o contactarlos directamente para pedir la actualización más reciente de sus días y horas de operación.</v>
-      </c>
-      <c r="AB3" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-                    &lt;img src="https://rumbonaturaleza.com/wp-content/uploads/2023/03/Siempre_Verde_Chiapas,_Centro_Ecoturístico_1.jpg" alt="Siempre Verde Chiapas, Centro Ecoturístico"&gt;                
-                </v>
-      </c>
-      <c r="AC3" t="str">
-        <v>Añadir sitio web</v>
+      <c r="Z3" t="str">
+        <v/>
       </c>
     </row>
-    <row r="4" xml:space="preserve">
+    <row r="4">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="str">
-        <v>Parque Ecoturistico Tzimbac</v>
+        <v>Centro Ecoturistico El Nuevo Mundo - Estoracon</v>
       </c>
       <c r="C4" t="str">
-        <v>Parque Ecoturistico Tzimbac</v>
+        <v>Centro Ecoturistico El Nuevo Mundo - Estoracon</v>
       </c>
       <c r="D4" t="str">
-        <v>parque ecoturistico tzimbac</v>
+        <v>centro ecoturistico el nuevo mundo - estoracon</v>
       </c>
       <c r="E4" t="str">
-        <v>Carretera a Monterrey Km. 2.2, Villarreal, 29125 Chis.</v>
+        <v>Carretera Sayula S/N, Francisco I. Madero, 30400 Cintalapa, Chis.</v>
       </c>
       <c r="F4" t="str">
-        <v>961 286 8575</v>
+        <v>961 284 4705</v>
       </c>
       <c r="G4" t="str">
         <v>Web no disponible</v>
       </c>
-      <c r="H4" t="str">
-        <v>No se cuenta con horario oficial</v>
-      </c>
       <c r="I4" t="str">
-        <v>No se cuenta con horario oficial</v>
+        <v>Lunes de 10:00 a 19:00,Martes de 10:00 a 19:00,Miércoles de 10:00 a 19:00,Jueves de 10:00 a 19:00,Viernes de 10:00 a 19:00,Sábado de 10:00 a 19:00,Domingo de 10:00 a 19:00</v>
       </c>
       <c r="J4" t="str">
-        <v>Santa Rita, Chiapas</v>
+        <v>Estoracón, Chiapas</v>
       </c>
       <c r="K4" t="str">
         <v>Chiapas</v>
       </c>
       <c r="L4" t="str">
-        <v>https://www.google.com/maps/place/Parque+Ecoturistico+Tzimbac/@16.8998672,-93.2289146,17z/data=!3m1!4b1!4m6!3m5!1s0x85ece790120fdba7:0xf3cf8d4d73cd7595!8m2!3d16.8998672!4d-93.2289146!16s%2Fg%2F12hm176_z?authuser=0&amp;hl=es</v>
+        <v>https://www.google.com/maps/place/Centro+Ecoturistico+El+Nuevo+Mundo+-+Estoracon/@16.8505798,-93.7933739,17z/data=!3m1!4b1!4m6!3m5!1s0x85eca6200d7617bb:0x7498371825377da6!8m2!3d16.8505798!4d-93.7933739!16s%2Fg%2F11dxpchfty?authuser=0&amp;hl=es</v>
       </c>
       <c r="M4" t="str">
-        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3817.515055110652!2d-93.2289146!3d16.8998672!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x85ece790120fdba7%3A0xf3cf8d4d73cd7595!2sParque%20Ecoturistico%20Tzimbac!5e0!3m2!1ses!2smx!4v1679160017598!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
+        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3818.5113687598837!2d-93.79337389999999!3d16.8505798!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x85eca6200d7617bb%3A0x7498371825377da6!2sCentro%20Ecoturistico%20El%20Nuevo%20Mundo%20-%20Estoracon!5e0!3m2!1ses!2smx!4v1679356394835!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
       </c>
       <c r="N4" t="str">
-        <v>VQXC+WC Santa Rita, Chiapas</v>
+        <v>V624+6M Estoracón, Chiapas</v>
       </c>
       <c r="O4" t="str">
-        <v>4.2</v>
+        <v>4.5</v>
       </c>
       <c r="P4" t="str">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="Q4" t="str">
-        <v>Si te gusta la naturaleza visítalo, si esperas muchas comodidades no es un sitio para ti. No hay señal, los baños están módicamente cómodos (si vas a la naturaleza no esperes lujos), hay área para acampar, muy limpio. Fuimos y nos tocó…,Buen lugar para descansar y rejarte un rato, sin embargo podría mejorar en muchos detalles, porque en época de lluvia es imposible disfrutar de la naturaleza, tener más sanitarios o en áreas más comunes.,Exelente lugar para ir con la familia y amigos. Podras acampar, explorar, senderismo, rappel, tirolesa, montar a caballo. Todo esto rodeo de magia y naturaleza respirando aire puro, fuera de la cantaminacion de la ciudad; puedes realozar…</v>
+        <v>Hermoso día de excursión en familia a este sitio remoto con 4 cascadas en plena naturaleza con piscina y una comida riquísima con buena atención, los Tucanes con muchi acercamiento, salimos de Cintalapa Chiapas,Muy bonita reserva recomendable,Se puede acampar ($180 por tienda de campaña), hay cabañas (sencilla $400, doble $800), rentan hamacas, tienda de campaña, venden refrescos, cervezas, sabritas, buena comida(camarones empanizado, en ensalada , mojarras, carne asada, pollo,…</v>
       </c>
       <c r="R4" t="str">
-        <v>https://lh5.googleusercontent.com/p/AF1QipNYYHKIZRIqOhYXADcr3o_zu4-ho3SpnynhRZrw=w408-h306-k-no</v>
+        <v>https://lh5.googleusercontent.com/p/AF1QipPOgfBL_SMdx6bZCZHeZCe150jGe-GqwXaX7lE=w408-h306-k-no</v>
       </c>
       <c r="S4" t="str">
-        <v>wget --no-check-certificate https://lh5.googleusercontent.com/p/AF1QipNYYHKIZRIqOhYXADcr3o_zu4-ho3SpnynhRZrw=w408-h306-k-no</v>
+        <v>wget --no-check-certificate https://lh5.googleusercontent.com/p/AF1QipPOgfBL_SMdx6bZCZHeZCe150jGe-GqwXaX7lE=w408-h306-k-no</v>
       </c>
       <c r="T4" t="str">
-        <v>AF1QipNYYHKIZRIqOhYXADcr3o_zu4-ho3SpnynhRZrw=w408-h306-k-no</v>
+        <v>AF1QipPOgfBL_SMdx6bZCZHeZCe150jGe-GqwXaX7lE=w408-h306-k-no</v>
       </c>
       <c r="U4" t="str">
-        <v>Parque_Ecoturistico_Tzimbac_2</v>
+        <v>Centro_Ecoturistico_El_Nuevo_Mundo_-_Estoracon_2</v>
       </c>
       <c r="V4" t="str">
-        <v>Parque_Ecoturistico_Tzimbac_2.jpg</v>
+        <v>Centro_Ecoturistico_El_Nuevo_Mundo_-_Estoracon_2.jpg</v>
       </c>
       <c r="W4" t="str">
-        <v>https://rumbonaturaleza.com/wp-content/uploads/2023/03/Parque_Ecoturistico_Tzimbac_2.jpg</v>
+        <v>https://rumbonaturaleza.com/wp-content/uploads/2023/03/Centro_Ecoturistico_El_Nuevo_Mundo_-_Estoracon_2.jpg</v>
       </c>
       <c r="X4" t="str">
-        <v>ren "AF1QipNYYHKIZRIqOhYXADcr3o_zu4-ho3SpnynhRZrw=w408-h306-k-no" "Parque_Ecoturistico_Tzimbac_2.jpg"</v>
+        <v>ren "AF1QipPOgfBL_SMdx6bZCZHeZCe150jGe-GqwXaX7lE=w408-h306-k-no" "Centro_Ecoturistico_El_Nuevo_Mundo_-_Estoracon_2.jpg"</v>
       </c>
       <c r="Y4" t="str">
         <v>parques-ecoturismo-en-chiapas</v>
       </c>
-      <c r="Z4" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-                    &lt;p&gt; ¿Estás buscando los mejores parques ecoturísticos en Chiapas? Entonces sin duda ¡estás en el lugar correcto!. Hoy en este artículo vamos a presentarte cuáles son los  parques ecológicos que han sido mejor evaluados en este estado. 
- Para poder definir esta listade los mejores, realizamos consultas en un montón de fuentes oficiales, redes sociales, rankings e incluso algunas entrevistas que nos permitieron determinar cuáles son y dónde se ubican los parques naturales que mejores experiencias han brindado a sus visitantes, y que mayor calificación han recibido en Chiapas durante los últimos años. 
- Con esta prueba social como respaldo, hoy te compartimos la lista de los parque ecoturístico mejor calificados en Chiapas en function getFullYear() { [native code] } junto con su ubicación, medios oficiales de contacto, horarios y cómo llegar hasta ellos; así como la calificación promedio con la que cuenta cada lugar. 
- Prepárate con esto y ¡a disfrutar del ecoturismo en Chiapas!&lt;/p&gt;                    
-                    </v>
-      </c>
-      <c r="AA4" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-                    &lt;h2&gt;&lt;b&gt;Parque Ecoturístico Parque Ecoturistico Tzimbac&lt;/b&gt;&lt;/h2&gt;
-                        &lt;img src="https://rumbonaturaleza.com/wp-content/uploads/2023/03/Parque_Ecoturistico_Tzimbac_2.jpg" alt="Parque Ecoturistico Tzimbac"&gt;   
-                        &lt;div&gt;&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3817.515055110652!2d-93.2289146!3d16.8998672!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x85ece790120fdba7%3A0xf3cf8d4d73cd7595!2sParque%20Ecoturistico%20Tzimbac!5e0!3m2!1ses!2smx!4v1679160017598!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;&lt;/div&gt;
-                        &lt;div&gt;&lt;/div&gt;
-                        &lt;p&gt;Si estás en undefined en búsqueda de algo de ecoturismo y aventura entonces el parque ecoturístico undefined no se te puede escapar. Hemos decidido incluir este parque ecoturístico en esta lista de los mejores de undefined gracias al respaldo y opiniones de más de undefined visitantes que lo han evaluado públicamente por lo menos con undefined estrellas de calificación (de las más altas para este estado del país). Así que chécate todos lo detalles necesarios para tu visita y ¡no se diga más! ¡a vivir el ecoturismo en undefined en undefined!&lt;/p&gt;
-                        &lt;h3&gt;&lt;b&gt;¿Cómo llegar al Parque Ecoturístico "Parque Ecoturistico Tzimbac"? &lt;/b&gt;&lt;/h3&gt;
-                            &lt;p&gt;Este sitio ecoturístico se ubica en Carretera a Monterrey Km. 2.2, Villarreal, 29125 Chis.
- Para llegar a este parque, simplemente sigue las indicaciones de tu aplicación de navegación preferida o utiliza este link al &lt;a href='https://www.google.com/maps/place/Parque+Ecoturistico+Tzimbac/@16.8998672,-93.2289146,17z/data=!3m1!4b1!4m6!3m5!1s0x85ece790120fdba7:0xf3cf8d4d73cd7595!8m2!3d16.8998672!4d-93.2289146!16s%2Fg%2F12hm176_z?authuser=0&amp;hl=es'&gt;Mapa del Parque Ecoturístico Parque Ecoturistico Tzimbac&lt;/a&gt;&lt;/p&gt;
-                        &lt;h3&gt;&lt;b&gt;¿Cuáles son los contactos del parque ecoturístico Parque Ecoturistico Tzimbac?&lt;/b&gt;&lt;/h3&gt;
-                            &lt;p&gt;Los contactos disponibles del Centro Ecoturístico Parque Ecoturistico Tzimbac son: &lt;/p&gt;
-                            &lt;ul&gt;
-                                &lt;li&gt;&lt;b&gt;Teléfono:&lt;/b&gt;961 286 8575&lt;/li&gt;
-                                &lt;li&gt;&lt;b&gt;SitioWeb:&lt;/b&gt;web no disponible&lt;/li&gt;                                
-                            &lt;/ul&gt;
-                        &lt;h3&gt;&lt;b&gt;¿En qué horarios y días se puede visitar el parque natural Parque Ecoturistico Tzimbac?&lt;/b&gt;&lt;/h3&gt;
-                        &lt;p&gt; Lamentablemente este sitio no cuenta con horarios publicados oficialmente, posiblemente debido a que existen variaciones frecuentes en sus horarios de operación. 
- Por este motivo, te recomendamos consultar sus sitios oficiales en una fecha cercana a tu visita o contactarlos directamente para pedir la actualización más reciente de sus días y horas de operación.</v>
-      </c>
-      <c r="AB4" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-                    &lt;img src="https://rumbonaturaleza.com/wp-content/uploads/2023/03/Parque_Ecoturistico_Tzimbac_2.jpg" alt="Parque Ecoturistico Tzimbac"&gt;                
-                </v>
+      <c r="Z4" t="str">
+        <v>Añadir sitio web</v>
+      </c>
+      <c r="AA4" t="str">
+        <v>Lunes de 10:00 a 19:00</v>
+      </c>
+      <c r="AB4" t="str">
+        <v>Martes de 10:00 a 19:00</v>
       </c>
       <c r="AC4" t="str">
-        <v>Añadir sitio web</v>
+        <v>Miércoles de 10:00 a 19:00</v>
+      </c>
+      <c r="AD4" t="str">
+        <v>Jueves de 10:00 a 19:00</v>
+      </c>
+      <c r="AE4" t="str">
+        <v>Viernes de 10:00 a 19:00</v>
+      </c>
+      <c r="AF4" t="str">
+        <v>Sábado de 10:00 a 19:00</v>
+      </c>
+      <c r="AG4" t="str">
+        <v>Domingo de 10:00 a 19:00</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:AC4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:AG4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>